<commit_message>
549587 Revisions per the RRR review.
</commit_message>
<xml_diff>
--- a/Requirement/Build 4/TAS eBilling RTM IB_ 2.0_592.xlsx
+++ b/Requirement/Build 4/TAS eBilling RTM IB_ 2.0_592.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="48" yWindow="-24" windowWidth="23040" windowHeight="9636" activeTab="2"/>
+    <workbookView xWindow="45" yWindow="-30" windowWidth="23040" windowHeight="9630" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -394,7 +394,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,12 +556,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -847,9 +841,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -864,19 +855,19 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -898,37 +889,37 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="3" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="3" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -949,7 +940,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -958,11 +949,14 @@
     <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1209,7 +1203,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1543,130 +1537,130 @@
       <selection activeCell="A23" sqref="A23:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="1"/>
-    <col min="3" max="3" width="21.109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="21.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:8" ht="22.95" x14ac:dyDescent="0.4">
-      <c r="A5" s="71" t="s">
+    <row r="5" spans="1:8" ht="22.9" x14ac:dyDescent="0.4">
+      <c r="A5" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-    </row>
-    <row r="6" spans="1:8" ht="22.95" x14ac:dyDescent="0.4">
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+    </row>
+    <row r="6" spans="1:8" ht="22.9" x14ac:dyDescent="0.4">
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-    </row>
-    <row r="8" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+    </row>
+    <row r="8" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
       <c r="C18" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="73" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
-    </row>
-    <row r="24" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B23" s="73"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
+    </row>
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A26" s="75" t="s">
+    <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="75"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="75"/>
-      <c r="H26" s="75"/>
-    </row>
-    <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="74"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
     </row>
-    <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
     </row>
-    <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
     </row>
-    <row r="33" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
     </row>
-    <row r="34" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
     </row>
   </sheetData>
@@ -1689,149 +1683,149 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="46.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.33203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="17.45" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
     </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="76" t="s">
+    <row r="2" spans="1:4" ht="17.45" x14ac:dyDescent="0.3">
+      <c r="A2" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-    </row>
-    <row r="3" spans="1:4" ht="13.95" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+    </row>
+    <row r="3" spans="1:4" ht="13.9" x14ac:dyDescent="0.25">
+      <c r="A3" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="57" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="62" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+    <row r="4" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+      <c r="A4" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="60">
+      <c r="B4" s="59">
         <v>1</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="61" t="s">
+      <c r="D4" s="60" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="62" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
+    <row r="5" spans="1:4" s="61" customFormat="1" ht="55.15" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="60">
+      <c r="B5" s="59">
         <v>2</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="D5" s="60" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="62" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
+    <row r="6" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+      <c r="A6" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="60">
+      <c r="B6" s="59">
         <v>3</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="61" t="s">
+      <c r="D6" s="60" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="62" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="59"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="61"/>
-    </row>
-    <row r="8" spans="1:4" s="62" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="61"/>
-    </row>
-    <row r="9" spans="1:4" s="62" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="59"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="61"/>
-    </row>
-    <row r="10" spans="1:4" s="62" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="59"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="61"/>
-    </row>
-    <row r="11" spans="1:4" s="62" customFormat="1" ht="13.95" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="65"/>
-    </row>
-    <row r="12" spans="1:4" s="62" customFormat="1" ht="13.95" x14ac:dyDescent="0.25">
-      <c r="A12" s="66"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="65"/>
-    </row>
-    <row r="13" spans="1:4" s="62" customFormat="1" ht="13.95" x14ac:dyDescent="0.25">
-      <c r="A13" s="67"/>
-      <c r="B13" s="68"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="69"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="55"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+      <c r="A7" s="58"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="60"/>
+    </row>
+    <row r="8" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+      <c r="A8" s="58"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="60"/>
+    </row>
+    <row r="9" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+      <c r="A9" s="58"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="60"/>
+    </row>
+    <row r="10" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+      <c r="A10" s="58"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="60"/>
+    </row>
+    <row r="11" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+      <c r="A11" s="65"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="64"/>
+    </row>
+    <row r="12" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+      <c r="A12" s="65"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="64"/>
+    </row>
+    <row r="13" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+      <c r="A13" s="66"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="68"/>
+    </row>
+    <row r="14" spans="1:4" ht="13.15" x14ac:dyDescent="0.25">
+      <c r="A14" s="54"/>
+    </row>
+    <row r="15" spans="1:4" ht="13.15" x14ac:dyDescent="0.25">
+      <c r="A15" s="54"/>
+    </row>
+    <row r="16" spans="1:4" ht="13.15" x14ac:dyDescent="0.25">
+      <c r="A16" s="54"/>
+    </row>
+    <row r="17" spans="1:1" ht="13.15" x14ac:dyDescent="0.25">
+      <c r="A17" s="54"/>
+    </row>
+    <row r="18" spans="1:1" ht="13.15" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="13.15" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="13.15" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="13.15" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="13.15" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
     </row>
   </sheetData>
@@ -1851,28 +1845,28 @@
   <dimension ref="A1:DQ99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="19" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="57.33203125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="10" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" style="10" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" style="10" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" customWidth="1"/>
-    <col min="11" max="11" width="28.33203125" style="10" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="57.28515625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" customWidth="1"/>
+    <col min="11" max="11" width="28.28515625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" style="10" customWidth="1"/>
     <col min="14" max="14" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:121" s="11" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:121" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>6</v>
       </c>
@@ -2023,7 +2017,7 @@
       <c r="DP1" s="21"/>
       <c r="DQ1" s="21"/>
     </row>
-    <row r="2" spans="1:121" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:121" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>36</v>
       </c>
@@ -2041,44 +2035,44 @@
       <c r="M2" s="22"/>
       <c r="N2" s="22"/>
     </row>
-    <row r="3" spans="1:121" s="43" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:121" s="42" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="80" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="41" t="s">
         <v>17</v>
       </c>
       <c r="K3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="54" t="s">
+      <c r="L3" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="57" t="s">
+      <c r="M3" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N3" s="12" t="s">
@@ -2086,35 +2080,35 @@
       </c>
       <c r="O3" s="13"/>
     </row>
-    <row r="4" spans="1:121" s="43" customFormat="1" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:121" s="42" customFormat="1" ht="61.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="41" t="s">
+      <c r="J4" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K4" s="12" t="s">
@@ -2123,7 +2117,7 @@
       <c r="L4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M4" s="57" t="s">
+      <c r="M4" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N4" s="12" t="s">
@@ -2131,132 +2125,132 @@
       </c>
       <c r="O4" s="13"/>
     </row>
-    <row r="5" spans="1:121" s="77" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="77" t="s">
+    <row r="5" spans="1:121" s="76" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="78"/>
-      <c r="S5" s="78"/>
-      <c r="T5" s="78"/>
-      <c r="U5" s="78"/>
-      <c r="V5" s="78"/>
-      <c r="W5" s="78"/>
-      <c r="X5" s="78"/>
-      <c r="Y5" s="78"/>
-      <c r="Z5" s="78"/>
-      <c r="AA5" s="78"/>
-      <c r="AB5" s="78"/>
-      <c r="AC5" s="78"/>
-      <c r="AD5" s="78"/>
-      <c r="AE5" s="78"/>
-      <c r="AF5" s="78"/>
-      <c r="AG5" s="78"/>
-      <c r="AH5" s="78"/>
-      <c r="AI5" s="78"/>
-      <c r="AJ5" s="78"/>
-      <c r="AK5" s="78"/>
-      <c r="AL5" s="78"/>
-      <c r="AM5" s="78"/>
-      <c r="AN5" s="78"/>
-      <c r="AO5" s="78"/>
-      <c r="AP5" s="78"/>
-      <c r="AQ5" s="78"/>
-      <c r="AR5" s="78"/>
-      <c r="AS5" s="78"/>
-      <c r="AT5" s="78"/>
-      <c r="AU5" s="78"/>
-      <c r="AV5" s="78"/>
-      <c r="AW5" s="78"/>
-      <c r="AX5" s="78"/>
-      <c r="AY5" s="78"/>
-      <c r="AZ5" s="78"/>
-      <c r="BA5" s="78"/>
-      <c r="BB5" s="78"/>
-      <c r="BC5" s="78"/>
-      <c r="BD5" s="78"/>
-      <c r="BE5" s="78"/>
-      <c r="BF5" s="78"/>
-      <c r="BG5" s="78"/>
-      <c r="BH5" s="78"/>
-      <c r="BI5" s="78"/>
-      <c r="BJ5" s="78"/>
-      <c r="BK5" s="78"/>
-      <c r="BL5" s="78"/>
-      <c r="BM5" s="78"/>
-      <c r="BN5" s="78"/>
-      <c r="BO5" s="78"/>
-      <c r="BP5" s="78"/>
-      <c r="BQ5" s="78"/>
-      <c r="BR5" s="78"/>
-      <c r="BS5" s="78"/>
-      <c r="BT5" s="78"/>
-      <c r="BU5" s="78"/>
-      <c r="BV5" s="78"/>
-      <c r="BW5" s="78"/>
-      <c r="BX5" s="78"/>
-      <c r="BY5" s="78"/>
-      <c r="BZ5" s="78"/>
-      <c r="CA5" s="78"/>
-      <c r="CB5" s="78"/>
-      <c r="CC5" s="78"/>
-      <c r="CD5" s="78"/>
-      <c r="CE5" s="78"/>
-      <c r="CF5" s="78"/>
-      <c r="CG5" s="78"/>
-      <c r="CH5" s="78"/>
-      <c r="CI5" s="78"/>
-      <c r="CJ5" s="78"/>
-      <c r="CK5" s="78"/>
-      <c r="CL5" s="78"/>
-      <c r="CM5" s="78"/>
-      <c r="CN5" s="78"/>
-      <c r="CO5" s="78"/>
-      <c r="CP5" s="78"/>
-      <c r="CQ5" s="78"/>
-      <c r="CR5" s="78"/>
-      <c r="CS5" s="78"/>
-      <c r="CT5" s="78"/>
-      <c r="CU5" s="78"/>
-      <c r="CV5" s="78"/>
-      <c r="CW5" s="78"/>
-      <c r="CX5" s="78"/>
-      <c r="CY5" s="78"/>
-      <c r="CZ5" s="78"/>
-      <c r="DA5" s="78"/>
-      <c r="DB5" s="78"/>
-      <c r="DC5" s="78"/>
-      <c r="DD5" s="78"/>
-      <c r="DE5" s="78"/>
-      <c r="DF5" s="78"/>
-      <c r="DG5" s="78"/>
-      <c r="DH5" s="78"/>
-      <c r="DI5" s="78"/>
-      <c r="DJ5" s="78"/>
-      <c r="DK5" s="78"/>
-      <c r="DL5" s="78"/>
-      <c r="DM5" s="78"/>
-      <c r="DN5" s="78"/>
-      <c r="DO5" s="78"/>
-      <c r="DP5" s="78"/>
-      <c r="DQ5" s="78"/>
-    </row>
-    <row r="6" spans="1:121" s="44" customFormat="1" ht="184.8" x14ac:dyDescent="0.25">
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="77"/>
+      <c r="R5" s="77"/>
+      <c r="S5" s="77"/>
+      <c r="T5" s="77"/>
+      <c r="U5" s="77"/>
+      <c r="V5" s="77"/>
+      <c r="W5" s="77"/>
+      <c r="X5" s="77"/>
+      <c r="Y5" s="77"/>
+      <c r="Z5" s="77"/>
+      <c r="AA5" s="77"/>
+      <c r="AB5" s="77"/>
+      <c r="AC5" s="77"/>
+      <c r="AD5" s="77"/>
+      <c r="AE5" s="77"/>
+      <c r="AF5" s="77"/>
+      <c r="AG5" s="77"/>
+      <c r="AH5" s="77"/>
+      <c r="AI5" s="77"/>
+      <c r="AJ5" s="77"/>
+      <c r="AK5" s="77"/>
+      <c r="AL5" s="77"/>
+      <c r="AM5" s="77"/>
+      <c r="AN5" s="77"/>
+      <c r="AO5" s="77"/>
+      <c r="AP5" s="77"/>
+      <c r="AQ5" s="77"/>
+      <c r="AR5" s="77"/>
+      <c r="AS5" s="77"/>
+      <c r="AT5" s="77"/>
+      <c r="AU5" s="77"/>
+      <c r="AV5" s="77"/>
+      <c r="AW5" s="77"/>
+      <c r="AX5" s="77"/>
+      <c r="AY5" s="77"/>
+      <c r="AZ5" s="77"/>
+      <c r="BA5" s="77"/>
+      <c r="BB5" s="77"/>
+      <c r="BC5" s="77"/>
+      <c r="BD5" s="77"/>
+      <c r="BE5" s="77"/>
+      <c r="BF5" s="77"/>
+      <c r="BG5" s="77"/>
+      <c r="BH5" s="77"/>
+      <c r="BI5" s="77"/>
+      <c r="BJ5" s="77"/>
+      <c r="BK5" s="77"/>
+      <c r="BL5" s="77"/>
+      <c r="BM5" s="77"/>
+      <c r="BN5" s="77"/>
+      <c r="BO5" s="77"/>
+      <c r="BP5" s="77"/>
+      <c r="BQ5" s="77"/>
+      <c r="BR5" s="77"/>
+      <c r="BS5" s="77"/>
+      <c r="BT5" s="77"/>
+      <c r="BU5" s="77"/>
+      <c r="BV5" s="77"/>
+      <c r="BW5" s="77"/>
+      <c r="BX5" s="77"/>
+      <c r="BY5" s="77"/>
+      <c r="BZ5" s="77"/>
+      <c r="CA5" s="77"/>
+      <c r="CB5" s="77"/>
+      <c r="CC5" s="77"/>
+      <c r="CD5" s="77"/>
+      <c r="CE5" s="77"/>
+      <c r="CF5" s="77"/>
+      <c r="CG5" s="77"/>
+      <c r="CH5" s="77"/>
+      <c r="CI5" s="77"/>
+      <c r="CJ5" s="77"/>
+      <c r="CK5" s="77"/>
+      <c r="CL5" s="77"/>
+      <c r="CM5" s="77"/>
+      <c r="CN5" s="77"/>
+      <c r="CO5" s="77"/>
+      <c r="CP5" s="77"/>
+      <c r="CQ5" s="77"/>
+      <c r="CR5" s="77"/>
+      <c r="CS5" s="77"/>
+      <c r="CT5" s="77"/>
+      <c r="CU5" s="77"/>
+      <c r="CV5" s="77"/>
+      <c r="CW5" s="77"/>
+      <c r="CX5" s="77"/>
+      <c r="CY5" s="77"/>
+      <c r="CZ5" s="77"/>
+      <c r="DA5" s="77"/>
+      <c r="DB5" s="77"/>
+      <c r="DC5" s="77"/>
+      <c r="DD5" s="77"/>
+      <c r="DE5" s="77"/>
+      <c r="DF5" s="77"/>
+      <c r="DG5" s="77"/>
+      <c r="DH5" s="77"/>
+      <c r="DI5" s="77"/>
+      <c r="DJ5" s="77"/>
+      <c r="DK5" s="77"/>
+      <c r="DL5" s="77"/>
+      <c r="DM5" s="77"/>
+      <c r="DN5" s="77"/>
+      <c r="DO5" s="77"/>
+      <c r="DP5" s="77"/>
+      <c r="DQ5" s="77"/>
+    </row>
+    <row r="6" spans="1:121" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>16</v>
       </c>
@@ -2266,7 +2260,7 @@
       <c r="C6" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="12" t="s">
@@ -2275,16 +2269,16 @@
       <c r="F6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I6" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="J6" s="41" t="s">
         <v>17</v>
       </c>
       <c r="K6" s="12" t="s">
@@ -2293,14 +2287,14 @@
       <c r="L6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="57" t="s">
+      <c r="M6" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N6" s="12" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:121" s="44" customFormat="1" ht="184.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:121" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>16</v>
       </c>
@@ -2310,7 +2304,7 @@
       <c r="C7" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="12" t="s">
@@ -2319,16 +2313,16 @@
       <c r="F7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="G7" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H7" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="J7" s="41" t="s">
         <v>17</v>
       </c>
       <c r="K7" s="12" t="s">
@@ -2337,14 +2331,14 @@
       <c r="L7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M7" s="57" t="s">
+      <c r="M7" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N7" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:121" s="44" customFormat="1" ht="184.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:121" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>16</v>
       </c>
@@ -2354,7 +2348,7 @@
       <c r="C8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="12" t="s">
@@ -2363,16 +2357,16 @@
       <c r="F8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I8" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J8" s="42" t="s">
+      <c r="J8" s="41" t="s">
         <v>17</v>
       </c>
       <c r="K8" s="12" t="s">
@@ -2381,14 +2375,14 @@
       <c r="L8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M8" s="57" t="s">
+      <c r="M8" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N8" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:121" s="44" customFormat="1" ht="184.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:121" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>16</v>
       </c>
@@ -2398,7 +2392,7 @@
       <c r="C9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="12" t="s">
@@ -2407,16 +2401,16 @@
       <c r="F9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="41" t="s">
+      <c r="G9" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="41" t="s">
+      <c r="H9" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J9" s="42" t="s">
+      <c r="J9" s="41" t="s">
         <v>17</v>
       </c>
       <c r="K9" s="12" t="s">
@@ -2425,14 +2419,14 @@
       <c r="L9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M9" s="57" t="s">
+      <c r="M9" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N9" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:121" s="44" customFormat="1" ht="97.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:121" s="43" customFormat="1" ht="97.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>16</v>
       </c>
@@ -2442,7 +2436,7 @@
       <c r="C10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="12" t="s">
@@ -2451,16 +2445,16 @@
       <c r="F10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="41" t="s">
+      <c r="G10" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="41" t="s">
+      <c r="H10" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I10" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="42" t="s">
+      <c r="J10" s="41" t="s">
         <v>17</v>
       </c>
       <c r="K10" s="12" t="s">
@@ -2469,14 +2463,14 @@
       <c r="L10" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M10" s="57" t="s">
+      <c r="M10" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N10" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:121" s="44" customFormat="1" ht="184.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:121" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>103</v>
       </c>
@@ -2486,7 +2480,7 @@
       <c r="C11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="12" t="s">
@@ -2495,16 +2489,16 @@
       <c r="F11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="41" t="s">
+      <c r="G11" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="41" t="s">
+      <c r="H11" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I11" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="42" t="s">
+      <c r="J11" s="41" t="s">
         <v>17</v>
       </c>
       <c r="K11" s="12" t="s">
@@ -2513,14 +2507,14 @@
       <c r="L11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M11" s="57" t="s">
+      <c r="M11" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N11" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:121" s="44" customFormat="1" ht="184.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:121" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>16</v>
       </c>
@@ -2530,7 +2524,7 @@
       <c r="C12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="12" t="s">
@@ -2539,16 +2533,16 @@
       <c r="F12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="41" t="s">
+      <c r="G12" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="41" t="s">
+      <c r="H12" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I12" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J12" s="42" t="s">
+      <c r="J12" s="41" t="s">
         <v>17</v>
       </c>
       <c r="K12" s="12" t="s">
@@ -2557,139 +2551,139 @@
       <c r="L12" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M12" s="57" t="s">
+      <c r="M12" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N12" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:121" s="77" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="77" t="s">
+    <row r="13" spans="1:121" s="76" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="78"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="78"/>
-      <c r="M13" s="78"/>
-      <c r="N13" s="78"/>
-      <c r="O13" s="78"/>
-      <c r="P13" s="78"/>
-      <c r="Q13" s="78"/>
-      <c r="R13" s="78"/>
-      <c r="S13" s="78"/>
-      <c r="T13" s="78"/>
-      <c r="U13" s="78"/>
-      <c r="V13" s="78"/>
-      <c r="W13" s="78"/>
-      <c r="X13" s="78"/>
-      <c r="Y13" s="78"/>
-      <c r="Z13" s="78"/>
-      <c r="AA13" s="78"/>
-      <c r="AB13" s="78"/>
-      <c r="AC13" s="78"/>
-      <c r="AD13" s="78"/>
-      <c r="AE13" s="78"/>
-      <c r="AF13" s="78"/>
-      <c r="AG13" s="78"/>
-      <c r="AH13" s="78"/>
-      <c r="AI13" s="78"/>
-      <c r="AJ13" s="78"/>
-      <c r="AK13" s="78"/>
-      <c r="AL13" s="78"/>
-      <c r="AM13" s="78"/>
-      <c r="AN13" s="78"/>
-      <c r="AO13" s="78"/>
-      <c r="AP13" s="78"/>
-      <c r="AQ13" s="78"/>
-      <c r="AR13" s="78"/>
-      <c r="AS13" s="78"/>
-      <c r="AT13" s="78"/>
-      <c r="AU13" s="78"/>
-      <c r="AV13" s="78"/>
-      <c r="AW13" s="78"/>
-      <c r="AX13" s="78"/>
-      <c r="AY13" s="78"/>
-      <c r="AZ13" s="78"/>
-      <c r="BA13" s="78"/>
-      <c r="BB13" s="78"/>
-      <c r="BC13" s="78"/>
-      <c r="BD13" s="78"/>
-      <c r="BE13" s="78"/>
-      <c r="BF13" s="78"/>
-      <c r="BG13" s="78"/>
-      <c r="BH13" s="78"/>
-      <c r="BI13" s="78"/>
-      <c r="BJ13" s="78"/>
-      <c r="BK13" s="78"/>
-      <c r="BL13" s="78"/>
-      <c r="BM13" s="78"/>
-      <c r="BN13" s="78"/>
-      <c r="BO13" s="78"/>
-      <c r="BP13" s="78"/>
-      <c r="BQ13" s="78"/>
-      <c r="BR13" s="78"/>
-      <c r="BS13" s="78"/>
-      <c r="BT13" s="78"/>
-      <c r="BU13" s="78"/>
-      <c r="BV13" s="78"/>
-      <c r="BW13" s="78"/>
-      <c r="BX13" s="78"/>
-      <c r="BY13" s="78"/>
-      <c r="BZ13" s="78"/>
-      <c r="CA13" s="78"/>
-      <c r="CB13" s="78"/>
-      <c r="CC13" s="78"/>
-      <c r="CD13" s="78"/>
-      <c r="CE13" s="78"/>
-      <c r="CF13" s="78"/>
-      <c r="CG13" s="78"/>
-      <c r="CH13" s="78"/>
-      <c r="CI13" s="78"/>
-      <c r="CJ13" s="78"/>
-      <c r="CK13" s="78"/>
-      <c r="CL13" s="78"/>
-      <c r="CM13" s="78"/>
-      <c r="CN13" s="78"/>
-      <c r="CO13" s="78"/>
-      <c r="CP13" s="78"/>
-      <c r="CQ13" s="78"/>
-      <c r="CR13" s="78"/>
-      <c r="CS13" s="78"/>
-      <c r="CT13" s="78"/>
-      <c r="CU13" s="78"/>
-      <c r="CV13" s="78"/>
-      <c r="CW13" s="78"/>
-      <c r="CX13" s="78"/>
-      <c r="CY13" s="78"/>
-      <c r="CZ13" s="78"/>
-      <c r="DA13" s="78"/>
-      <c r="DB13" s="78"/>
-      <c r="DC13" s="78"/>
-      <c r="DD13" s="78"/>
-      <c r="DE13" s="78"/>
-      <c r="DF13" s="78"/>
-      <c r="DG13" s="78"/>
-      <c r="DH13" s="78"/>
-      <c r="DI13" s="78"/>
-      <c r="DJ13" s="78"/>
-      <c r="DK13" s="78"/>
-      <c r="DL13" s="78"/>
-      <c r="DM13" s="78"/>
-      <c r="DN13" s="78"/>
-      <c r="DO13" s="78"/>
-      <c r="DP13" s="78"/>
-      <c r="DQ13" s="78"/>
-    </row>
-    <row r="14" spans="1:121" s="44" customFormat="1" ht="97.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="77"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="77"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="77"/>
+      <c r="K13" s="77"/>
+      <c r="L13" s="77"/>
+      <c r="M13" s="77"/>
+      <c r="N13" s="77"/>
+      <c r="O13" s="77"/>
+      <c r="P13" s="77"/>
+      <c r="Q13" s="77"/>
+      <c r="R13" s="77"/>
+      <c r="S13" s="77"/>
+      <c r="T13" s="77"/>
+      <c r="U13" s="77"/>
+      <c r="V13" s="77"/>
+      <c r="W13" s="77"/>
+      <c r="X13" s="77"/>
+      <c r="Y13" s="77"/>
+      <c r="Z13" s="77"/>
+      <c r="AA13" s="77"/>
+      <c r="AB13" s="77"/>
+      <c r="AC13" s="77"/>
+      <c r="AD13" s="77"/>
+      <c r="AE13" s="77"/>
+      <c r="AF13" s="77"/>
+      <c r="AG13" s="77"/>
+      <c r="AH13" s="77"/>
+      <c r="AI13" s="77"/>
+      <c r="AJ13" s="77"/>
+      <c r="AK13" s="77"/>
+      <c r="AL13" s="77"/>
+      <c r="AM13" s="77"/>
+      <c r="AN13" s="77"/>
+      <c r="AO13" s="77"/>
+      <c r="AP13" s="77"/>
+      <c r="AQ13" s="77"/>
+      <c r="AR13" s="77"/>
+      <c r="AS13" s="77"/>
+      <c r="AT13" s="77"/>
+      <c r="AU13" s="77"/>
+      <c r="AV13" s="77"/>
+      <c r="AW13" s="77"/>
+      <c r="AX13" s="77"/>
+      <c r="AY13" s="77"/>
+      <c r="AZ13" s="77"/>
+      <c r="BA13" s="77"/>
+      <c r="BB13" s="77"/>
+      <c r="BC13" s="77"/>
+      <c r="BD13" s="77"/>
+      <c r="BE13" s="77"/>
+      <c r="BF13" s="77"/>
+      <c r="BG13" s="77"/>
+      <c r="BH13" s="77"/>
+      <c r="BI13" s="77"/>
+      <c r="BJ13" s="77"/>
+      <c r="BK13" s="77"/>
+      <c r="BL13" s="77"/>
+      <c r="BM13" s="77"/>
+      <c r="BN13" s="77"/>
+      <c r="BO13" s="77"/>
+      <c r="BP13" s="77"/>
+      <c r="BQ13" s="77"/>
+      <c r="BR13" s="77"/>
+      <c r="BS13" s="77"/>
+      <c r="BT13" s="77"/>
+      <c r="BU13" s="77"/>
+      <c r="BV13" s="77"/>
+      <c r="BW13" s="77"/>
+      <c r="BX13" s="77"/>
+      <c r="BY13" s="77"/>
+      <c r="BZ13" s="77"/>
+      <c r="CA13" s="77"/>
+      <c r="CB13" s="77"/>
+      <c r="CC13" s="77"/>
+      <c r="CD13" s="77"/>
+      <c r="CE13" s="77"/>
+      <c r="CF13" s="77"/>
+      <c r="CG13" s="77"/>
+      <c r="CH13" s="77"/>
+      <c r="CI13" s="77"/>
+      <c r="CJ13" s="77"/>
+      <c r="CK13" s="77"/>
+      <c r="CL13" s="77"/>
+      <c r="CM13" s="77"/>
+      <c r="CN13" s="77"/>
+      <c r="CO13" s="77"/>
+      <c r="CP13" s="77"/>
+      <c r="CQ13" s="77"/>
+      <c r="CR13" s="77"/>
+      <c r="CS13" s="77"/>
+      <c r="CT13" s="77"/>
+      <c r="CU13" s="77"/>
+      <c r="CV13" s="77"/>
+      <c r="CW13" s="77"/>
+      <c r="CX13" s="77"/>
+      <c r="CY13" s="77"/>
+      <c r="CZ13" s="77"/>
+      <c r="DA13" s="77"/>
+      <c r="DB13" s="77"/>
+      <c r="DC13" s="77"/>
+      <c r="DD13" s="77"/>
+      <c r="DE13" s="77"/>
+      <c r="DF13" s="77"/>
+      <c r="DG13" s="77"/>
+      <c r="DH13" s="77"/>
+      <c r="DI13" s="77"/>
+      <c r="DJ13" s="77"/>
+      <c r="DK13" s="77"/>
+      <c r="DL13" s="77"/>
+      <c r="DM13" s="77"/>
+      <c r="DN13" s="77"/>
+      <c r="DO13" s="77"/>
+      <c r="DP13" s="77"/>
+      <c r="DQ13" s="77"/>
+    </row>
+    <row r="14" spans="1:121" s="43" customFormat="1" ht="97.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>16</v>
       </c>
@@ -2699,7 +2693,7 @@
       <c r="C14" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="12" t="s">
@@ -2708,16 +2702,16 @@
       <c r="F14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="41" t="s">
+      <c r="G14" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="41" t="s">
+      <c r="H14" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I14" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J14" s="41" t="s">
+      <c r="J14" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="12" t="s">
@@ -2726,32 +2720,32 @@
       <c r="L14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M14" s="57" t="s">
+      <c r="M14" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N14" s="12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:121" s="79" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="79" t="s">
+    <row r="15" spans="1:121" s="78" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="80"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="80"/>
-      <c r="K15" s="80"/>
-      <c r="L15" s="80"/>
-      <c r="M15" s="80"/>
-      <c r="N15" s="80"/>
-    </row>
-    <row r="16" spans="1:121" s="44" customFormat="1" ht="154.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="79"/>
+    </row>
+    <row r="16" spans="1:121" s="43" customFormat="1" ht="154.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>16</v>
       </c>
@@ -2761,7 +2755,7 @@
       <c r="C16" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="41" t="s">
+      <c r="D16" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="12" t="s">
@@ -2770,16 +2764,16 @@
       <c r="F16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="41" t="s">
+      <c r="G16" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="41" t="s">
+      <c r="H16" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I16" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J16" s="41" t="s">
+      <c r="J16" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K16" s="12" t="s">
@@ -2788,14 +2782,14 @@
       <c r="L16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M16" s="57" t="s">
+      <c r="M16" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N16" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="44" customFormat="1" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="43" customFormat="1" ht="151.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>16</v>
       </c>
@@ -2805,7 +2799,7 @@
       <c r="C17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="12" t="s">
@@ -2814,16 +2808,16 @@
       <c r="F17" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="G17" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="41" t="s">
+      <c r="H17" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J17" s="41" t="s">
+      <c r="J17" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K17" s="12" t="s">
@@ -2832,14 +2826,14 @@
       <c r="L17" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M17" s="57" t="s">
+      <c r="M17" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N17" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="44" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="43" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>16</v>
       </c>
@@ -2849,7 +2843,7 @@
       <c r="C18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="12" t="s">
@@ -2858,16 +2852,16 @@
       <c r="F18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="41" t="s">
+      <c r="G18" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="41" t="s">
+      <c r="H18" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I18" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="41" t="s">
+      <c r="J18" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K18" s="12" t="s">
@@ -2876,14 +2870,14 @@
       <c r="L18" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M18" s="57" t="s">
+      <c r="M18" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N18" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="44" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="43" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>16</v>
       </c>
@@ -2893,7 +2887,7 @@
       <c r="C19" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="41" t="s">
+      <c r="D19" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="12" t="s">
@@ -2902,16 +2896,16 @@
       <c r="F19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="41" t="s">
+      <c r="G19" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="41" t="s">
+      <c r="H19" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I19" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J19" s="41" t="s">
+      <c r="J19" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K19" s="12" t="s">
@@ -2920,32 +2914,32 @@
       <c r="L19" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M19" s="57" t="s">
+      <c r="M19" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N19" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="77" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="77" t="s">
+    <row r="20" spans="1:14" s="76" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="78"/>
-      <c r="C20" s="78"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="78"/>
-      <c r="L20" s="78"/>
-      <c r="M20" s="78"/>
-      <c r="N20" s="78"/>
-    </row>
-    <row r="21" spans="1:14" s="49" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="B20" s="77"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="77"/>
+      <c r="J20" s="77"/>
+      <c r="K20" s="77"/>
+      <c r="L20" s="77"/>
+      <c r="M20" s="77"/>
+      <c r="N20" s="77"/>
+    </row>
+    <row r="21" spans="1:14" s="48" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>16</v>
       </c>
@@ -2982,14 +2976,14 @@
       <c r="L21" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M21" s="57" t="s">
+      <c r="M21" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N21" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="49" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="48" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>16</v>
       </c>
@@ -3026,14 +3020,14 @@
       <c r="L22" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M22" s="57" t="s">
+      <c r="M22" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N22" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="49" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="48" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>16</v>
       </c>
@@ -3070,14 +3064,14 @@
       <c r="L23" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M23" s="57" t="s">
+      <c r="M23" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N23" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="49" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="48" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>16</v>
       </c>
@@ -3114,14 +3108,14 @@
       <c r="L24" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M24" s="57" t="s">
+      <c r="M24" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N24" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="49" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="48" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>16</v>
       </c>
@@ -3158,32 +3152,32 @@
       <c r="L25" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M25" s="57" t="s">
+      <c r="M25" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N25" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="77" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="77" t="s">
+    <row r="26" spans="1:14" s="76" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="78"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="78"/>
-      <c r="I26" s="78"/>
-      <c r="J26" s="78"/>
-      <c r="K26" s="78"/>
-      <c r="L26" s="78"/>
-      <c r="M26" s="78"/>
-      <c r="N26" s="78"/>
-    </row>
-    <row r="27" spans="1:14" s="29" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="B26" s="77"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="77"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="77"/>
+      <c r="J26" s="77"/>
+      <c r="K26" s="77"/>
+      <c r="L26" s="77"/>
+      <c r="M26" s="77"/>
+      <c r="N26" s="77"/>
+    </row>
+    <row r="27" spans="1:14" s="29" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>16</v>
       </c>
@@ -3193,25 +3187,25 @@
       <c r="C27" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="41" t="s">
+      <c r="D27" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="46" t="s">
+      <c r="F27" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="41" t="s">
+      <c r="G27" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="41" t="s">
+      <c r="H27" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I27" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J27" s="41" t="s">
+      <c r="J27" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K27" s="29" t="s">
@@ -3220,14 +3214,14 @@
       <c r="L27" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M27" s="57" t="s">
+      <c r="M27" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N27" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="45" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>16</v>
       </c>
@@ -3237,25 +3231,25 @@
       <c r="C28" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="41" t="s">
+      <c r="D28" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F28" s="46" t="s">
+      <c r="F28" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="G28" s="41" t="s">
+      <c r="G28" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="41" t="s">
+      <c r="H28" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I28" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J28" s="41" t="s">
+      <c r="J28" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K28" s="13" t="s">
@@ -3264,32 +3258,32 @@
       <c r="L28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M28" s="57" t="s">
+      <c r="M28" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N28" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="77" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="77" t="s">
+    <row r="29" spans="1:14" s="76" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="78"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="78"/>
-      <c r="I29" s="78"/>
-      <c r="J29" s="78"/>
-      <c r="K29" s="78"/>
-      <c r="L29" s="78"/>
-      <c r="M29" s="78"/>
-      <c r="N29" s="78"/>
-    </row>
-    <row r="30" spans="1:14" s="56" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="B29" s="77"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
+      <c r="H29" s="77"/>
+      <c r="I29" s="77"/>
+      <c r="J29" s="77"/>
+      <c r="K29" s="77"/>
+      <c r="L29" s="77"/>
+      <c r="M29" s="77"/>
+      <c r="N29" s="77"/>
+    </row>
+    <row r="30" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>16</v>
       </c>
@@ -3299,25 +3293,25 @@
       <c r="C30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="41" t="s">
+      <c r="D30" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F30" s="70" t="s">
+      <c r="F30" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G30" s="41" t="s">
+      <c r="G30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="41" t="s">
+      <c r="H30" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J30" s="41" t="s">
+      <c r="J30" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K30" s="12" t="s">
@@ -3326,14 +3320,14 @@
       <c r="L30" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M30" s="57" t="s">
+      <c r="M30" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N30" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="56" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>16</v>
       </c>
@@ -3343,7 +3337,7 @@
       <c r="C31" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="41" t="s">
+      <c r="D31" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E31" s="12" t="s">
@@ -3352,16 +3346,16 @@
       <c r="F31" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G31" s="41" t="s">
+      <c r="G31" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H31" s="41" t="s">
+      <c r="H31" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I31" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J31" s="41" t="s">
+      <c r="J31" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K31" s="12" t="s">
@@ -3370,14 +3364,14 @@
       <c r="L31" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M31" s="57" t="s">
+      <c r="M31" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N31" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="56" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>16</v>
       </c>
@@ -3387,7 +3381,7 @@
       <c r="C32" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="41" t="s">
+      <c r="D32" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E32" s="12" t="s">
@@ -3396,16 +3390,16 @@
       <c r="F32" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G32" s="41" t="s">
+      <c r="G32" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H32" s="41" t="s">
+      <c r="H32" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I32" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J32" s="41" t="s">
+      <c r="J32" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K32" s="12" t="s">
@@ -3414,14 +3408,14 @@
       <c r="L32" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M32" s="57" t="s">
+      <c r="M32" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N32" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="56" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>16</v>
       </c>
@@ -3431,7 +3425,7 @@
       <c r="C33" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="41" t="s">
+      <c r="D33" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E33" s="12" t="s">
@@ -3440,16 +3434,16 @@
       <c r="F33" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G33" s="41" t="s">
+      <c r="G33" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H33" s="41" t="s">
+      <c r="H33" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I33" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J33" s="41" t="s">
+      <c r="J33" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K33" s="12" t="s">
@@ -3458,14 +3452,14 @@
       <c r="L33" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M33" s="57" t="s">
+      <c r="M33" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N33" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="56" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>16</v>
       </c>
@@ -3475,7 +3469,7 @@
       <c r="C34" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="41" t="s">
+      <c r="D34" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E34" s="12" t="s">
@@ -3484,16 +3478,16 @@
       <c r="F34" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G34" s="41" t="s">
+      <c r="G34" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H34" s="41" t="s">
+      <c r="H34" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I34" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J34" s="41" t="s">
+      <c r="J34" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K34" s="12" t="s">
@@ -3502,14 +3496,14 @@
       <c r="L34" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M34" s="57" t="s">
+      <c r="M34" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N34" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="56" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>16</v>
       </c>
@@ -3519,7 +3513,7 @@
       <c r="C35" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="41" t="s">
+      <c r="D35" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E35" s="12" t="s">
@@ -3528,16 +3522,16 @@
       <c r="F35" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G35" s="41" t="s">
+      <c r="G35" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="41" t="s">
+      <c r="H35" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I35" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J35" s="41" t="s">
+      <c r="J35" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K35" s="12" t="s">
@@ -3546,14 +3540,14 @@
       <c r="L35" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M35" s="57" t="s">
+      <c r="M35" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N35" s="12" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="56" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>16</v>
       </c>
@@ -3563,7 +3557,7 @@
       <c r="C36" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="41" t="s">
+      <c r="D36" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E36" s="12" t="s">
@@ -3572,16 +3566,16 @@
       <c r="F36" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G36" s="41" t="s">
+      <c r="G36" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H36" s="41" t="s">
+      <c r="H36" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I36" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J36" s="41" t="s">
+      <c r="J36" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K36" s="12" t="s">
@@ -3590,14 +3584,14 @@
       <c r="L36" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M36" s="57" t="s">
+      <c r="M36" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N36" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="56" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>16</v>
       </c>
@@ -3607,7 +3601,7 @@
       <c r="C37" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="41" t="s">
+      <c r="D37" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E37" s="12" t="s">
@@ -3616,16 +3610,16 @@
       <c r="F37" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G37" s="41" t="s">
+      <c r="G37" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H37" s="41" t="s">
+      <c r="H37" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I37" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J37" s="41" t="s">
+      <c r="J37" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K37" s="12" t="s">
@@ -3634,14 +3628,14 @@
       <c r="L37" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M37" s="57" t="s">
+      <c r="M37" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N37" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="56" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>16</v>
       </c>
@@ -3651,7 +3645,7 @@
       <c r="C38" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E38" s="12" t="s">
@@ -3660,16 +3654,16 @@
       <c r="F38" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G38" s="41" t="s">
+      <c r="G38" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H38" s="41" t="s">
+      <c r="H38" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I38" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J38" s="41" t="s">
+      <c r="J38" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K38" s="12" t="s">
@@ -3678,14 +3672,14 @@
       <c r="L38" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M38" s="57" t="s">
+      <c r="M38" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N38" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:14" s="56" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>16</v>
       </c>
@@ -3695,7 +3689,7 @@
       <c r="C39" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="41" t="s">
+      <c r="D39" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E39" s="12" t="s">
@@ -3704,16 +3698,16 @@
       <c r="F39" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G39" s="41" t="s">
+      <c r="G39" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H39" s="41" t="s">
+      <c r="H39" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I39" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J39" s="41" t="s">
+      <c r="J39" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K39" s="12" t="s">
@@ -3722,14 +3716,14 @@
       <c r="L39" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M39" s="57" t="s">
+      <c r="M39" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N39" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="56" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>16</v>
       </c>
@@ -3739,7 +3733,7 @@
       <c r="C40" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="41" t="s">
+      <c r="D40" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E40" s="12" t="s">
@@ -3748,16 +3742,16 @@
       <c r="F40" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G40" s="41" t="s">
+      <c r="G40" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H40" s="41" t="s">
+      <c r="H40" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I40" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J40" s="41" t="s">
+      <c r="J40" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K40" s="12" t="s">
@@ -3766,14 +3760,14 @@
       <c r="L40" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M40" s="57" t="s">
+      <c r="M40" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N40" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:14" s="56" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>16</v>
       </c>
@@ -3783,7 +3777,7 @@
       <c r="C41" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D41" s="41" t="s">
+      <c r="D41" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E41" s="12" t="s">
@@ -3792,16 +3786,16 @@
       <c r="F41" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G41" s="41" t="s">
+      <c r="G41" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H41" s="41" t="s">
+      <c r="H41" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I41" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J41" s="41" t="s">
+      <c r="J41" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K41" s="12" t="s">
@@ -3810,14 +3804,14 @@
       <c r="L41" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M41" s="57" t="s">
+      <c r="M41" s="56" t="s">
         <v>76</v>
       </c>
       <c r="N41" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="56" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -3833,7 +3827,7 @@
       <c r="M42" s="12"/>
       <c r="N42" s="12"/>
     </row>
-    <row r="43" spans="1:14" s="56" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
@@ -3849,7 +3843,7 @@
       <c r="M43" s="12"/>
       <c r="N43" s="12"/>
     </row>
-    <row r="44" spans="1:14" s="56" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
@@ -3865,7 +3859,7 @@
       <c r="M44" s="12"/>
       <c r="N44" s="12"/>
     </row>
-    <row r="45" spans="1:14" s="56" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
@@ -3881,7 +3875,7 @@
       <c r="M45" s="12"/>
       <c r="N45" s="12"/>
     </row>
-    <row r="46" spans="1:14" s="56" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
@@ -3897,7 +3891,7 @@
       <c r="M46" s="12"/>
       <c r="N46" s="12"/>
     </row>
-    <row r="47" spans="1:14" s="56" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
@@ -3913,7 +3907,7 @@
       <c r="M47" s="12"/>
       <c r="N47" s="12"/>
     </row>
-    <row r="48" spans="1:14" s="56" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
@@ -3929,7 +3923,7 @@
       <c r="M48" s="12"/>
       <c r="N48" s="12"/>
     </row>
-    <row r="49" spans="1:14" s="56" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
@@ -3945,7 +3939,7 @@
       <c r="M49" s="12"/>
       <c r="N49" s="12"/>
     </row>
-    <row r="50" spans="1:14" s="56" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
@@ -3961,7 +3955,7 @@
       <c r="M50" s="12"/>
       <c r="N50" s="12"/>
     </row>
-    <row r="51" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
@@ -3977,7 +3971,7 @@
       <c r="M51" s="13"/>
       <c r="N51" s="13"/>
     </row>
-    <row r="52" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="13"/>
@@ -3993,7 +3987,7 @@
       <c r="M52" s="13"/>
       <c r="N52" s="13"/>
     </row>
-    <row r="53" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
@@ -4009,7 +4003,7 @@
       <c r="M53" s="13"/>
       <c r="N53" s="13"/>
     </row>
-    <row r="54" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
@@ -4019,13 +4013,13 @@
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
-      <c r="J54" s="47"/>
-      <c r="K54" s="47"/>
-      <c r="L54" s="47"/>
-      <c r="M54" s="47"/>
+      <c r="J54" s="46"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="46"/>
+      <c r="M54" s="46"/>
       <c r="N54" s="13"/>
     </row>
-    <row r="55" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="13"/>
@@ -4035,13 +4029,13 @@
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
       <c r="I55" s="13"/>
-      <c r="J55" s="48"/>
+      <c r="J55" s="47"/>
       <c r="K55" s="13"/>
-      <c r="L55" s="48"/>
-      <c r="M55" s="48"/>
+      <c r="L55" s="47"/>
+      <c r="M55" s="47"/>
       <c r="N55" s="13"/>
     </row>
-    <row r="56" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
@@ -4053,11 +4047,11 @@
       <c r="I56" s="13"/>
       <c r="J56" s="13"/>
       <c r="K56" s="13"/>
-      <c r="L56" s="48"/>
-      <c r="M56" s="48"/>
+      <c r="L56" s="47"/>
+      <c r="M56" s="47"/>
       <c r="N56" s="13"/>
     </row>
-    <row r="57" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="13"/>
@@ -4069,11 +4063,11 @@
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
       <c r="K57" s="13"/>
-      <c r="L57" s="48"/>
-      <c r="M57" s="48"/>
+      <c r="L57" s="47"/>
+      <c r="M57" s="47"/>
       <c r="N57" s="13"/>
     </row>
-    <row r="58" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
@@ -4089,7 +4083,7 @@
       <c r="M58" s="13"/>
       <c r="N58" s="13"/>
     </row>
-    <row r="59" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
@@ -4105,7 +4099,7 @@
       <c r="M59" s="13"/>
       <c r="N59" s="13"/>
     </row>
-    <row r="60" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
@@ -4121,7 +4115,7 @@
       <c r="M60" s="13"/>
       <c r="N60" s="13"/>
     </row>
-    <row r="61" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
@@ -4137,7 +4131,7 @@
       <c r="M61" s="13"/>
       <c r="N61" s="13"/>
     </row>
-    <row r="62" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -4153,7 +4147,7 @@
       <c r="M62" s="13"/>
       <c r="N62" s="13"/>
     </row>
-    <row r="63" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
@@ -4169,36 +4163,36 @@
       <c r="M63" s="13"/>
       <c r="N63" s="13"/>
     </row>
-    <row r="64" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="3:13" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="3:13" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="J66" s="50"/>
-      <c r="K66" s="50"/>
-      <c r="L66" s="50"/>
-      <c r="M66" s="50"/>
-    </row>
-    <row r="67" spans="3:13" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="J67" s="51"/>
-      <c r="L67" s="51"/>
-      <c r="M67" s="51"/>
-    </row>
-    <row r="68" spans="3:13" s="45" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="C68" s="49"/>
-      <c r="F68" s="49"/>
-      <c r="J68" s="52"/>
-      <c r="K68" s="49"/>
-      <c r="L68" s="51"/>
-      <c r="M68" s="51"/>
-    </row>
-    <row r="69" spans="3:13" s="45" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="C69" s="49"/>
-      <c r="F69" s="49"/>
-      <c r="J69" s="52"/>
-      <c r="K69" s="49"/>
-      <c r="L69" s="51"/>
-      <c r="M69" s="51"/>
-    </row>
-    <row r="70" spans="3:13" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="65" spans="3:13" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="66" spans="3:13" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J66" s="49"/>
+      <c r="K66" s="49"/>
+      <c r="L66" s="49"/>
+      <c r="M66" s="49"/>
+    </row>
+    <row r="67" spans="3:13" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J67" s="50"/>
+      <c r="L67" s="50"/>
+      <c r="M67" s="50"/>
+    </row>
+    <row r="68" spans="3:13" s="44" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C68" s="48"/>
+      <c r="F68" s="48"/>
+      <c r="J68" s="51"/>
+      <c r="K68" s="48"/>
+      <c r="L68" s="50"/>
+      <c r="M68" s="50"/>
+    </row>
+    <row r="69" spans="3:13" s="44" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C69" s="48"/>
+      <c r="F69" s="48"/>
+      <c r="J69" s="51"/>
+      <c r="K69" s="48"/>
+      <c r="L69" s="50"/>
+      <c r="M69" s="50"/>
+    </row>
+    <row r="70" spans="3:13" s="24" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C70" s="30"/>
       <c r="F70" s="30"/>
       <c r="J70" s="32"/>
@@ -4206,7 +4200,7 @@
       <c r="L70" s="31"/>
       <c r="M70" s="31"/>
     </row>
-    <row r="71" spans="3:13" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:13" s="24" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C71" s="30"/>
       <c r="F71" s="30"/>
       <c r="J71" s="32"/>
@@ -4214,31 +4208,31 @@
       <c r="L71" s="31"/>
       <c r="M71" s="31"/>
     </row>
-    <row r="72" spans="3:13" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:13" s="33" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C72" s="34"/>
       <c r="F72" s="34"/>
       <c r="K72" s="34"/>
       <c r="M72" s="34"/>
     </row>
-    <row r="73" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C73" s="35"/>
       <c r="F73" s="35"/>
       <c r="K73" s="35"/>
       <c r="M73" s="35"/>
     </row>
-    <row r="74" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C74" s="35"/>
       <c r="F74" s="35"/>
       <c r="K74" s="35"/>
       <c r="M74" s="35"/>
     </row>
-    <row r="75" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C75" s="35"/>
       <c r="F75" s="35"/>
       <c r="K75" s="35"/>
       <c r="M75" s="35"/>
     </row>
-    <row r="76" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C76" s="35"/>
       <c r="F76" s="35"/>
       <c r="J76" s="37"/>
@@ -4246,7 +4240,7 @@
       <c r="L76" s="37"/>
       <c r="M76" s="37"/>
     </row>
-    <row r="77" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C77" s="35"/>
       <c r="F77" s="35"/>
       <c r="J77" s="38"/>
@@ -4254,7 +4248,7 @@
       <c r="L77" s="39"/>
       <c r="M77" s="39"/>
     </row>
-    <row r="78" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C78" s="35"/>
       <c r="F78" s="35"/>
       <c r="J78" s="38"/>
@@ -4262,7 +4256,7 @@
       <c r="L78" s="39"/>
       <c r="M78" s="39"/>
     </row>
-    <row r="79" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C79" s="35"/>
       <c r="F79" s="35"/>
       <c r="J79" s="38"/>
@@ -4270,7 +4264,7 @@
       <c r="L79" s="39"/>
       <c r="M79" s="39"/>
     </row>
-    <row r="80" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C80" s="35"/>
       <c r="F80" s="35"/>
       <c r="J80" s="38"/>
@@ -4278,7 +4272,7 @@
       <c r="L80" s="38"/>
       <c r="M80" s="38"/>
     </row>
-    <row r="81" spans="1:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C81" s="35"/>
       <c r="F81" s="35"/>
       <c r="J81" s="38"/>
@@ -4286,31 +4280,31 @@
       <c r="L81" s="38"/>
       <c r="M81" s="38"/>
     </row>
-    <row r="82" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C82" s="18"/>
       <c r="F82" s="18"/>
       <c r="K82" s="18"/>
       <c r="M82" s="18"/>
     </row>
-    <row r="83" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C83" s="18"/>
       <c r="F83" s="18"/>
       <c r="K83" s="18"/>
       <c r="M83" s="18"/>
     </row>
-    <row r="84" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C84" s="18"/>
       <c r="F84" s="18"/>
       <c r="K84" s="18"/>
       <c r="M84" s="18"/>
     </row>
-    <row r="85" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C85" s="18"/>
       <c r="F85" s="18"/>
       <c r="K85" s="18"/>
       <c r="M85" s="18"/>
     </row>
-    <row r="86" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C86" s="18"/>
       <c r="F86" s="18"/>
       <c r="J86" s="15"/>
@@ -4318,7 +4312,7 @@
       <c r="L86" s="15"/>
       <c r="M86" s="15"/>
     </row>
-    <row r="87" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C87" s="18"/>
       <c r="F87" s="18"/>
       <c r="J87" s="17"/>
@@ -4326,7 +4320,7 @@
       <c r="L87" s="16"/>
       <c r="M87" s="16"/>
     </row>
-    <row r="88" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C88" s="18"/>
       <c r="F88" s="18"/>
       <c r="J88" s="17"/>
@@ -4334,7 +4328,7 @@
       <c r="L88" s="16"/>
       <c r="M88" s="16"/>
     </row>
-    <row r="89" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C89" s="18"/>
       <c r="F89" s="18"/>
       <c r="J89" s="17"/>
@@ -4342,7 +4336,7 @@
       <c r="L89" s="16"/>
       <c r="M89" s="16"/>
     </row>
-    <row r="90" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C90" s="18"/>
       <c r="F90" s="18"/>
       <c r="J90" s="17"/>
@@ -4350,7 +4344,7 @@
       <c r="L90" s="17"/>
       <c r="M90" s="17"/>
     </row>
-    <row r="91" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C91" s="18"/>
       <c r="F91" s="18"/>
       <c r="J91" s="17"/>
@@ -4358,7 +4352,7 @@
       <c r="L91" s="17"/>
       <c r="M91" s="17"/>
     </row>
-    <row r="92" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="20"/>
       <c r="C92" s="18"/>
       <c r="D92" s="18"/>
@@ -4370,7 +4364,7 @@
       <c r="K92" s="18"/>
       <c r="M92" s="18"/>
     </row>
-    <row r="93" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C93" s="18"/>
       <c r="D93" s="18"/>
       <c r="E93" s="18"/>
@@ -4381,7 +4375,7 @@
       <c r="K93" s="18"/>
       <c r="M93" s="18"/>
     </row>
-    <row r="94" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C94" s="18"/>
       <c r="D94" s="18"/>
       <c r="E94" s="18"/>
@@ -4392,7 +4386,7 @@
       <c r="K94" s="18"/>
       <c r="M94" s="18"/>
     </row>
-    <row r="95" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C95" s="18"/>
       <c r="D95" s="18"/>
       <c r="E95" s="18"/>
@@ -4403,7 +4397,7 @@
       <c r="K95" s="18"/>
       <c r="M95" s="18"/>
     </row>
-    <row r="96" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C96" s="18"/>
       <c r="D96" s="18"/>
       <c r="E96" s="18"/>
@@ -4414,7 +4408,7 @@
       <c r="K96" s="18"/>
       <c r="M96" s="18"/>
     </row>
-    <row r="97" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C97" s="18"/>
       <c r="D97" s="18"/>
       <c r="E97" s="18"/>
@@ -4425,7 +4419,7 @@
       <c r="K97" s="18"/>
       <c r="M97" s="18"/>
     </row>
-    <row r="98" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C98" s="18"/>
       <c r="D98" s="18"/>
       <c r="E98" s="18"/>
@@ -4436,7 +4430,7 @@
       <c r="K98" s="18"/>
       <c r="M98" s="18"/>
     </row>
-    <row r="99" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C99" s="18"/>
       <c r="D99" s="18"/>
       <c r="E99" s="18"/>
@@ -4448,7 +4442,6 @@
       <c r="M99" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1"/>
   <mergeCells count="6">
     <mergeCell ref="A29:XFD29"/>
     <mergeCell ref="A5:XFD5"/>

</xml_diff>

<commit_message>
549587 Update on 1/22/18 per Release Office Feedback
</commit_message>
<xml_diff>
--- a/Requirement/Build 4/TAS eBilling RTM IB_ 2.0_592.xlsx
+++ b/Requirement/Build 4/TAS eBilling RTM IB_ 2.0_592.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="112">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -360,9 +360,6 @@
     <t>DE316, DE318</t>
   </si>
   <si>
-    <t>US 1108/US131 - Enter/Edit Dental Claims</t>
-  </si>
-  <si>
     <t>US 1108 - Enter/Edit Dental Claims                  US 131 - Create 837D Transaction</t>
   </si>
   <si>
@@ -384,6 +381,33 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>TC1237 - CIT eBilling  TS Validate the existing claims Still Display on the TPJI screen when there is an active Outpatient Dental Claim (O/D)  Regression US14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US 1108/US131 - Enter/Edit Dental Claims    </t>
+  </si>
+  <si>
+    <t>TC1227 -CIT eBilling  TS eBilling create a CMS 1500 Outpatient Professional Claim - Regression US1108 &amp; US131</t>
+  </si>
+  <si>
+    <t>TC1228 -CIT  eBilling  TS Create a UB04 (Inst) Claim - Regression US1108 &amp; US131</t>
+  </si>
+  <si>
+    <t>TC1229 - CIT  eBilling Create an Institutional Claim via Autobiller - Regression US1109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US2487 - Insurance Company Entry/Edit - Dental      </t>
+  </si>
+  <si>
+    <t>TC2232 -CIT eBilling US2487 - Insurance Company Entry/Edit - Dental - Regression Not applicable</t>
+  </si>
+  <si>
+    <t>TC2231 -CIT eBilling US2488 - Update Reports - Form Type J430D - Regression Not applicable</t>
+  </si>
+  <si>
+    <t>TC2230 - CIT eBilling TS18 MRW - Print MRA US2489 - Regression</t>
   </si>
 </sst>
 </file>
@@ -925,6 +949,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -954,9 +981,6 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1203,7 +1227,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1545,31 +1569,31 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:8" ht="22.9" x14ac:dyDescent="0.4">
-      <c r="A5" s="70" t="s">
+      <c r="A5" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
     </row>
     <row r="6" spans="1:8" ht="22.9" x14ac:dyDescent="0.4">
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
     </row>
     <row r="8" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
       <c r="C8" s="3"/>
@@ -1614,16 +1638,16 @@
       <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="74" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
     </row>
     <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
@@ -1634,16 +1658,16 @@
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="74"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="74"/>
-      <c r="H26" s="74"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
@@ -1696,12 +1720,12 @@
       <c r="A1" s="7"/>
     </row>
     <row r="2" spans="1:4" ht="17.45" x14ac:dyDescent="0.3">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
     </row>
     <row r="3" spans="1:4" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
@@ -1842,20 +1866,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DQ99"/>
+  <dimension ref="A1:DQ106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="19" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="10" customWidth="1"/>
-    <col min="6" max="6" width="57.28515625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="46.28515625" style="10" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="10" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" style="10" customWidth="1"/>
     <col min="9" max="9" width="13.140625" style="10" customWidth="1"/>
@@ -2042,7 +2064,7 @@
       <c r="B3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="80" t="s">
+      <c r="C3" s="70" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="40" t="s">
@@ -2051,7 +2073,7 @@
       <c r="E3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="80" t="s">
+      <c r="F3" s="70" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="13" t="s">
@@ -2080,14 +2102,14 @@
       </c>
       <c r="O3" s="13"/>
     </row>
-    <row r="4" spans="1:121" s="42" customFormat="1" ht="61.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:121" s="42" customFormat="1" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="70" t="s">
         <v>32</v>
       </c>
       <c r="D4" s="40" t="s">
@@ -2125,176 +2147,177 @@
       </c>
       <c r="O4" s="13"/>
     </row>
-    <row r="5" spans="1:121" s="76" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="76" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="77"/>
-      <c r="S5" s="77"/>
-      <c r="T5" s="77"/>
-      <c r="U5" s="77"/>
-      <c r="V5" s="77"/>
-      <c r="W5" s="77"/>
-      <c r="X5" s="77"/>
-      <c r="Y5" s="77"/>
-      <c r="Z5" s="77"/>
-      <c r="AA5" s="77"/>
-      <c r="AB5" s="77"/>
-      <c r="AC5" s="77"/>
-      <c r="AD5" s="77"/>
-      <c r="AE5" s="77"/>
-      <c r="AF5" s="77"/>
-      <c r="AG5" s="77"/>
-      <c r="AH5" s="77"/>
-      <c r="AI5" s="77"/>
-      <c r="AJ5" s="77"/>
-      <c r="AK5" s="77"/>
-      <c r="AL5" s="77"/>
-      <c r="AM5" s="77"/>
-      <c r="AN5" s="77"/>
-      <c r="AO5" s="77"/>
-      <c r="AP5" s="77"/>
-      <c r="AQ5" s="77"/>
-      <c r="AR5" s="77"/>
-      <c r="AS5" s="77"/>
-      <c r="AT5" s="77"/>
-      <c r="AU5" s="77"/>
-      <c r="AV5" s="77"/>
-      <c r="AW5" s="77"/>
-      <c r="AX5" s="77"/>
-      <c r="AY5" s="77"/>
-      <c r="AZ5" s="77"/>
-      <c r="BA5" s="77"/>
-      <c r="BB5" s="77"/>
-      <c r="BC5" s="77"/>
-      <c r="BD5" s="77"/>
-      <c r="BE5" s="77"/>
-      <c r="BF5" s="77"/>
-      <c r="BG5" s="77"/>
-      <c r="BH5" s="77"/>
-      <c r="BI5" s="77"/>
-      <c r="BJ5" s="77"/>
-      <c r="BK5" s="77"/>
-      <c r="BL5" s="77"/>
-      <c r="BM5" s="77"/>
-      <c r="BN5" s="77"/>
-      <c r="BO5" s="77"/>
-      <c r="BP5" s="77"/>
-      <c r="BQ5" s="77"/>
-      <c r="BR5" s="77"/>
-      <c r="BS5" s="77"/>
-      <c r="BT5" s="77"/>
-      <c r="BU5" s="77"/>
-      <c r="BV5" s="77"/>
-      <c r="BW5" s="77"/>
-      <c r="BX5" s="77"/>
-      <c r="BY5" s="77"/>
-      <c r="BZ5" s="77"/>
-      <c r="CA5" s="77"/>
-      <c r="CB5" s="77"/>
-      <c r="CC5" s="77"/>
-      <c r="CD5" s="77"/>
-      <c r="CE5" s="77"/>
-      <c r="CF5" s="77"/>
-      <c r="CG5" s="77"/>
-      <c r="CH5" s="77"/>
-      <c r="CI5" s="77"/>
-      <c r="CJ5" s="77"/>
-      <c r="CK5" s="77"/>
-      <c r="CL5" s="77"/>
-      <c r="CM5" s="77"/>
-      <c r="CN5" s="77"/>
-      <c r="CO5" s="77"/>
-      <c r="CP5" s="77"/>
-      <c r="CQ5" s="77"/>
-      <c r="CR5" s="77"/>
-      <c r="CS5" s="77"/>
-      <c r="CT5" s="77"/>
-      <c r="CU5" s="77"/>
-      <c r="CV5" s="77"/>
-      <c r="CW5" s="77"/>
-      <c r="CX5" s="77"/>
-      <c r="CY5" s="77"/>
-      <c r="CZ5" s="77"/>
-      <c r="DA5" s="77"/>
-      <c r="DB5" s="77"/>
-      <c r="DC5" s="77"/>
-      <c r="DD5" s="77"/>
-      <c r="DE5" s="77"/>
-      <c r="DF5" s="77"/>
-      <c r="DG5" s="77"/>
-      <c r="DH5" s="77"/>
-      <c r="DI5" s="77"/>
-      <c r="DJ5" s="77"/>
-      <c r="DK5" s="77"/>
-      <c r="DL5" s="77"/>
-      <c r="DM5" s="77"/>
-      <c r="DN5" s="77"/>
-      <c r="DO5" s="77"/>
-      <c r="DP5" s="77"/>
-      <c r="DQ5" s="77"/>
-    </row>
-    <row r="6" spans="1:121" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="40" t="s">
+    <row r="5" spans="1:121" s="42" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="70" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="13" t="s">
+      <c r="H5" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J6" s="41" t="s">
+      <c r="J5" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="13" t="s">
+      <c r="K5" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="56" t="s">
+      <c r="M5" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="N6" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:121" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="N5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="13"/>
+    </row>
+    <row r="6" spans="1:121" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="78"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="78"/>
+      <c r="S6" s="78"/>
+      <c r="T6" s="78"/>
+      <c r="U6" s="78"/>
+      <c r="V6" s="78"/>
+      <c r="W6" s="78"/>
+      <c r="X6" s="78"/>
+      <c r="Y6" s="78"/>
+      <c r="Z6" s="78"/>
+      <c r="AA6" s="78"/>
+      <c r="AB6" s="78"/>
+      <c r="AC6" s="78"/>
+      <c r="AD6" s="78"/>
+      <c r="AE6" s="78"/>
+      <c r="AF6" s="78"/>
+      <c r="AG6" s="78"/>
+      <c r="AH6" s="78"/>
+      <c r="AI6" s="78"/>
+      <c r="AJ6" s="78"/>
+      <c r="AK6" s="78"/>
+      <c r="AL6" s="78"/>
+      <c r="AM6" s="78"/>
+      <c r="AN6" s="78"/>
+      <c r="AO6" s="78"/>
+      <c r="AP6" s="78"/>
+      <c r="AQ6" s="78"/>
+      <c r="AR6" s="78"/>
+      <c r="AS6" s="78"/>
+      <c r="AT6" s="78"/>
+      <c r="AU6" s="78"/>
+      <c r="AV6" s="78"/>
+      <c r="AW6" s="78"/>
+      <c r="AX6" s="78"/>
+      <c r="AY6" s="78"/>
+      <c r="AZ6" s="78"/>
+      <c r="BA6" s="78"/>
+      <c r="BB6" s="78"/>
+      <c r="BC6" s="78"/>
+      <c r="BD6" s="78"/>
+      <c r="BE6" s="78"/>
+      <c r="BF6" s="78"/>
+      <c r="BG6" s="78"/>
+      <c r="BH6" s="78"/>
+      <c r="BI6" s="78"/>
+      <c r="BJ6" s="78"/>
+      <c r="BK6" s="78"/>
+      <c r="BL6" s="78"/>
+      <c r="BM6" s="78"/>
+      <c r="BN6" s="78"/>
+      <c r="BO6" s="78"/>
+      <c r="BP6" s="78"/>
+      <c r="BQ6" s="78"/>
+      <c r="BR6" s="78"/>
+      <c r="BS6" s="78"/>
+      <c r="BT6" s="78"/>
+      <c r="BU6" s="78"/>
+      <c r="BV6" s="78"/>
+      <c r="BW6" s="78"/>
+      <c r="BX6" s="78"/>
+      <c r="BY6" s="78"/>
+      <c r="BZ6" s="78"/>
+      <c r="CA6" s="78"/>
+      <c r="CB6" s="78"/>
+      <c r="CC6" s="78"/>
+      <c r="CD6" s="78"/>
+      <c r="CE6" s="78"/>
+      <c r="CF6" s="78"/>
+      <c r="CG6" s="78"/>
+      <c r="CH6" s="78"/>
+      <c r="CI6" s="78"/>
+      <c r="CJ6" s="78"/>
+      <c r="CK6" s="78"/>
+      <c r="CL6" s="78"/>
+      <c r="CM6" s="78"/>
+      <c r="CN6" s="78"/>
+      <c r="CO6" s="78"/>
+      <c r="CP6" s="78"/>
+      <c r="CQ6" s="78"/>
+      <c r="CR6" s="78"/>
+      <c r="CS6" s="78"/>
+      <c r="CT6" s="78"/>
+      <c r="CU6" s="78"/>
+      <c r="CV6" s="78"/>
+      <c r="CW6" s="78"/>
+      <c r="CX6" s="78"/>
+      <c r="CY6" s="78"/>
+      <c r="CZ6" s="78"/>
+      <c r="DA6" s="78"/>
+      <c r="DB6" s="78"/>
+      <c r="DC6" s="78"/>
+      <c r="DD6" s="78"/>
+      <c r="DE6" s="78"/>
+      <c r="DF6" s="78"/>
+      <c r="DG6" s="78"/>
+      <c r="DH6" s="78"/>
+      <c r="DI6" s="78"/>
+      <c r="DJ6" s="78"/>
+      <c r="DK6" s="78"/>
+      <c r="DL6" s="78"/>
+      <c r="DM6" s="78"/>
+      <c r="DN6" s="78"/>
+      <c r="DO6" s="78"/>
+      <c r="DP6" s="78"/>
+      <c r="DQ6" s="78"/>
+    </row>
+    <row r="7" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>16</v>
       </c>
@@ -2308,7 +2331,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>21</v>
@@ -2326,7 +2349,7 @@
         <v>17</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>39</v>
+        <v>105</v>
       </c>
       <c r="L7" s="13" t="s">
         <v>35</v>
@@ -2335,10 +2358,10 @@
         <v>76</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:121" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>16</v>
       </c>
@@ -2352,7 +2375,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>21</v>
@@ -2370,7 +2393,7 @@
         <v>17</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="L8" s="13" t="s">
         <v>35</v>
@@ -2379,10 +2402,10 @@
         <v>76</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:121" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>16</v>
       </c>
@@ -2414,7 +2437,7 @@
         <v>17</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L9" s="13" t="s">
         <v>35</v>
@@ -2423,10 +2446,10 @@
         <v>76</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:121" s="43" customFormat="1" ht="97.9" customHeight="1" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>16</v>
       </c>
@@ -2440,7 +2463,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>21</v>
@@ -2458,7 +2481,7 @@
         <v>17</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L10" s="13" t="s">
         <v>35</v>
@@ -2467,24 +2490,24 @@
         <v>76</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:121" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D11" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>21</v>
@@ -2502,7 +2525,7 @@
         <v>17</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L11" s="13" t="s">
         <v>35</v>
@@ -2511,10 +2534,10 @@
         <v>76</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:121" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>16</v>
       </c>
@@ -2528,7 +2551,7 @@
         <v>16</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>21</v>
@@ -2546,7 +2569,7 @@
         <v>17</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="L12" s="13" t="s">
         <v>35</v>
@@ -2555,137 +2578,56 @@
         <v>76</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:121" s="76" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="76" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="77"/>
-      <c r="J13" s="77"/>
-      <c r="K13" s="77"/>
-      <c r="L13" s="77"/>
-      <c r="M13" s="77"/>
-      <c r="N13" s="77"/>
-      <c r="O13" s="77"/>
-      <c r="P13" s="77"/>
-      <c r="Q13" s="77"/>
-      <c r="R13" s="77"/>
-      <c r="S13" s="77"/>
-      <c r="T13" s="77"/>
-      <c r="U13" s="77"/>
-      <c r="V13" s="77"/>
-      <c r="W13" s="77"/>
-      <c r="X13" s="77"/>
-      <c r="Y13" s="77"/>
-      <c r="Z13" s="77"/>
-      <c r="AA13" s="77"/>
-      <c r="AB13" s="77"/>
-      <c r="AC13" s="77"/>
-      <c r="AD13" s="77"/>
-      <c r="AE13" s="77"/>
-      <c r="AF13" s="77"/>
-      <c r="AG13" s="77"/>
-      <c r="AH13" s="77"/>
-      <c r="AI13" s="77"/>
-      <c r="AJ13" s="77"/>
-      <c r="AK13" s="77"/>
-      <c r="AL13" s="77"/>
-      <c r="AM13" s="77"/>
-      <c r="AN13" s="77"/>
-      <c r="AO13" s="77"/>
-      <c r="AP13" s="77"/>
-      <c r="AQ13" s="77"/>
-      <c r="AR13" s="77"/>
-      <c r="AS13" s="77"/>
-      <c r="AT13" s="77"/>
-      <c r="AU13" s="77"/>
-      <c r="AV13" s="77"/>
-      <c r="AW13" s="77"/>
-      <c r="AX13" s="77"/>
-      <c r="AY13" s="77"/>
-      <c r="AZ13" s="77"/>
-      <c r="BA13" s="77"/>
-      <c r="BB13" s="77"/>
-      <c r="BC13" s="77"/>
-      <c r="BD13" s="77"/>
-      <c r="BE13" s="77"/>
-      <c r="BF13" s="77"/>
-      <c r="BG13" s="77"/>
-      <c r="BH13" s="77"/>
-      <c r="BI13" s="77"/>
-      <c r="BJ13" s="77"/>
-      <c r="BK13" s="77"/>
-      <c r="BL13" s="77"/>
-      <c r="BM13" s="77"/>
-      <c r="BN13" s="77"/>
-      <c r="BO13" s="77"/>
-      <c r="BP13" s="77"/>
-      <c r="BQ13" s="77"/>
-      <c r="BR13" s="77"/>
-      <c r="BS13" s="77"/>
-      <c r="BT13" s="77"/>
-      <c r="BU13" s="77"/>
-      <c r="BV13" s="77"/>
-      <c r="BW13" s="77"/>
-      <c r="BX13" s="77"/>
-      <c r="BY13" s="77"/>
-      <c r="BZ13" s="77"/>
-      <c r="CA13" s="77"/>
-      <c r="CB13" s="77"/>
-      <c r="CC13" s="77"/>
-      <c r="CD13" s="77"/>
-      <c r="CE13" s="77"/>
-      <c r="CF13" s="77"/>
-      <c r="CG13" s="77"/>
-      <c r="CH13" s="77"/>
-      <c r="CI13" s="77"/>
-      <c r="CJ13" s="77"/>
-      <c r="CK13" s="77"/>
-      <c r="CL13" s="77"/>
-      <c r="CM13" s="77"/>
-      <c r="CN13" s="77"/>
-      <c r="CO13" s="77"/>
-      <c r="CP13" s="77"/>
-      <c r="CQ13" s="77"/>
-      <c r="CR13" s="77"/>
-      <c r="CS13" s="77"/>
-      <c r="CT13" s="77"/>
-      <c r="CU13" s="77"/>
-      <c r="CV13" s="77"/>
-      <c r="CW13" s="77"/>
-      <c r="CX13" s="77"/>
-      <c r="CY13" s="77"/>
-      <c r="CZ13" s="77"/>
-      <c r="DA13" s="77"/>
-      <c r="DB13" s="77"/>
-      <c r="DC13" s="77"/>
-      <c r="DD13" s="77"/>
-      <c r="DE13" s="77"/>
-      <c r="DF13" s="77"/>
-      <c r="DG13" s="77"/>
-      <c r="DH13" s="77"/>
-      <c r="DI13" s="77"/>
-      <c r="DJ13" s="77"/>
-      <c r="DK13" s="77"/>
-      <c r="DL13" s="77"/>
-      <c r="DM13" s="77"/>
-      <c r="DN13" s="77"/>
-      <c r="DO13" s="77"/>
-      <c r="DP13" s="77"/>
-      <c r="DQ13" s="77"/>
-    </row>
-    <row r="14" spans="1:121" s="43" customFormat="1" ht="97.9" customHeight="1" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>31</v>
@@ -2697,10 +2639,10 @@
         <v>16</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G14" s="40" t="s">
         <v>15</v>
@@ -2711,11 +2653,11 @@
       <c r="I14" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J14" s="40" t="s">
+      <c r="J14" s="41" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L14" s="13" t="s">
         <v>35</v>
@@ -2724,72 +2666,179 @@
         <v>76</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:121" s="78" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="79"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="79"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="79"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="79"/>
-    </row>
-    <row r="16" spans="1:121" s="43" customFormat="1" ht="154.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="40" t="s">
+      <c r="C15" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="13" t="s">
+      <c r="H15" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J16" s="40" t="s">
+      <c r="J15" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="L16" s="13" t="s">
+      <c r="K15" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M16" s="56" t="s">
+      <c r="M15" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="N16" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" s="43" customFormat="1" ht="151.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N15" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:121" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="78"/>
+      <c r="L16" s="78"/>
+      <c r="M16" s="78"/>
+      <c r="N16" s="78"/>
+      <c r="O16" s="78"/>
+      <c r="P16" s="78"/>
+      <c r="Q16" s="78"/>
+      <c r="R16" s="78"/>
+      <c r="S16" s="78"/>
+      <c r="T16" s="78"/>
+      <c r="U16" s="78"/>
+      <c r="V16" s="78"/>
+      <c r="W16" s="78"/>
+      <c r="X16" s="78"/>
+      <c r="Y16" s="78"/>
+      <c r="Z16" s="78"/>
+      <c r="AA16" s="78"/>
+      <c r="AB16" s="78"/>
+      <c r="AC16" s="78"/>
+      <c r="AD16" s="78"/>
+      <c r="AE16" s="78"/>
+      <c r="AF16" s="78"/>
+      <c r="AG16" s="78"/>
+      <c r="AH16" s="78"/>
+      <c r="AI16" s="78"/>
+      <c r="AJ16" s="78"/>
+      <c r="AK16" s="78"/>
+      <c r="AL16" s="78"/>
+      <c r="AM16" s="78"/>
+      <c r="AN16" s="78"/>
+      <c r="AO16" s="78"/>
+      <c r="AP16" s="78"/>
+      <c r="AQ16" s="78"/>
+      <c r="AR16" s="78"/>
+      <c r="AS16" s="78"/>
+      <c r="AT16" s="78"/>
+      <c r="AU16" s="78"/>
+      <c r="AV16" s="78"/>
+      <c r="AW16" s="78"/>
+      <c r="AX16" s="78"/>
+      <c r="AY16" s="78"/>
+      <c r="AZ16" s="78"/>
+      <c r="BA16" s="78"/>
+      <c r="BB16" s="78"/>
+      <c r="BC16" s="78"/>
+      <c r="BD16" s="78"/>
+      <c r="BE16" s="78"/>
+      <c r="BF16" s="78"/>
+      <c r="BG16" s="78"/>
+      <c r="BH16" s="78"/>
+      <c r="BI16" s="78"/>
+      <c r="BJ16" s="78"/>
+      <c r="BK16" s="78"/>
+      <c r="BL16" s="78"/>
+      <c r="BM16" s="78"/>
+      <c r="BN16" s="78"/>
+      <c r="BO16" s="78"/>
+      <c r="BP16" s="78"/>
+      <c r="BQ16" s="78"/>
+      <c r="BR16" s="78"/>
+      <c r="BS16" s="78"/>
+      <c r="BT16" s="78"/>
+      <c r="BU16" s="78"/>
+      <c r="BV16" s="78"/>
+      <c r="BW16" s="78"/>
+      <c r="BX16" s="78"/>
+      <c r="BY16" s="78"/>
+      <c r="BZ16" s="78"/>
+      <c r="CA16" s="78"/>
+      <c r="CB16" s="78"/>
+      <c r="CC16" s="78"/>
+      <c r="CD16" s="78"/>
+      <c r="CE16" s="78"/>
+      <c r="CF16" s="78"/>
+      <c r="CG16" s="78"/>
+      <c r="CH16" s="78"/>
+      <c r="CI16" s="78"/>
+      <c r="CJ16" s="78"/>
+      <c r="CK16" s="78"/>
+      <c r="CL16" s="78"/>
+      <c r="CM16" s="78"/>
+      <c r="CN16" s="78"/>
+      <c r="CO16" s="78"/>
+      <c r="CP16" s="78"/>
+      <c r="CQ16" s="78"/>
+      <c r="CR16" s="78"/>
+      <c r="CS16" s="78"/>
+      <c r="CT16" s="78"/>
+      <c r="CU16" s="78"/>
+      <c r="CV16" s="78"/>
+      <c r="CW16" s="78"/>
+      <c r="CX16" s="78"/>
+      <c r="CY16" s="78"/>
+      <c r="CZ16" s="78"/>
+      <c r="DA16" s="78"/>
+      <c r="DB16" s="78"/>
+      <c r="DC16" s="78"/>
+      <c r="DD16" s="78"/>
+      <c r="DE16" s="78"/>
+      <c r="DF16" s="78"/>
+      <c r="DG16" s="78"/>
+      <c r="DH16" s="78"/>
+      <c r="DI16" s="78"/>
+      <c r="DJ16" s="78"/>
+      <c r="DK16" s="78"/>
+      <c r="DL16" s="78"/>
+      <c r="DM16" s="78"/>
+      <c r="DN16" s="78"/>
+      <c r="DO16" s="78"/>
+      <c r="DP16" s="78"/>
+      <c r="DQ16" s="78"/>
+    </row>
+    <row r="17" spans="1:14" s="43" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>16</v>
       </c>
@@ -2803,10 +2852,10 @@
         <v>16</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G17" s="40" t="s">
         <v>15</v>
@@ -2821,7 +2870,7 @@
         <v>17</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L17" s="13" t="s">
         <v>35</v>
@@ -2830,10 +2879,10 @@
         <v>76</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" s="43" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="52" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>16</v>
       </c>
@@ -2847,10 +2896,10 @@
         <v>16</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G18" s="40" t="s">
         <v>15</v>
@@ -2864,8 +2913,8 @@
       <c r="J18" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="12" t="s">
-        <v>49</v>
+      <c r="K18" s="52" t="s">
+        <v>107</v>
       </c>
       <c r="L18" s="13" t="s">
         <v>35</v>
@@ -2874,72 +2923,72 @@
         <v>76</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" s="43" customFormat="1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="79" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="80"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="80"/>
+      <c r="K19" s="80"/>
+      <c r="L19" s="80"/>
+      <c r="M19" s="80"/>
+      <c r="N19" s="80"/>
+    </row>
+    <row r="20" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C20" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="12" t="s">
+      <c r="D20" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F20" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="40" t="s">
+      <c r="G20" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="13" t="s">
+      <c r="H20" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J19" s="40" t="s">
+      <c r="J20" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="L19" s="13" t="s">
+      <c r="K20" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L20" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M19" s="56" t="s">
+      <c r="M20" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="N19" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" s="76" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="76" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="77"/>
-      <c r="C20" s="77"/>
-      <c r="D20" s="77"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="77"/>
-      <c r="G20" s="77"/>
-      <c r="H20" s="77"/>
-      <c r="I20" s="77"/>
-      <c r="J20" s="77"/>
-      <c r="K20" s="77"/>
-      <c r="L20" s="77"/>
-      <c r="M20" s="77"/>
-      <c r="N20" s="77"/>
-    </row>
-    <row r="21" spans="1:14" s="48" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="N20" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>16</v>
       </c>
@@ -2949,29 +2998,29 @@
       <c r="C21" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I21" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J21" s="12" t="s">
+      <c r="J21" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="13" t="s">
-        <v>58</v>
+      <c r="K21" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="L21" s="13" t="s">
         <v>35</v>
@@ -2983,7 +3032,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="48" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>16</v>
       </c>
@@ -2993,29 +3042,29 @@
       <c r="C22" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="H22" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I22" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J22" s="12" t="s">
+      <c r="J22" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="13" t="s">
-        <v>59</v>
+      <c r="K22" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="L22" s="13" t="s">
         <v>35</v>
@@ -3024,10 +3073,10 @@
         <v>76</v>
       </c>
       <c r="N22" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="48" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>16</v>
       </c>
@@ -3037,29 +3086,29 @@
       <c r="C23" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="12" t="s">
+      <c r="H23" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I23" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J23" s="12" t="s">
+      <c r="J23" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="13" t="s">
-        <v>60</v>
+      <c r="K23" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="L23" s="13" t="s">
         <v>35</v>
@@ -3068,10 +3117,10 @@
         <v>76</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" s="48" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>16</v>
       </c>
@@ -3081,103 +3130,103 @@
       <c r="C24" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="12" t="s">
+      <c r="H24" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I24" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J24" s="12" t="s">
+      <c r="J24" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="13" t="s">
-        <v>61</v>
+      <c r="K24" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="L24" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="M24" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="N24" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="77" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="78"/>
+      <c r="C25" s="78"/>
+      <c r="D25" s="78"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="78"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="78"/>
+      <c r="L25" s="78"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="78"/>
+    </row>
+    <row r="26" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="L26" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M24" s="56" t="s">
+      <c r="M26" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="N24" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" s="48" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J25" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K25" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="L25" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M25" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N25" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" s="76" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="76" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="77"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="77"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="77"/>
-      <c r="K26" s="77"/>
-      <c r="L26" s="77"/>
-      <c r="M26" s="77"/>
-      <c r="N26" s="77"/>
-    </row>
-    <row r="27" spans="1:14" s="29" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+      <c r="N26" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>16</v>
       </c>
@@ -3187,29 +3236,29 @@
       <c r="C27" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F27" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="40" t="s">
+      <c r="H27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I27" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J27" s="40" t="s">
+      <c r="J27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="29" t="s">
-        <v>54</v>
+      <c r="K27" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="L27" s="13" t="s">
         <v>35</v>
@@ -3221,7 +3270,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>16</v>
       </c>
@@ -3231,29 +3280,29 @@
       <c r="C28" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="12" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F28" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="40" t="s">
+      <c r="H28" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I28" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J28" s="40" t="s">
+      <c r="J28" s="12" t="s">
         <v>17</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="L28" s="13" t="s">
         <v>35</v>
@@ -3265,25 +3314,51 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="76" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="76" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" s="77"/>
-      <c r="C29" s="77"/>
-      <c r="D29" s="77"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="77"/>
-      <c r="G29" s="77"/>
-      <c r="H29" s="77"/>
-      <c r="I29" s="77"/>
-      <c r="J29" s="77"/>
-      <c r="K29" s="77"/>
-      <c r="L29" s="77"/>
-      <c r="M29" s="77"/>
-      <c r="N29" s="77"/>
-    </row>
-    <row r="30" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M29" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="N29" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>16</v>
       </c>
@@ -3293,29 +3368,29 @@
       <c r="C30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="12" t="s">
         <v>16</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F30" s="69" t="s">
-        <v>81</v>
-      </c>
-      <c r="G30" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="40" t="s">
+      <c r="H30" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J30" s="40" t="s">
+      <c r="J30" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K30" s="12" t="s">
-        <v>82</v>
+      <c r="K30" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="L30" s="13" t="s">
         <v>35</v>
@@ -3324,10 +3399,10 @@
         <v>76</v>
       </c>
       <c r="N30" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>16</v>
       </c>
@@ -3337,85 +3412,59 @@
       <c r="C31" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="12" t="s">
         <v>16</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G31" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H31" s="40" t="s">
+      <c r="H31" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I31" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J31" s="40" t="s">
+      <c r="J31" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K31" s="12" t="s">
-        <v>83</v>
+      <c r="K31" s="13" t="s">
+        <v>110</v>
       </c>
       <c r="L31" s="13" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="M31" s="56" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="N31" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G32" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J32" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K32" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="L32" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M32" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N32" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="77" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="78"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="78"/>
+      <c r="E32" s="78"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="78"/>
+      <c r="H32" s="78"/>
+      <c r="I32" s="78"/>
+      <c r="J32" s="78"/>
+      <c r="K32" s="78"/>
+      <c r="L32" s="78"/>
+      <c r="M32" s="78"/>
+      <c r="N32" s="78"/>
+    </row>
+    <row r="33" spans="1:14" s="29" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>16</v>
       </c>
@@ -3429,10 +3478,10 @@
         <v>16</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>81</v>
+        <v>51</v>
+      </c>
+      <c r="F33" s="45" t="s">
+        <v>52</v>
       </c>
       <c r="G33" s="40" t="s">
         <v>15</v>
@@ -3446,8 +3495,8 @@
       <c r="J33" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K33" s="12" t="s">
-        <v>85</v>
+      <c r="K33" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="L33" s="13" t="s">
         <v>35</v>
@@ -3459,7 +3508,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" s="29" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>16</v>
       </c>
@@ -3473,10 +3522,10 @@
         <v>16</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>81</v>
+        <v>51</v>
+      </c>
+      <c r="F34" s="45" t="s">
+        <v>52</v>
       </c>
       <c r="G34" s="40" t="s">
         <v>15</v>
@@ -3490,8 +3539,8 @@
       <c r="J34" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K34" s="12" t="s">
-        <v>86</v>
+      <c r="K34" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="L34" s="13" t="s">
         <v>35</v>
@@ -3503,7 +3552,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>16</v>
       </c>
@@ -3517,10 +3566,10 @@
         <v>16</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>81</v>
+        <v>51</v>
+      </c>
+      <c r="F35" s="45" t="s">
+        <v>52</v>
       </c>
       <c r="G35" s="40" t="s">
         <v>15</v>
@@ -3534,8 +3583,8 @@
       <c r="J35" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K35" s="12" t="s">
-        <v>87</v>
+      <c r="K35" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="L35" s="13" t="s">
         <v>35</v>
@@ -3544,52 +3593,26 @@
         <v>76</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="F36" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G36" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H36" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J36" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="L36" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M36" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N36" s="12" t="s">
-        <v>16</v>
-      </c>
+      <c r="B36" s="78"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="78"/>
+      <c r="I36" s="78"/>
+      <c r="J36" s="78"/>
+      <c r="K36" s="78"/>
+      <c r="L36" s="78"/>
+      <c r="M36" s="78"/>
+      <c r="N36" s="78"/>
     </row>
     <row r="37" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
@@ -3607,7 +3630,7 @@
       <c r="E37" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F37" s="12" t="s">
+      <c r="F37" s="69" t="s">
         <v>81</v>
       </c>
       <c r="G37" s="40" t="s">
@@ -3623,7 +3646,7 @@
         <v>17</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="L37" s="13" t="s">
         <v>35</v>
@@ -3667,7 +3690,7 @@
         <v>17</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L38" s="13" t="s">
         <v>35</v>
@@ -3711,7 +3734,7 @@
         <v>17</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="L39" s="13" t="s">
         <v>35</v>
@@ -3755,7 +3778,7 @@
         <v>17</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="L40" s="13" t="s">
         <v>35</v>
@@ -3799,7 +3822,7 @@
         <v>17</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="L41" s="13" t="s">
         <v>35</v>
@@ -3811,117 +3834,313 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="12"/>
-      <c r="M42" s="12"/>
-      <c r="N42" s="12"/>
-    </row>
-    <row r="43" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="12"/>
-      <c r="K43" s="12"/>
-      <c r="L43" s="12"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-    </row>
-    <row r="44" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
-      <c r="K44" s="12"/>
-      <c r="L44" s="12"/>
-      <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
-    </row>
-    <row r="45" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-    </row>
-    <row r="46" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="12"/>
-      <c r="K46" s="12"/>
-      <c r="L46" s="12"/>
-      <c r="M46" s="12"/>
-      <c r="N46" s="12"/>
-    </row>
-    <row r="47" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="12"/>
-      <c r="K47" s="12"/>
-      <c r="L47" s="12"/>
-      <c r="M47" s="12"/>
-      <c r="N47" s="12"/>
-    </row>
-    <row r="48" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="12"/>
-      <c r="K48" s="12"/>
-      <c r="L48" s="12"/>
-      <c r="M48" s="12"/>
-      <c r="N48" s="12"/>
+    <row r="42" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G42" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J42" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="L42" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M42" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="N42" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G43" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J43" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="K43" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="L43" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M43" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="N43" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G44" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J44" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="L44" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M44" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G45" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J45" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="K45" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="L45" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M45" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="N45" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G46" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J46" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="K46" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="L46" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M46" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="N46" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G47" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J47" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="K47" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M47" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="N47" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G48" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J48" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="K48" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="L48" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M48" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="N48" s="12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="49" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="12"/>
@@ -3955,117 +4174,117 @@
       <c r="M50" s="12"/>
       <c r="N50" s="12"/>
     </row>
-    <row r="51" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="13"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="13"/>
-      <c r="K51" s="13"/>
-      <c r="L51" s="13"/>
-      <c r="M51" s="13"/>
-      <c r="N51" s="13"/>
-    </row>
-    <row r="52" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
-      <c r="J52" s="13"/>
-      <c r="K52" s="13"/>
-      <c r="L52" s="13"/>
-      <c r="M52" s="13"/>
-      <c r="N52" s="13"/>
-    </row>
-    <row r="53" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="13"/>
-      <c r="B53" s="13"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="13"/>
-      <c r="L53" s="13"/>
-      <c r="M53" s="13"/>
-      <c r="N53" s="13"/>
-    </row>
-    <row r="54" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="13"/>
-      <c r="B54" s="13"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="46"/>
-      <c r="K54" s="46"/>
-      <c r="L54" s="46"/>
-      <c r="M54" s="46"/>
-      <c r="N54" s="13"/>
-    </row>
-    <row r="55" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="13"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
-      <c r="J55" s="47"/>
-      <c r="K55" s="13"/>
-      <c r="L55" s="47"/>
-      <c r="M55" s="47"/>
-      <c r="N55" s="13"/>
-    </row>
-    <row r="56" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="13"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
-      <c r="K56" s="13"/>
-      <c r="L56" s="47"/>
-      <c r="M56" s="47"/>
-      <c r="N56" s="13"/>
-    </row>
-    <row r="57" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="13"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
-      <c r="K57" s="13"/>
-      <c r="L57" s="47"/>
-      <c r="M57" s="47"/>
-      <c r="N57" s="13"/>
+    <row r="51" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
+      <c r="L51" s="12"/>
+      <c r="M51" s="12"/>
+      <c r="N51" s="12"/>
+    </row>
+    <row r="52" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+      <c r="K52" s="12"/>
+      <c r="L52" s="12"/>
+      <c r="M52" s="12"/>
+      <c r="N52" s="12"/>
+    </row>
+    <row r="53" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="12"/>
+      <c r="K53" s="12"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
+      <c r="N53" s="12"/>
+    </row>
+    <row r="54" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="12"/>
+      <c r="K54" s="12"/>
+      <c r="L54" s="12"/>
+      <c r="M54" s="12"/>
+      <c r="N54" s="12"/>
+    </row>
+    <row r="55" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12"/>
+      <c r="N55" s="12"/>
+    </row>
+    <row r="56" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="12"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="12"/>
+      <c r="L56" s="12"/>
+      <c r="M56" s="12"/>
+      <c r="N56" s="12"/>
+    </row>
+    <row r="57" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="12"/>
+      <c r="L57" s="12"/>
+      <c r="M57" s="12"/>
+      <c r="N57" s="12"/>
     </row>
     <row r="58" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="13"/>
@@ -4125,10 +4344,10 @@
       <c r="G61" s="13"/>
       <c r="H61" s="13"/>
       <c r="I61" s="13"/>
-      <c r="J61" s="13"/>
-      <c r="K61" s="13"/>
-      <c r="L61" s="13"/>
-      <c r="M61" s="13"/>
+      <c r="J61" s="46"/>
+      <c r="K61" s="46"/>
+      <c r="L61" s="46"/>
+      <c r="M61" s="46"/>
       <c r="N61" s="13"/>
     </row>
     <row r="62" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -4141,10 +4360,10 @@
       <c r="G62" s="13"/>
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
+      <c r="J62" s="47"/>
       <c r="K62" s="13"/>
-      <c r="L62" s="13"/>
-      <c r="M62" s="13"/>
+      <c r="L62" s="47"/>
+      <c r="M62" s="47"/>
       <c r="N62" s="13"/>
     </row>
     <row r="63" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -4159,278 +4378,313 @@
       <c r="I63" s="13"/>
       <c r="J63" s="13"/>
       <c r="K63" s="13"/>
-      <c r="L63" s="13"/>
-      <c r="M63" s="13"/>
+      <c r="L63" s="47"/>
+      <c r="M63" s="47"/>
       <c r="N63" s="13"/>
     </row>
-    <row r="64" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="65" spans="3:13" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="66" spans="3:13" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="J66" s="49"/>
-      <c r="K66" s="49"/>
-      <c r="L66" s="49"/>
-      <c r="M66" s="49"/>
-    </row>
-    <row r="67" spans="3:13" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="J67" s="50"/>
-      <c r="L67" s="50"/>
-      <c r="M67" s="50"/>
-    </row>
-    <row r="68" spans="3:13" s="44" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C68" s="48"/>
-      <c r="F68" s="48"/>
-      <c r="J68" s="51"/>
-      <c r="K68" s="48"/>
-      <c r="L68" s="50"/>
-      <c r="M68" s="50"/>
-    </row>
-    <row r="69" spans="3:13" s="44" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C69" s="48"/>
-      <c r="F69" s="48"/>
-      <c r="J69" s="51"/>
-      <c r="K69" s="48"/>
-      <c r="L69" s="50"/>
-      <c r="M69" s="50"/>
-    </row>
-    <row r="70" spans="3:13" s="24" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C70" s="30"/>
-      <c r="F70" s="30"/>
-      <c r="J70" s="32"/>
-      <c r="K70" s="30"/>
-      <c r="L70" s="31"/>
-      <c r="M70" s="31"/>
-    </row>
-    <row r="71" spans="3:13" s="24" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C71" s="30"/>
-      <c r="F71" s="30"/>
-      <c r="J71" s="32"/>
-      <c r="K71" s="30"/>
-      <c r="L71" s="31"/>
-      <c r="M71" s="31"/>
-    </row>
-    <row r="72" spans="3:13" s="33" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C72" s="34"/>
-      <c r="F72" s="34"/>
-      <c r="K72" s="34"/>
-      <c r="M72" s="34"/>
-    </row>
-    <row r="73" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C73" s="35"/>
-      <c r="F73" s="35"/>
-      <c r="K73" s="35"/>
-      <c r="M73" s="35"/>
-    </row>
-    <row r="74" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C74" s="35"/>
-      <c r="F74" s="35"/>
-      <c r="K74" s="35"/>
-      <c r="M74" s="35"/>
-    </row>
-    <row r="75" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C75" s="35"/>
-      <c r="F75" s="35"/>
-      <c r="K75" s="35"/>
-      <c r="M75" s="35"/>
-    </row>
-    <row r="76" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C76" s="35"/>
-      <c r="F76" s="35"/>
-      <c r="J76" s="37"/>
-      <c r="K76" s="37"/>
-      <c r="L76" s="37"/>
-      <c r="M76" s="37"/>
-    </row>
-    <row r="77" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C77" s="35"/>
-      <c r="F77" s="35"/>
-      <c r="J77" s="38"/>
-      <c r="K77" s="35"/>
-      <c r="L77" s="39"/>
-      <c r="M77" s="39"/>
-    </row>
-    <row r="78" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C78" s="35"/>
-      <c r="F78" s="35"/>
-      <c r="J78" s="38"/>
-      <c r="K78" s="35"/>
-      <c r="L78" s="39"/>
-      <c r="M78" s="39"/>
-    </row>
-    <row r="79" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C79" s="35"/>
-      <c r="F79" s="35"/>
-      <c r="J79" s="38"/>
-      <c r="K79" s="35"/>
-      <c r="L79" s="39"/>
-      <c r="M79" s="39"/>
-    </row>
-    <row r="80" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="13"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="13"/>
+      <c r="L64" s="47"/>
+      <c r="M64" s="47"/>
+      <c r="N64" s="13"/>
+    </row>
+    <row r="65" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="13"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="13"/>
+      <c r="L65" s="13"/>
+      <c r="M65" s="13"/>
+      <c r="N65" s="13"/>
+    </row>
+    <row r="66" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="13"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="13"/>
+      <c r="L66" s="13"/>
+      <c r="M66" s="13"/>
+      <c r="N66" s="13"/>
+    </row>
+    <row r="67" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="13"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13"/>
+      <c r="M67" s="13"/>
+      <c r="N67" s="13"/>
+    </row>
+    <row r="68" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A68" s="13"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13"/>
+      <c r="L68" s="13"/>
+      <c r="M68" s="13"/>
+      <c r="N68" s="13"/>
+    </row>
+    <row r="69" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="13"/>
+      <c r="B69" s="13"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="13"/>
+      <c r="M69" s="13"/>
+      <c r="N69" s="13"/>
+    </row>
+    <row r="70" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="13"/>
+      <c r="B70" s="13"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="13"/>
+      <c r="L70" s="13"/>
+      <c r="M70" s="13"/>
+      <c r="N70" s="13"/>
+    </row>
+    <row r="71" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J73" s="49"/>
+      <c r="K73" s="49"/>
+      <c r="L73" s="49"/>
+      <c r="M73" s="49"/>
+    </row>
+    <row r="74" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J74" s="50"/>
+      <c r="L74" s="50"/>
+      <c r="M74" s="50"/>
+    </row>
+    <row r="75" spans="1:14" s="44" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C75" s="48"/>
+      <c r="F75" s="48"/>
+      <c r="J75" s="51"/>
+      <c r="K75" s="48"/>
+      <c r="L75" s="50"/>
+      <c r="M75" s="50"/>
+    </row>
+    <row r="76" spans="1:14" s="44" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C76" s="48"/>
+      <c r="F76" s="48"/>
+      <c r="J76" s="51"/>
+      <c r="K76" s="48"/>
+      <c r="L76" s="50"/>
+      <c r="M76" s="50"/>
+    </row>
+    <row r="77" spans="1:14" s="24" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C77" s="30"/>
+      <c r="F77" s="30"/>
+      <c r="J77" s="32"/>
+      <c r="K77" s="30"/>
+      <c r="L77" s="31"/>
+      <c r="M77" s="31"/>
+    </row>
+    <row r="78" spans="1:14" s="24" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C78" s="30"/>
+      <c r="F78" s="30"/>
+      <c r="J78" s="32"/>
+      <c r="K78" s="30"/>
+      <c r="L78" s="31"/>
+      <c r="M78" s="31"/>
+    </row>
+    <row r="79" spans="1:14" s="33" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C79" s="34"/>
+      <c r="F79" s="34"/>
+      <c r="K79" s="34"/>
+      <c r="M79" s="34"/>
+    </row>
+    <row r="80" spans="1:14" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C80" s="35"/>
       <c r="F80" s="35"/>
-      <c r="J80" s="38"/>
-      <c r="K80" s="38"/>
-      <c r="L80" s="38"/>
-      <c r="M80" s="38"/>
-    </row>
-    <row r="81" spans="1:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K80" s="35"/>
+      <c r="M80" s="35"/>
+    </row>
+    <row r="81" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C81" s="35"/>
       <c r="F81" s="35"/>
-      <c r="J81" s="38"/>
-      <c r="K81" s="38"/>
-      <c r="L81" s="38"/>
-      <c r="M81" s="38"/>
-    </row>
-    <row r="82" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C82" s="18"/>
-      <c r="F82" s="18"/>
-      <c r="K82" s="18"/>
-      <c r="M82" s="18"/>
-    </row>
-    <row r="83" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C83" s="18"/>
-      <c r="F83" s="18"/>
-      <c r="K83" s="18"/>
-      <c r="M83" s="18"/>
-    </row>
-    <row r="84" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C84" s="18"/>
-      <c r="F84" s="18"/>
-      <c r="K84" s="18"/>
-      <c r="M84" s="18"/>
-    </row>
-    <row r="85" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C85" s="18"/>
-      <c r="F85" s="18"/>
-      <c r="K85" s="18"/>
-      <c r="M85" s="18"/>
-    </row>
-    <row r="86" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C86" s="18"/>
-      <c r="F86" s="18"/>
-      <c r="J86" s="15"/>
-      <c r="K86" s="15"/>
-      <c r="L86" s="15"/>
-      <c r="M86" s="15"/>
-    </row>
-    <row r="87" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C87" s="18"/>
-      <c r="F87" s="18"/>
-      <c r="J87" s="17"/>
-      <c r="K87" s="18"/>
-      <c r="L87" s="16"/>
-      <c r="M87" s="16"/>
-    </row>
-    <row r="88" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C88" s="18"/>
-      <c r="F88" s="18"/>
-      <c r="J88" s="17"/>
-      <c r="K88" s="18"/>
-      <c r="L88" s="16"/>
-      <c r="M88" s="16"/>
-    </row>
-    <row r="89" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K81" s="35"/>
+      <c r="M81" s="35"/>
+    </row>
+    <row r="82" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C82" s="35"/>
+      <c r="F82" s="35"/>
+      <c r="K82" s="35"/>
+      <c r="M82" s="35"/>
+    </row>
+    <row r="83" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C83" s="35"/>
+      <c r="F83" s="35"/>
+      <c r="J83" s="37"/>
+      <c r="K83" s="37"/>
+      <c r="L83" s="37"/>
+      <c r="M83" s="37"/>
+    </row>
+    <row r="84" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C84" s="35"/>
+      <c r="F84" s="35"/>
+      <c r="J84" s="38"/>
+      <c r="K84" s="35"/>
+      <c r="L84" s="39"/>
+      <c r="M84" s="39"/>
+    </row>
+    <row r="85" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C85" s="35"/>
+      <c r="F85" s="35"/>
+      <c r="J85" s="38"/>
+      <c r="K85" s="35"/>
+      <c r="L85" s="39"/>
+      <c r="M85" s="39"/>
+    </row>
+    <row r="86" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C86" s="35"/>
+      <c r="F86" s="35"/>
+      <c r="J86" s="38"/>
+      <c r="K86" s="35"/>
+      <c r="L86" s="39"/>
+      <c r="M86" s="39"/>
+    </row>
+    <row r="87" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C87" s="35"/>
+      <c r="F87" s="35"/>
+      <c r="J87" s="38"/>
+      <c r="K87" s="38"/>
+      <c r="L87" s="38"/>
+      <c r="M87" s="38"/>
+    </row>
+    <row r="88" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C88" s="35"/>
+      <c r="F88" s="35"/>
+      <c r="J88" s="38"/>
+      <c r="K88" s="38"/>
+      <c r="L88" s="38"/>
+      <c r="M88" s="38"/>
+    </row>
+    <row r="89" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C89" s="18"/>
       <c r="F89" s="18"/>
-      <c r="J89" s="17"/>
       <c r="K89" s="18"/>
-      <c r="L89" s="16"/>
-      <c r="M89" s="16"/>
-    </row>
-    <row r="90" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M89" s="18"/>
+    </row>
+    <row r="90" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C90" s="18"/>
       <c r="F90" s="18"/>
-      <c r="J90" s="17"/>
-      <c r="K90" s="17"/>
-      <c r="L90" s="17"/>
-      <c r="M90" s="17"/>
-    </row>
-    <row r="91" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K90" s="18"/>
+      <c r="M90" s="18"/>
+    </row>
+    <row r="91" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C91" s="18"/>
       <c r="F91" s="18"/>
-      <c r="J91" s="17"/>
-      <c r="K91" s="17"/>
-      <c r="L91" s="17"/>
-      <c r="M91" s="17"/>
-    </row>
-    <row r="92" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="20"/>
+      <c r="K91" s="18"/>
+      <c r="M91" s="18"/>
+    </row>
+    <row r="92" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C92" s="18"/>
-      <c r="D92" s="18"/>
-      <c r="E92" s="18"/>
       <c r="F92" s="18"/>
-      <c r="G92" s="18"/>
-      <c r="H92" s="18"/>
-      <c r="I92" s="18"/>
       <c r="K92" s="18"/>
       <c r="M92" s="18"/>
     </row>
-    <row r="93" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C93" s="18"/>
-      <c r="D93" s="18"/>
-      <c r="E93" s="18"/>
       <c r="F93" s="18"/>
-      <c r="G93" s="18"/>
-      <c r="H93" s="18"/>
-      <c r="I93" s="18"/>
-      <c r="K93" s="18"/>
-      <c r="M93" s="18"/>
-    </row>
-    <row r="94" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J93" s="15"/>
+      <c r="K93" s="15"/>
+      <c r="L93" s="15"/>
+      <c r="M93" s="15"/>
+    </row>
+    <row r="94" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C94" s="18"/>
-      <c r="D94" s="18"/>
-      <c r="E94" s="18"/>
       <c r="F94" s="18"/>
-      <c r="G94" s="18"/>
-      <c r="H94" s="18"/>
-      <c r="I94" s="18"/>
+      <c r="J94" s="17"/>
       <c r="K94" s="18"/>
-      <c r="M94" s="18"/>
-    </row>
-    <row r="95" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L94" s="16"/>
+      <c r="M94" s="16"/>
+    </row>
+    <row r="95" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C95" s="18"/>
-      <c r="D95" s="18"/>
-      <c r="E95" s="18"/>
       <c r="F95" s="18"/>
-      <c r="G95" s="18"/>
-      <c r="H95" s="18"/>
-      <c r="I95" s="18"/>
+      <c r="J95" s="17"/>
       <c r="K95" s="18"/>
-      <c r="M95" s="18"/>
-    </row>
-    <row r="96" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L95" s="16"/>
+      <c r="M95" s="16"/>
+    </row>
+    <row r="96" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C96" s="18"/>
-      <c r="D96" s="18"/>
-      <c r="E96" s="18"/>
       <c r="F96" s="18"/>
-      <c r="G96" s="18"/>
-      <c r="H96" s="18"/>
-      <c r="I96" s="18"/>
+      <c r="J96" s="17"/>
       <c r="K96" s="18"/>
-      <c r="M96" s="18"/>
-    </row>
-    <row r="97" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L96" s="16"/>
+      <c r="M96" s="16"/>
+    </row>
+    <row r="97" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C97" s="18"/>
-      <c r="D97" s="18"/>
-      <c r="E97" s="18"/>
       <c r="F97" s="18"/>
-      <c r="G97" s="18"/>
-      <c r="H97" s="18"/>
-      <c r="I97" s="18"/>
-      <c r="K97" s="18"/>
-      <c r="M97" s="18"/>
-    </row>
-    <row r="98" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J97" s="17"/>
+      <c r="K97" s="17"/>
+      <c r="L97" s="17"/>
+      <c r="M97" s="17"/>
+    </row>
+    <row r="98" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C98" s="18"/>
-      <c r="D98" s="18"/>
-      <c r="E98" s="18"/>
       <c r="F98" s="18"/>
-      <c r="G98" s="18"/>
-      <c r="H98" s="18"/>
-      <c r="I98" s="18"/>
-      <c r="K98" s="18"/>
-      <c r="M98" s="18"/>
-    </row>
-    <row r="99" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J98" s="17"/>
+      <c r="K98" s="17"/>
+      <c r="L98" s="17"/>
+      <c r="M98" s="17"/>
+    </row>
+    <row r="99" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="20"/>
       <c r="C99" s="18"/>
       <c r="D99" s="18"/>
       <c r="E99" s="18"/>
@@ -4441,20 +4695,98 @@
       <c r="K99" s="18"/>
       <c r="M99" s="18"/>
     </row>
+    <row r="100" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C100" s="18"/>
+      <c r="D100" s="18"/>
+      <c r="E100" s="18"/>
+      <c r="F100" s="18"/>
+      <c r="G100" s="18"/>
+      <c r="H100" s="18"/>
+      <c r="I100" s="18"/>
+      <c r="K100" s="18"/>
+      <c r="M100" s="18"/>
+    </row>
+    <row r="101" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C101" s="18"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="18"/>
+      <c r="F101" s="18"/>
+      <c r="G101" s="18"/>
+      <c r="H101" s="18"/>
+      <c r="I101" s="18"/>
+      <c r="K101" s="18"/>
+      <c r="M101" s="18"/>
+    </row>
+    <row r="102" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="18"/>
+      <c r="G102" s="18"/>
+      <c r="H102" s="18"/>
+      <c r="I102" s="18"/>
+      <c r="K102" s="18"/>
+      <c r="M102" s="18"/>
+    </row>
+    <row r="103" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C103" s="18"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="18"/>
+      <c r="G103" s="18"/>
+      <c r="H103" s="18"/>
+      <c r="I103" s="18"/>
+      <c r="K103" s="18"/>
+      <c r="M103" s="18"/>
+    </row>
+    <row r="104" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C104" s="18"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="18"/>
+      <c r="F104" s="18"/>
+      <c r="G104" s="18"/>
+      <c r="H104" s="18"/>
+      <c r="I104" s="18"/>
+      <c r="K104" s="18"/>
+      <c r="M104" s="18"/>
+    </row>
+    <row r="105" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="18"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
+      <c r="H105" s="18"/>
+      <c r="I105" s="18"/>
+      <c r="K105" s="18"/>
+      <c r="M105" s="18"/>
+    </row>
+    <row r="106" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="18"/>
+      <c r="G106" s="18"/>
+      <c r="H106" s="18"/>
+      <c r="I106" s="18"/>
+      <c r="K106" s="18"/>
+      <c r="M106" s="18"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A29:XFD29"/>
-    <mergeCell ref="A5:XFD5"/>
-    <mergeCell ref="A13:XFD13"/>
-    <mergeCell ref="A15:XFD15"/>
-    <mergeCell ref="A20:XFD20"/>
-    <mergeCell ref="A26:XFD26"/>
+    <mergeCell ref="A32:XFD32"/>
+    <mergeCell ref="A36:XFD36"/>
+    <mergeCell ref="A6:XFD6"/>
+    <mergeCell ref="A16:XFD16"/>
+    <mergeCell ref="A19:XFD19"/>
+    <mergeCell ref="A25:XFD25"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F27" r:id="rId1" location="/79590444732ud/detail/userstory/134825813356" display="https://rally1.rallydev.com/ - /79590444732ud/detail/userstory/134825813356"/>
-    <hyperlink ref="F28" r:id="rId2" location="/79590444732ud/detail/userstory/134825813356" display="https://rally1.rallydev.com/ - /79590444732ud/detail/userstory/134825813356"/>
+    <hyperlink ref="F33" r:id="rId1" location="/79590444732ud/detail/userstory/134825813356" display="https://rally1.rallydev.com/ - /79590444732ud/detail/userstory/134825813356"/>
+    <hyperlink ref="F35" r:id="rId2" location="/79590444732ud/detail/userstory/134825813356" display="https://rally1.rallydev.com/ - /79590444732ud/detail/userstory/134825813356"/>
+    <hyperlink ref="F34" r:id="rId3" location="/79590444732ud/detail/userstory/134825813356" display="https://rally1.rallydev.com/ - /79590444732ud/detail/userstory/134825813356"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
549587 Updated per feedback from the release office
</commit_message>
<xml_diff>
--- a/Requirement/Build 4/TAS eBilling RTM IB_ 2.0_592.xlsx
+++ b/Requirement/Build 4/TAS eBilling RTM IB_ 2.0_592.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="105">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -383,31 +383,10 @@
     <t>NA</t>
   </si>
   <si>
-    <t>TC1237 - CIT eBilling  TS Validate the existing claims Still Display on the TPJI screen when there is an active Outpatient Dental Claim (O/D)  Regression US14</t>
-  </si>
-  <si>
     <t xml:space="preserve">US 1108/US131 - Enter/Edit Dental Claims    </t>
   </si>
   <si>
-    <t>TC1227 -CIT eBilling  TS eBilling create a CMS 1500 Outpatient Professional Claim - Regression US1108 &amp; US131</t>
-  </si>
-  <si>
-    <t>TC1228 -CIT  eBilling  TS Create a UB04 (Inst) Claim - Regression US1108 &amp; US131</t>
-  </si>
-  <si>
-    <t>TC1229 - CIT  eBilling Create an Institutional Claim via Autobiller - Regression US1109</t>
-  </si>
-  <si>
     <t xml:space="preserve">US2487 - Insurance Company Entry/Edit - Dental      </t>
-  </si>
-  <si>
-    <t>TC2232 -CIT eBilling US2487 - Insurance Company Entry/Edit - Dental - Regression Not applicable</t>
-  </si>
-  <si>
-    <t>TC2231 -CIT eBilling US2488 - Update Reports - Form Type J430D - Regression Not applicable</t>
-  </si>
-  <si>
-    <t>TC2230 - CIT eBilling TS18 MRW - Print MRA US2489 - Regression</t>
   </si>
 </sst>
 </file>
@@ -1227,7 +1206,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1866,9 +1845,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DQ106"/>
+  <dimension ref="A1:DQ99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2147,175 +2128,174 @@
       </c>
       <c r="O4" s="13"/>
     </row>
-    <row r="5" spans="1:121" s="42" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="70" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="40" t="s">
+    <row r="5" spans="1:121" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="77" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="78"/>
+      <c r="S5" s="78"/>
+      <c r="T5" s="78"/>
+      <c r="U5" s="78"/>
+      <c r="V5" s="78"/>
+      <c r="W5" s="78"/>
+      <c r="X5" s="78"/>
+      <c r="Y5" s="78"/>
+      <c r="Z5" s="78"/>
+      <c r="AA5" s="78"/>
+      <c r="AB5" s="78"/>
+      <c r="AC5" s="78"/>
+      <c r="AD5" s="78"/>
+      <c r="AE5" s="78"/>
+      <c r="AF5" s="78"/>
+      <c r="AG5" s="78"/>
+      <c r="AH5" s="78"/>
+      <c r="AI5" s="78"/>
+      <c r="AJ5" s="78"/>
+      <c r="AK5" s="78"/>
+      <c r="AL5" s="78"/>
+      <c r="AM5" s="78"/>
+      <c r="AN5" s="78"/>
+      <c r="AO5" s="78"/>
+      <c r="AP5" s="78"/>
+      <c r="AQ5" s="78"/>
+      <c r="AR5" s="78"/>
+      <c r="AS5" s="78"/>
+      <c r="AT5" s="78"/>
+      <c r="AU5" s="78"/>
+      <c r="AV5" s="78"/>
+      <c r="AW5" s="78"/>
+      <c r="AX5" s="78"/>
+      <c r="AY5" s="78"/>
+      <c r="AZ5" s="78"/>
+      <c r="BA5" s="78"/>
+      <c r="BB5" s="78"/>
+      <c r="BC5" s="78"/>
+      <c r="BD5" s="78"/>
+      <c r="BE5" s="78"/>
+      <c r="BF5" s="78"/>
+      <c r="BG5" s="78"/>
+      <c r="BH5" s="78"/>
+      <c r="BI5" s="78"/>
+      <c r="BJ5" s="78"/>
+      <c r="BK5" s="78"/>
+      <c r="BL5" s="78"/>
+      <c r="BM5" s="78"/>
+      <c r="BN5" s="78"/>
+      <c r="BO5" s="78"/>
+      <c r="BP5" s="78"/>
+      <c r="BQ5" s="78"/>
+      <c r="BR5" s="78"/>
+      <c r="BS5" s="78"/>
+      <c r="BT5" s="78"/>
+      <c r="BU5" s="78"/>
+      <c r="BV5" s="78"/>
+      <c r="BW5" s="78"/>
+      <c r="BX5" s="78"/>
+      <c r="BY5" s="78"/>
+      <c r="BZ5" s="78"/>
+      <c r="CA5" s="78"/>
+      <c r="CB5" s="78"/>
+      <c r="CC5" s="78"/>
+      <c r="CD5" s="78"/>
+      <c r="CE5" s="78"/>
+      <c r="CF5" s="78"/>
+      <c r="CG5" s="78"/>
+      <c r="CH5" s="78"/>
+      <c r="CI5" s="78"/>
+      <c r="CJ5" s="78"/>
+      <c r="CK5" s="78"/>
+      <c r="CL5" s="78"/>
+      <c r="CM5" s="78"/>
+      <c r="CN5" s="78"/>
+      <c r="CO5" s="78"/>
+      <c r="CP5" s="78"/>
+      <c r="CQ5" s="78"/>
+      <c r="CR5" s="78"/>
+      <c r="CS5" s="78"/>
+      <c r="CT5" s="78"/>
+      <c r="CU5" s="78"/>
+      <c r="CV5" s="78"/>
+      <c r="CW5" s="78"/>
+      <c r="CX5" s="78"/>
+      <c r="CY5" s="78"/>
+      <c r="CZ5" s="78"/>
+      <c r="DA5" s="78"/>
+      <c r="DB5" s="78"/>
+      <c r="DC5" s="78"/>
+      <c r="DD5" s="78"/>
+      <c r="DE5" s="78"/>
+      <c r="DF5" s="78"/>
+      <c r="DG5" s="78"/>
+      <c r="DH5" s="78"/>
+      <c r="DI5" s="78"/>
+      <c r="DJ5" s="78"/>
+      <c r="DK5" s="78"/>
+      <c r="DL5" s="78"/>
+      <c r="DM5" s="78"/>
+      <c r="DN5" s="78"/>
+      <c r="DO5" s="78"/>
+      <c r="DP5" s="78"/>
+      <c r="DQ5" s="78"/>
+    </row>
+    <row r="6" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="13" t="s">
+      <c r="H6" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J5" s="40" t="s">
+      <c r="J6" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L5" s="13" t="s">
+      <c r="K6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="56" t="s">
+      <c r="M6" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="N5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="O5" s="13"/>
-    </row>
-    <row r="6" spans="1:121" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="77" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="78"/>
-      <c r="P6" s="78"/>
-      <c r="Q6" s="78"/>
-      <c r="R6" s="78"/>
-      <c r="S6" s="78"/>
-      <c r="T6" s="78"/>
-      <c r="U6" s="78"/>
-      <c r="V6" s="78"/>
-      <c r="W6" s="78"/>
-      <c r="X6" s="78"/>
-      <c r="Y6" s="78"/>
-      <c r="Z6" s="78"/>
-      <c r="AA6" s="78"/>
-      <c r="AB6" s="78"/>
-      <c r="AC6" s="78"/>
-      <c r="AD6" s="78"/>
-      <c r="AE6" s="78"/>
-      <c r="AF6" s="78"/>
-      <c r="AG6" s="78"/>
-      <c r="AH6" s="78"/>
-      <c r="AI6" s="78"/>
-      <c r="AJ6" s="78"/>
-      <c r="AK6" s="78"/>
-      <c r="AL6" s="78"/>
-      <c r="AM6" s="78"/>
-      <c r="AN6" s="78"/>
-      <c r="AO6" s="78"/>
-      <c r="AP6" s="78"/>
-      <c r="AQ6" s="78"/>
-      <c r="AR6" s="78"/>
-      <c r="AS6" s="78"/>
-      <c r="AT6" s="78"/>
-      <c r="AU6" s="78"/>
-      <c r="AV6" s="78"/>
-      <c r="AW6" s="78"/>
-      <c r="AX6" s="78"/>
-      <c r="AY6" s="78"/>
-      <c r="AZ6" s="78"/>
-      <c r="BA6" s="78"/>
-      <c r="BB6" s="78"/>
-      <c r="BC6" s="78"/>
-      <c r="BD6" s="78"/>
-      <c r="BE6" s="78"/>
-      <c r="BF6" s="78"/>
-      <c r="BG6" s="78"/>
-      <c r="BH6" s="78"/>
-      <c r="BI6" s="78"/>
-      <c r="BJ6" s="78"/>
-      <c r="BK6" s="78"/>
-      <c r="BL6" s="78"/>
-      <c r="BM6" s="78"/>
-      <c r="BN6" s="78"/>
-      <c r="BO6" s="78"/>
-      <c r="BP6" s="78"/>
-      <c r="BQ6" s="78"/>
-      <c r="BR6" s="78"/>
-      <c r="BS6" s="78"/>
-      <c r="BT6" s="78"/>
-      <c r="BU6" s="78"/>
-      <c r="BV6" s="78"/>
-      <c r="BW6" s="78"/>
-      <c r="BX6" s="78"/>
-      <c r="BY6" s="78"/>
-      <c r="BZ6" s="78"/>
-      <c r="CA6" s="78"/>
-      <c r="CB6" s="78"/>
-      <c r="CC6" s="78"/>
-      <c r="CD6" s="78"/>
-      <c r="CE6" s="78"/>
-      <c r="CF6" s="78"/>
-      <c r="CG6" s="78"/>
-      <c r="CH6" s="78"/>
-      <c r="CI6" s="78"/>
-      <c r="CJ6" s="78"/>
-      <c r="CK6" s="78"/>
-      <c r="CL6" s="78"/>
-      <c r="CM6" s="78"/>
-      <c r="CN6" s="78"/>
-      <c r="CO6" s="78"/>
-      <c r="CP6" s="78"/>
-      <c r="CQ6" s="78"/>
-      <c r="CR6" s="78"/>
-      <c r="CS6" s="78"/>
-      <c r="CT6" s="78"/>
-      <c r="CU6" s="78"/>
-      <c r="CV6" s="78"/>
-      <c r="CW6" s="78"/>
-      <c r="CX6" s="78"/>
-      <c r="CY6" s="78"/>
-      <c r="CZ6" s="78"/>
-      <c r="DA6" s="78"/>
-      <c r="DB6" s="78"/>
-      <c r="DC6" s="78"/>
-      <c r="DD6" s="78"/>
-      <c r="DE6" s="78"/>
-      <c r="DF6" s="78"/>
-      <c r="DG6" s="78"/>
-      <c r="DH6" s="78"/>
-      <c r="DI6" s="78"/>
-      <c r="DJ6" s="78"/>
-      <c r="DK6" s="78"/>
-      <c r="DL6" s="78"/>
-      <c r="DM6" s="78"/>
-      <c r="DN6" s="78"/>
-      <c r="DO6" s="78"/>
-      <c r="DP6" s="78"/>
-      <c r="DQ6" s="78"/>
+      <c r="N6" s="12" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="7" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
@@ -2331,7 +2311,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>21</v>
@@ -2349,7 +2329,7 @@
         <v>17</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>105</v>
+        <v>39</v>
       </c>
       <c r="L7" s="13" t="s">
         <v>35</v>
@@ -2358,7 +2338,7 @@
         <v>76</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
@@ -2375,7 +2355,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>21</v>
@@ -2393,7 +2373,7 @@
         <v>17</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>106</v>
+        <v>40</v>
       </c>
       <c r="L8" s="13" t="s">
         <v>35</v>
@@ -2402,7 +2382,7 @@
         <v>76</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
@@ -2419,7 +2399,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>21</v>
@@ -2437,7 +2417,7 @@
         <v>17</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="L9" s="13" t="s">
         <v>35</v>
@@ -2446,7 +2426,7 @@
         <v>76</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
@@ -2463,7 +2443,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>21</v>
@@ -2481,7 +2461,7 @@
         <v>17</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L10" s="13" t="s">
         <v>35</v>
@@ -2490,24 +2470,24 @@
         <v>76</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D11" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>21</v>
@@ -2525,7 +2505,7 @@
         <v>17</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L11" s="13" t="s">
         <v>35</v>
@@ -2534,7 +2514,7 @@
         <v>76</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
@@ -2551,7 +2531,7 @@
         <v>16</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>21</v>
@@ -2569,7 +2549,7 @@
         <v>17</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="L12" s="13" t="s">
         <v>35</v>
@@ -2578,56 +2558,137 @@
         <v>76</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M13" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N13" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:121" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="78"/>
+      <c r="M13" s="78"/>
+      <c r="N13" s="78"/>
+      <c r="O13" s="78"/>
+      <c r="P13" s="78"/>
+      <c r="Q13" s="78"/>
+      <c r="R13" s="78"/>
+      <c r="S13" s="78"/>
+      <c r="T13" s="78"/>
+      <c r="U13" s="78"/>
+      <c r="V13" s="78"/>
+      <c r="W13" s="78"/>
+      <c r="X13" s="78"/>
+      <c r="Y13" s="78"/>
+      <c r="Z13" s="78"/>
+      <c r="AA13" s="78"/>
+      <c r="AB13" s="78"/>
+      <c r="AC13" s="78"/>
+      <c r="AD13" s="78"/>
+      <c r="AE13" s="78"/>
+      <c r="AF13" s="78"/>
+      <c r="AG13" s="78"/>
+      <c r="AH13" s="78"/>
+      <c r="AI13" s="78"/>
+      <c r="AJ13" s="78"/>
+      <c r="AK13" s="78"/>
+      <c r="AL13" s="78"/>
+      <c r="AM13" s="78"/>
+      <c r="AN13" s="78"/>
+      <c r="AO13" s="78"/>
+      <c r="AP13" s="78"/>
+      <c r="AQ13" s="78"/>
+      <c r="AR13" s="78"/>
+      <c r="AS13" s="78"/>
+      <c r="AT13" s="78"/>
+      <c r="AU13" s="78"/>
+      <c r="AV13" s="78"/>
+      <c r="AW13" s="78"/>
+      <c r="AX13" s="78"/>
+      <c r="AY13" s="78"/>
+      <c r="AZ13" s="78"/>
+      <c r="BA13" s="78"/>
+      <c r="BB13" s="78"/>
+      <c r="BC13" s="78"/>
+      <c r="BD13" s="78"/>
+      <c r="BE13" s="78"/>
+      <c r="BF13" s="78"/>
+      <c r="BG13" s="78"/>
+      <c r="BH13" s="78"/>
+      <c r="BI13" s="78"/>
+      <c r="BJ13" s="78"/>
+      <c r="BK13" s="78"/>
+      <c r="BL13" s="78"/>
+      <c r="BM13" s="78"/>
+      <c r="BN13" s="78"/>
+      <c r="BO13" s="78"/>
+      <c r="BP13" s="78"/>
+      <c r="BQ13" s="78"/>
+      <c r="BR13" s="78"/>
+      <c r="BS13" s="78"/>
+      <c r="BT13" s="78"/>
+      <c r="BU13" s="78"/>
+      <c r="BV13" s="78"/>
+      <c r="BW13" s="78"/>
+      <c r="BX13" s="78"/>
+      <c r="BY13" s="78"/>
+      <c r="BZ13" s="78"/>
+      <c r="CA13" s="78"/>
+      <c r="CB13" s="78"/>
+      <c r="CC13" s="78"/>
+      <c r="CD13" s="78"/>
+      <c r="CE13" s="78"/>
+      <c r="CF13" s="78"/>
+      <c r="CG13" s="78"/>
+      <c r="CH13" s="78"/>
+      <c r="CI13" s="78"/>
+      <c r="CJ13" s="78"/>
+      <c r="CK13" s="78"/>
+      <c r="CL13" s="78"/>
+      <c r="CM13" s="78"/>
+      <c r="CN13" s="78"/>
+      <c r="CO13" s="78"/>
+      <c r="CP13" s="78"/>
+      <c r="CQ13" s="78"/>
+      <c r="CR13" s="78"/>
+      <c r="CS13" s="78"/>
+      <c r="CT13" s="78"/>
+      <c r="CU13" s="78"/>
+      <c r="CV13" s="78"/>
+      <c r="CW13" s="78"/>
+      <c r="CX13" s="78"/>
+      <c r="CY13" s="78"/>
+      <c r="CZ13" s="78"/>
+      <c r="DA13" s="78"/>
+      <c r="DB13" s="78"/>
+      <c r="DC13" s="78"/>
+      <c r="DD13" s="78"/>
+      <c r="DE13" s="78"/>
+      <c r="DF13" s="78"/>
+      <c r="DG13" s="78"/>
+      <c r="DH13" s="78"/>
+      <c r="DI13" s="78"/>
+      <c r="DJ13" s="78"/>
+      <c r="DK13" s="78"/>
+      <c r="DL13" s="78"/>
+      <c r="DM13" s="78"/>
+      <c r="DN13" s="78"/>
+      <c r="DO13" s="78"/>
+      <c r="DP13" s="78"/>
+      <c r="DQ13" s="78"/>
+    </row>
+    <row r="14" spans="1:121" s="43" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>31</v>
@@ -2639,10 +2700,10 @@
         <v>16</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G14" s="40" t="s">
         <v>15</v>
@@ -2653,11 +2714,11 @@
       <c r="I14" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J14" s="41" t="s">
+      <c r="J14" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L14" s="13" t="s">
         <v>35</v>
@@ -2666,179 +2727,72 @@
         <v>76</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:121" s="79" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="79" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="80"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="80"/>
+      <c r="K15" s="80"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="80"/>
+      <c r="N15" s="80"/>
+    </row>
+    <row r="16" spans="1:121" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="40" t="s">
+      <c r="C16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="13" t="s">
+      <c r="H16" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="41" t="s">
+      <c r="J16" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="L15" s="13" t="s">
+      <c r="K16" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M15" s="56" t="s">
+      <c r="M16" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="N15" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:121" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="77" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="78"/>
-      <c r="M16" s="78"/>
-      <c r="N16" s="78"/>
-      <c r="O16" s="78"/>
-      <c r="P16" s="78"/>
-      <c r="Q16" s="78"/>
-      <c r="R16" s="78"/>
-      <c r="S16" s="78"/>
-      <c r="T16" s="78"/>
-      <c r="U16" s="78"/>
-      <c r="V16" s="78"/>
-      <c r="W16" s="78"/>
-      <c r="X16" s="78"/>
-      <c r="Y16" s="78"/>
-      <c r="Z16" s="78"/>
-      <c r="AA16" s="78"/>
-      <c r="AB16" s="78"/>
-      <c r="AC16" s="78"/>
-      <c r="AD16" s="78"/>
-      <c r="AE16" s="78"/>
-      <c r="AF16" s="78"/>
-      <c r="AG16" s="78"/>
-      <c r="AH16" s="78"/>
-      <c r="AI16" s="78"/>
-      <c r="AJ16" s="78"/>
-      <c r="AK16" s="78"/>
-      <c r="AL16" s="78"/>
-      <c r="AM16" s="78"/>
-      <c r="AN16" s="78"/>
-      <c r="AO16" s="78"/>
-      <c r="AP16" s="78"/>
-      <c r="AQ16" s="78"/>
-      <c r="AR16" s="78"/>
-      <c r="AS16" s="78"/>
-      <c r="AT16" s="78"/>
-      <c r="AU16" s="78"/>
-      <c r="AV16" s="78"/>
-      <c r="AW16" s="78"/>
-      <c r="AX16" s="78"/>
-      <c r="AY16" s="78"/>
-      <c r="AZ16" s="78"/>
-      <c r="BA16" s="78"/>
-      <c r="BB16" s="78"/>
-      <c r="BC16" s="78"/>
-      <c r="BD16" s="78"/>
-      <c r="BE16" s="78"/>
-      <c r="BF16" s="78"/>
-      <c r="BG16" s="78"/>
-      <c r="BH16" s="78"/>
-      <c r="BI16" s="78"/>
-      <c r="BJ16" s="78"/>
-      <c r="BK16" s="78"/>
-      <c r="BL16" s="78"/>
-      <c r="BM16" s="78"/>
-      <c r="BN16" s="78"/>
-      <c r="BO16" s="78"/>
-      <c r="BP16" s="78"/>
-      <c r="BQ16" s="78"/>
-      <c r="BR16" s="78"/>
-      <c r="BS16" s="78"/>
-      <c r="BT16" s="78"/>
-      <c r="BU16" s="78"/>
-      <c r="BV16" s="78"/>
-      <c r="BW16" s="78"/>
-      <c r="BX16" s="78"/>
-      <c r="BY16" s="78"/>
-      <c r="BZ16" s="78"/>
-      <c r="CA16" s="78"/>
-      <c r="CB16" s="78"/>
-      <c r="CC16" s="78"/>
-      <c r="CD16" s="78"/>
-      <c r="CE16" s="78"/>
-      <c r="CF16" s="78"/>
-      <c r="CG16" s="78"/>
-      <c r="CH16" s="78"/>
-      <c r="CI16" s="78"/>
-      <c r="CJ16" s="78"/>
-      <c r="CK16" s="78"/>
-      <c r="CL16" s="78"/>
-      <c r="CM16" s="78"/>
-      <c r="CN16" s="78"/>
-      <c r="CO16" s="78"/>
-      <c r="CP16" s="78"/>
-      <c r="CQ16" s="78"/>
-      <c r="CR16" s="78"/>
-      <c r="CS16" s="78"/>
-      <c r="CT16" s="78"/>
-      <c r="CU16" s="78"/>
-      <c r="CV16" s="78"/>
-      <c r="CW16" s="78"/>
-      <c r="CX16" s="78"/>
-      <c r="CY16" s="78"/>
-      <c r="CZ16" s="78"/>
-      <c r="DA16" s="78"/>
-      <c r="DB16" s="78"/>
-      <c r="DC16" s="78"/>
-      <c r="DD16" s="78"/>
-      <c r="DE16" s="78"/>
-      <c r="DF16" s="78"/>
-      <c r="DG16" s="78"/>
-      <c r="DH16" s="78"/>
-      <c r="DI16" s="78"/>
-      <c r="DJ16" s="78"/>
-      <c r="DK16" s="78"/>
-      <c r="DL16" s="78"/>
-      <c r="DM16" s="78"/>
-      <c r="DN16" s="78"/>
-      <c r="DO16" s="78"/>
-      <c r="DP16" s="78"/>
-      <c r="DQ16" s="78"/>
-    </row>
-    <row r="17" spans="1:14" s="43" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="N16" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>16</v>
       </c>
@@ -2852,10 +2806,10 @@
         <v>16</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G17" s="40" t="s">
         <v>15</v>
@@ -2870,7 +2824,7 @@
         <v>17</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="L17" s="13" t="s">
         <v>35</v>
@@ -2879,10 +2833,10 @@
         <v>76</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" s="52" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>16</v>
       </c>
@@ -2896,10 +2850,10 @@
         <v>16</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G18" s="40" t="s">
         <v>15</v>
@@ -2913,8 +2867,8 @@
       <c r="J18" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="52" t="s">
-        <v>107</v>
+      <c r="K18" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="L18" s="13" t="s">
         <v>35</v>
@@ -2923,72 +2877,72 @@
         <v>76</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" s="79" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="79" t="s">
-        <v>108</v>
-      </c>
-      <c r="B19" s="80"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="80"/>
-      <c r="I19" s="80"/>
-      <c r="J19" s="80"/>
-      <c r="K19" s="80"/>
-      <c r="L19" s="80"/>
-      <c r="M19" s="80"/>
-      <c r="N19" s="80"/>
-    </row>
-    <row r="20" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C19" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="12" t="s">
+      <c r="D19" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="40" t="s">
+      <c r="G19" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="13" t="s">
+      <c r="H19" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J20" s="40" t="s">
+      <c r="J19" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K20" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="L20" s="13" t="s">
+      <c r="K19" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M20" s="56" t="s">
+      <c r="M19" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="N20" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="N19" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="77" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="78"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="78"/>
+      <c r="L20" s="78"/>
+      <c r="M20" s="78"/>
+      <c r="N20" s="78"/>
+    </row>
+    <row r="21" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>16</v>
       </c>
@@ -2998,29 +2952,29 @@
       <c r="C21" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="12" t="s">
         <v>16</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="40" t="s">
+      <c r="H21" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I21" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J21" s="40" t="s">
+      <c r="J21" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="12" t="s">
-        <v>48</v>
+      <c r="K21" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="L21" s="13" t="s">
         <v>35</v>
@@ -3032,7 +2986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>16</v>
       </c>
@@ -3042,29 +2996,29 @@
       <c r="C22" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="12" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="40" t="s">
+      <c r="H22" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I22" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J22" s="40" t="s">
+      <c r="J22" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="12" t="s">
-        <v>49</v>
+      <c r="K22" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="L22" s="13" t="s">
         <v>35</v>
@@ -3073,10 +3027,10 @@
         <v>76</v>
       </c>
       <c r="N22" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>16</v>
       </c>
@@ -3086,29 +3040,29 @@
       <c r="C23" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="12" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="40" t="s">
+      <c r="H23" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I23" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J23" s="40" t="s">
+      <c r="J23" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="12" t="s">
-        <v>50</v>
+      <c r="K23" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="L23" s="13" t="s">
         <v>35</v>
@@ -3117,10 +3071,10 @@
         <v>76</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>16</v>
       </c>
@@ -3130,103 +3084,103 @@
       <c r="C24" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="12" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="40" t="s">
+      <c r="H24" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I24" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J24" s="40" t="s">
+      <c r="J24" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="12" t="s">
-        <v>109</v>
+      <c r="K24" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="L24" s="13" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="M24" s="56" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="77" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="78"/>
-      <c r="C25" s="78"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="78"/>
-      <c r="H25" s="78"/>
-      <c r="I25" s="78"/>
-      <c r="J25" s="78"/>
-      <c r="K25" s="78"/>
-      <c r="L25" s="78"/>
-      <c r="M25" s="78"/>
-      <c r="N25" s="78"/>
-    </row>
-    <row r="26" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="14" t="s">
+      <c r="F25" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="G25" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H26" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="13" t="s">
+      <c r="H25" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J26" s="12" t="s">
+      <c r="J25" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K26" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="L26" s="13" t="s">
+      <c r="K25" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L25" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M26" s="56" t="s">
+      <c r="M25" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="N26" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="N25" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="77" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="78"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="78"/>
+      <c r="L26" s="78"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="78"/>
+    </row>
+    <row r="27" spans="1:14" s="29" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>16</v>
       </c>
@@ -3236,29 +3190,29 @@
       <c r="C27" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="H27" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I27" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J27" s="12" t="s">
+      <c r="J27" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="13" t="s">
-        <v>59</v>
+      <c r="K27" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="L27" s="13" t="s">
         <v>35</v>
@@ -3270,7 +3224,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" s="29" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>16</v>
       </c>
@@ -3280,29 +3234,29 @@
       <c r="C28" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="12" t="s">
+      <c r="H28" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I28" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J28" s="12" t="s">
+      <c r="J28" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="L28" s="13" t="s">
         <v>35</v>
@@ -3314,51 +3268,25 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K29" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="L29" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M29" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N29" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="77" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="78"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="78"/>
+      <c r="I29" s="78"/>
+      <c r="J29" s="78"/>
+      <c r="K29" s="78"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="78"/>
+      <c r="N29" s="78"/>
+    </row>
+    <row r="30" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>16</v>
       </c>
@@ -3368,29 +3296,29 @@
       <c r="C30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F30" s="69" t="s">
+        <v>81</v>
+      </c>
+      <c r="G30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="12" t="s">
+      <c r="H30" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J30" s="12" t="s">
+      <c r="J30" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K30" s="13" t="s">
-        <v>62</v>
+      <c r="K30" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="L30" s="13" t="s">
         <v>35</v>
@@ -3399,10 +3327,10 @@
         <v>76</v>
       </c>
       <c r="N30" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>16</v>
       </c>
@@ -3412,59 +3340,85 @@
       <c r="C31" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G31" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G31" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="H31" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I31" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J31" s="12" t="s">
+      <c r="J31" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K31" s="13" t="s">
-        <v>110</v>
+      <c r="K31" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="L31" s="13" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="M31" s="56" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="N31" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="77" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="78"/>
-      <c r="C32" s="78"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="78"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
-      <c r="H32" s="78"/>
-      <c r="I32" s="78"/>
-      <c r="J32" s="78"/>
-      <c r="K32" s="78"/>
-      <c r="L32" s="78"/>
-      <c r="M32" s="78"/>
-      <c r="N32" s="78"/>
-    </row>
-    <row r="33" spans="1:14" s="29" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G32" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J32" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="L32" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M32" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>16</v>
       </c>
@@ -3478,10 +3432,10 @@
         <v>16</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F33" s="45" t="s">
-        <v>52</v>
+        <v>80</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="G33" s="40" t="s">
         <v>15</v>
@@ -3495,8 +3449,8 @@
       <c r="J33" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K33" s="29" t="s">
-        <v>54</v>
+      <c r="K33" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="L33" s="13" t="s">
         <v>35</v>
@@ -3508,7 +3462,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="29" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>16</v>
       </c>
@@ -3522,10 +3476,10 @@
         <v>16</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F34" s="45" t="s">
-        <v>52</v>
+        <v>80</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="G34" s="40" t="s">
         <v>15</v>
@@ -3539,8 +3493,8 @@
       <c r="J34" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K34" s="13" t="s">
-        <v>55</v>
+      <c r="K34" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="L34" s="13" t="s">
         <v>35</v>
@@ -3552,7 +3506,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>16</v>
       </c>
@@ -3566,10 +3520,10 @@
         <v>16</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F35" s="45" t="s">
-        <v>52</v>
+        <v>80</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="G35" s="40" t="s">
         <v>15</v>
@@ -3583,8 +3537,8 @@
       <c r="J35" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K35" s="13" t="s">
-        <v>111</v>
+      <c r="K35" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="L35" s="13" t="s">
         <v>35</v>
@@ -3593,26 +3547,52 @@
         <v>76</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="78"/>
-      <c r="C36" s="78"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="78"/>
-      <c r="G36" s="78"/>
-      <c r="H36" s="78"/>
-      <c r="I36" s="78"/>
-      <c r="J36" s="78"/>
-      <c r="K36" s="78"/>
-      <c r="L36" s="78"/>
-      <c r="M36" s="78"/>
-      <c r="N36" s="78"/>
+      <c r="F36" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G36" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J36" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="L36" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M36" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="37" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
@@ -3630,7 +3610,7 @@
       <c r="E37" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F37" s="69" t="s">
+      <c r="F37" s="12" t="s">
         <v>81</v>
       </c>
       <c r="G37" s="40" t="s">
@@ -3646,7 +3626,7 @@
         <v>17</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="L37" s="13" t="s">
         <v>35</v>
@@ -3690,7 +3670,7 @@
         <v>17</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="L38" s="13" t="s">
         <v>35</v>
@@ -3734,7 +3714,7 @@
         <v>17</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="L39" s="13" t="s">
         <v>35</v>
@@ -3778,7 +3758,7 @@
         <v>17</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="L40" s="13" t="s">
         <v>35</v>
@@ -3822,7 +3802,7 @@
         <v>17</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="L41" s="13" t="s">
         <v>35</v>
@@ -3834,313 +3814,117 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G42" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H42" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J42" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K42" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="L42" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M42" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N42" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F43" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G43" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H43" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I43" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J43" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K43" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="L43" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M43" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N43" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F44" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G44" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H44" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I44" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J44" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K44" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="L44" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M44" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N44" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G45" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H45" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I45" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J45" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K45" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="L45" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M45" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N45" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F46" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G46" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H46" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I46" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J46" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K46" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="L46" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M46" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N46" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G47" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H47" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I47" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J47" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K47" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="L47" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M47" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N47" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D48" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G48" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H48" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I48" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J48" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K48" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="L48" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M48" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N48" s="12" t="s">
-        <v>16</v>
-      </c>
+    <row r="42" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="12"/>
+      <c r="N42" s="12"/>
+    </row>
+    <row r="43" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="12"/>
+      <c r="N43" s="12"/>
+    </row>
+    <row r="44" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
+      <c r="N44" s="12"/>
+    </row>
+    <row r="45" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+    </row>
+    <row r="46" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+    </row>
+    <row r="47" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+    </row>
+    <row r="48" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="12"/>
+      <c r="M48" s="12"/>
+      <c r="N48" s="12"/>
     </row>
     <row r="49" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="12"/>
@@ -4174,117 +3958,117 @@
       <c r="M50" s="12"/>
       <c r="N50" s="12"/>
     </row>
-    <row r="51" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="12"/>
-      <c r="K51" s="12"/>
-      <c r="L51" s="12"/>
-      <c r="M51" s="12"/>
-      <c r="N51" s="12"/>
-    </row>
-    <row r="52" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="12"/>
-      <c r="K52" s="12"/>
-      <c r="L52" s="12"/>
-      <c r="M52" s="12"/>
-      <c r="N52" s="12"/>
-    </row>
-    <row r="53" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
-      <c r="K53" s="12"/>
-      <c r="L53" s="12"/>
-      <c r="M53" s="12"/>
-      <c r="N53" s="12"/>
-    </row>
-    <row r="54" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="12"/>
-      <c r="K54" s="12"/>
-      <c r="L54" s="12"/>
-      <c r="M54" s="12"/>
-      <c r="N54" s="12"/>
-    </row>
-    <row r="55" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="12"/>
-      <c r="L55" s="12"/>
-      <c r="M55" s="12"/>
-      <c r="N55" s="12"/>
-    </row>
-    <row r="56" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-      <c r="K56" s="12"/>
-      <c r="L56" s="12"/>
-      <c r="M56" s="12"/>
-      <c r="N56" s="12"/>
-    </row>
-    <row r="57" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12"/>
-      <c r="K57" s="12"/>
-      <c r="L57" s="12"/>
-      <c r="M57" s="12"/>
-      <c r="N57" s="12"/>
+    <row r="51" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="13"/>
+      <c r="N51" s="13"/>
+    </row>
+    <row r="52" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="13"/>
+      <c r="N52" s="13"/>
+    </row>
+    <row r="53" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="13"/>
+      <c r="N53" s="13"/>
+    </row>
+    <row r="54" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="13"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="46"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="46"/>
+      <c r="M54" s="46"/>
+      <c r="N54" s="13"/>
+    </row>
+    <row r="55" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="13"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="47"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="47"/>
+      <c r="M55" s="47"/>
+      <c r="N55" s="13"/>
+    </row>
+    <row r="56" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="13"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="47"/>
+      <c r="M56" s="47"/>
+      <c r="N56" s="13"/>
+    </row>
+    <row r="57" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="13"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="47"/>
+      <c r="M57" s="47"/>
+      <c r="N57" s="13"/>
     </row>
     <row r="58" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="13"/>
@@ -4344,10 +4128,10 @@
       <c r="G61" s="13"/>
       <c r="H61" s="13"/>
       <c r="I61" s="13"/>
-      <c r="J61" s="46"/>
-      <c r="K61" s="46"/>
-      <c r="L61" s="46"/>
-      <c r="M61" s="46"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
+      <c r="M61" s="13"/>
       <c r="N61" s="13"/>
     </row>
     <row r="62" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -4360,10 +4144,10 @@
       <c r="G62" s="13"/>
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
-      <c r="J62" s="47"/>
+      <c r="J62" s="13"/>
       <c r="K62" s="13"/>
-      <c r="L62" s="47"/>
-      <c r="M62" s="47"/>
+      <c r="L62" s="13"/>
+      <c r="M62" s="13"/>
       <c r="N62" s="13"/>
     </row>
     <row r="63" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -4378,313 +4162,278 @@
       <c r="I63" s="13"/>
       <c r="J63" s="13"/>
       <c r="K63" s="13"/>
-      <c r="L63" s="47"/>
-      <c r="M63" s="47"/>
+      <c r="L63" s="13"/>
+      <c r="M63" s="13"/>
       <c r="N63" s="13"/>
     </row>
-    <row r="64" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="13"/>
-      <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="13"/>
-      <c r="K64" s="13"/>
-      <c r="L64" s="47"/>
-      <c r="M64" s="47"/>
-      <c r="N64" s="13"/>
-    </row>
-    <row r="65" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="13"/>
-      <c r="B65" s="13"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="13"/>
-      <c r="K65" s="13"/>
-      <c r="L65" s="13"/>
-      <c r="M65" s="13"/>
-      <c r="N65" s="13"/>
-    </row>
-    <row r="66" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="13"/>
-      <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="13"/>
-      <c r="I66" s="13"/>
-      <c r="J66" s="13"/>
-      <c r="K66" s="13"/>
-      <c r="L66" s="13"/>
-      <c r="M66" s="13"/>
-      <c r="N66" s="13"/>
-    </row>
-    <row r="67" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="13"/>
-      <c r="B67" s="13"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
-      <c r="H67" s="13"/>
-      <c r="I67" s="13"/>
-      <c r="J67" s="13"/>
-      <c r="K67" s="13"/>
-      <c r="L67" s="13"/>
-      <c r="M67" s="13"/>
-      <c r="N67" s="13"/>
-    </row>
-    <row r="68" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="13"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="13"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
-      <c r="J68" s="13"/>
-      <c r="K68" s="13"/>
-      <c r="L68" s="13"/>
-      <c r="M68" s="13"/>
-      <c r="N68" s="13"/>
-    </row>
-    <row r="69" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="13"/>
-      <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="13"/>
-      <c r="H69" s="13"/>
-      <c r="I69" s="13"/>
-      <c r="J69" s="13"/>
-      <c r="K69" s="13"/>
-      <c r="L69" s="13"/>
-      <c r="M69" s="13"/>
-      <c r="N69" s="13"/>
-    </row>
-    <row r="70" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="13"/>
-      <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="13"/>
-      <c r="J70" s="13"/>
-      <c r="K70" s="13"/>
-      <c r="L70" s="13"/>
-      <c r="M70" s="13"/>
-      <c r="N70" s="13"/>
-    </row>
-    <row r="71" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="J73" s="49"/>
-      <c r="K73" s="49"/>
-      <c r="L73" s="49"/>
-      <c r="M73" s="49"/>
-    </row>
-    <row r="74" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="J74" s="50"/>
-      <c r="L74" s="50"/>
-      <c r="M74" s="50"/>
-    </row>
-    <row r="75" spans="1:14" s="44" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="J75" s="51"/>
-      <c r="K75" s="48"/>
-      <c r="L75" s="50"/>
-      <c r="M75" s="50"/>
-    </row>
-    <row r="76" spans="1:14" s="44" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C76" s="48"/>
-      <c r="F76" s="48"/>
-      <c r="J76" s="51"/>
-      <c r="K76" s="48"/>
-      <c r="L76" s="50"/>
-      <c r="M76" s="50"/>
-    </row>
-    <row r="77" spans="1:14" s="24" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C77" s="30"/>
-      <c r="F77" s="30"/>
-      <c r="J77" s="32"/>
-      <c r="K77" s="30"/>
-      <c r="L77" s="31"/>
-      <c r="M77" s="31"/>
-    </row>
-    <row r="78" spans="1:14" s="24" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C78" s="30"/>
-      <c r="F78" s="30"/>
-      <c r="J78" s="32"/>
-      <c r="K78" s="30"/>
-      <c r="L78" s="31"/>
-      <c r="M78" s="31"/>
-    </row>
-    <row r="79" spans="1:14" s="33" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C79" s="34"/>
-      <c r="F79" s="34"/>
-      <c r="K79" s="34"/>
-      <c r="M79" s="34"/>
-    </row>
-    <row r="80" spans="1:14" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="65" spans="3:13" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="66" spans="3:13" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J66" s="49"/>
+      <c r="K66" s="49"/>
+      <c r="L66" s="49"/>
+      <c r="M66" s="49"/>
+    </row>
+    <row r="67" spans="3:13" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J67" s="50"/>
+      <c r="L67" s="50"/>
+      <c r="M67" s="50"/>
+    </row>
+    <row r="68" spans="3:13" s="44" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C68" s="48"/>
+      <c r="F68" s="48"/>
+      <c r="J68" s="51"/>
+      <c r="K68" s="48"/>
+      <c r="L68" s="50"/>
+      <c r="M68" s="50"/>
+    </row>
+    <row r="69" spans="3:13" s="44" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C69" s="48"/>
+      <c r="F69" s="48"/>
+      <c r="J69" s="51"/>
+      <c r="K69" s="48"/>
+      <c r="L69" s="50"/>
+      <c r="M69" s="50"/>
+    </row>
+    <row r="70" spans="3:13" s="24" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C70" s="30"/>
+      <c r="F70" s="30"/>
+      <c r="J70" s="32"/>
+      <c r="K70" s="30"/>
+      <c r="L70" s="31"/>
+      <c r="M70" s="31"/>
+    </row>
+    <row r="71" spans="3:13" s="24" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C71" s="30"/>
+      <c r="F71" s="30"/>
+      <c r="J71" s="32"/>
+      <c r="K71" s="30"/>
+      <c r="L71" s="31"/>
+      <c r="M71" s="31"/>
+    </row>
+    <row r="72" spans="3:13" s="33" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C72" s="34"/>
+      <c r="F72" s="34"/>
+      <c r="K72" s="34"/>
+      <c r="M72" s="34"/>
+    </row>
+    <row r="73" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C73" s="35"/>
+      <c r="F73" s="35"/>
+      <c r="K73" s="35"/>
+      <c r="M73" s="35"/>
+    </row>
+    <row r="74" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C74" s="35"/>
+      <c r="F74" s="35"/>
+      <c r="K74" s="35"/>
+      <c r="M74" s="35"/>
+    </row>
+    <row r="75" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C75" s="35"/>
+      <c r="F75" s="35"/>
+      <c r="K75" s="35"/>
+      <c r="M75" s="35"/>
+    </row>
+    <row r="76" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C76" s="35"/>
+      <c r="F76" s="35"/>
+      <c r="J76" s="37"/>
+      <c r="K76" s="37"/>
+      <c r="L76" s="37"/>
+      <c r="M76" s="37"/>
+    </row>
+    <row r="77" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C77" s="35"/>
+      <c r="F77" s="35"/>
+      <c r="J77" s="38"/>
+      <c r="K77" s="35"/>
+      <c r="L77" s="39"/>
+      <c r="M77" s="39"/>
+    </row>
+    <row r="78" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C78" s="35"/>
+      <c r="F78" s="35"/>
+      <c r="J78" s="38"/>
+      <c r="K78" s="35"/>
+      <c r="L78" s="39"/>
+      <c r="M78" s="39"/>
+    </row>
+    <row r="79" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C79" s="35"/>
+      <c r="F79" s="35"/>
+      <c r="J79" s="38"/>
+      <c r="K79" s="35"/>
+      <c r="L79" s="39"/>
+      <c r="M79" s="39"/>
+    </row>
+    <row r="80" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C80" s="35"/>
       <c r="F80" s="35"/>
-      <c r="K80" s="35"/>
-      <c r="M80" s="35"/>
-    </row>
-    <row r="81" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J80" s="38"/>
+      <c r="K80" s="38"/>
+      <c r="L80" s="38"/>
+      <c r="M80" s="38"/>
+    </row>
+    <row r="81" spans="1:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C81" s="35"/>
       <c r="F81" s="35"/>
-      <c r="K81" s="35"/>
-      <c r="M81" s="35"/>
-    </row>
-    <row r="82" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C82" s="35"/>
-      <c r="F82" s="35"/>
-      <c r="K82" s="35"/>
-      <c r="M82" s="35"/>
-    </row>
-    <row r="83" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C83" s="35"/>
-      <c r="F83" s="35"/>
-      <c r="J83" s="37"/>
-      <c r="K83" s="37"/>
-      <c r="L83" s="37"/>
-      <c r="M83" s="37"/>
-    </row>
-    <row r="84" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C84" s="35"/>
-      <c r="F84" s="35"/>
-      <c r="J84" s="38"/>
-      <c r="K84" s="35"/>
-      <c r="L84" s="39"/>
-      <c r="M84" s="39"/>
-    </row>
-    <row r="85" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C85" s="35"/>
-      <c r="F85" s="35"/>
-      <c r="J85" s="38"/>
-      <c r="K85" s="35"/>
-      <c r="L85" s="39"/>
-      <c r="M85" s="39"/>
-    </row>
-    <row r="86" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C86" s="35"/>
-      <c r="F86" s="35"/>
-      <c r="J86" s="38"/>
-      <c r="K86" s="35"/>
-      <c r="L86" s="39"/>
-      <c r="M86" s="39"/>
-    </row>
-    <row r="87" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C87" s="35"/>
-      <c r="F87" s="35"/>
-      <c r="J87" s="38"/>
-      <c r="K87" s="38"/>
-      <c r="L87" s="38"/>
-      <c r="M87" s="38"/>
-    </row>
-    <row r="88" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C88" s="35"/>
-      <c r="F88" s="35"/>
-      <c r="J88" s="38"/>
-      <c r="K88" s="38"/>
-      <c r="L88" s="38"/>
-      <c r="M88" s="38"/>
-    </row>
-    <row r="89" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J81" s="38"/>
+      <c r="K81" s="38"/>
+      <c r="L81" s="38"/>
+      <c r="M81" s="38"/>
+    </row>
+    <row r="82" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="K82" s="18"/>
+      <c r="M82" s="18"/>
+    </row>
+    <row r="83" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="K83" s="18"/>
+      <c r="M83" s="18"/>
+    </row>
+    <row r="84" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="K84" s="18"/>
+      <c r="M84" s="18"/>
+    </row>
+    <row r="85" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="K85" s="18"/>
+      <c r="M85" s="18"/>
+    </row>
+    <row r="86" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C86" s="18"/>
+      <c r="F86" s="18"/>
+      <c r="J86" s="15"/>
+      <c r="K86" s="15"/>
+      <c r="L86" s="15"/>
+      <c r="M86" s="15"/>
+    </row>
+    <row r="87" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C87" s="18"/>
+      <c r="F87" s="18"/>
+      <c r="J87" s="17"/>
+      <c r="K87" s="18"/>
+      <c r="L87" s="16"/>
+      <c r="M87" s="16"/>
+    </row>
+    <row r="88" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C88" s="18"/>
+      <c r="F88" s="18"/>
+      <c r="J88" s="17"/>
+      <c r="K88" s="18"/>
+      <c r="L88" s="16"/>
+      <c r="M88" s="16"/>
+    </row>
+    <row r="89" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C89" s="18"/>
       <c r="F89" s="18"/>
+      <c r="J89" s="17"/>
       <c r="K89" s="18"/>
-      <c r="M89" s="18"/>
-    </row>
-    <row r="90" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L89" s="16"/>
+      <c r="M89" s="16"/>
+    </row>
+    <row r="90" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C90" s="18"/>
       <c r="F90" s="18"/>
-      <c r="K90" s="18"/>
-      <c r="M90" s="18"/>
-    </row>
-    <row r="91" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J90" s="17"/>
+      <c r="K90" s="17"/>
+      <c r="L90" s="17"/>
+      <c r="M90" s="17"/>
+    </row>
+    <row r="91" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C91" s="18"/>
       <c r="F91" s="18"/>
-      <c r="K91" s="18"/>
-      <c r="M91" s="18"/>
-    </row>
-    <row r="92" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J91" s="17"/>
+      <c r="K91" s="17"/>
+      <c r="L91" s="17"/>
+      <c r="M91" s="17"/>
+    </row>
+    <row r="92" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="20"/>
       <c r="C92" s="18"/>
+      <c r="D92" s="18"/>
+      <c r="E92" s="18"/>
       <c r="F92" s="18"/>
+      <c r="G92" s="18"/>
+      <c r="H92" s="18"/>
+      <c r="I92" s="18"/>
       <c r="K92" s="18"/>
       <c r="M92" s="18"/>
     </row>
-    <row r="93" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C93" s="18"/>
+      <c r="D93" s="18"/>
+      <c r="E93" s="18"/>
       <c r="F93" s="18"/>
-      <c r="J93" s="15"/>
-      <c r="K93" s="15"/>
-      <c r="L93" s="15"/>
-      <c r="M93" s="15"/>
-    </row>
-    <row r="94" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G93" s="18"/>
+      <c r="H93" s="18"/>
+      <c r="I93" s="18"/>
+      <c r="K93" s="18"/>
+      <c r="M93" s="18"/>
+    </row>
+    <row r="94" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C94" s="18"/>
+      <c r="D94" s="18"/>
+      <c r="E94" s="18"/>
       <c r="F94" s="18"/>
-      <c r="J94" s="17"/>
+      <c r="G94" s="18"/>
+      <c r="H94" s="18"/>
+      <c r="I94" s="18"/>
       <c r="K94" s="18"/>
-      <c r="L94" s="16"/>
-      <c r="M94" s="16"/>
-    </row>
-    <row r="95" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M94" s="18"/>
+    </row>
+    <row r="95" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C95" s="18"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="18"/>
       <c r="F95" s="18"/>
-      <c r="J95" s="17"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="18"/>
+      <c r="I95" s="18"/>
       <c r="K95" s="18"/>
-      <c r="L95" s="16"/>
-      <c r="M95" s="16"/>
-    </row>
-    <row r="96" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M95" s="18"/>
+    </row>
+    <row r="96" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C96" s="18"/>
+      <c r="D96" s="18"/>
+      <c r="E96" s="18"/>
       <c r="F96" s="18"/>
-      <c r="J96" s="17"/>
+      <c r="G96" s="18"/>
+      <c r="H96" s="18"/>
+      <c r="I96" s="18"/>
       <c r="K96" s="18"/>
-      <c r="L96" s="16"/>
-      <c r="M96" s="16"/>
-    </row>
-    <row r="97" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M96" s="18"/>
+    </row>
+    <row r="97" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18"/>
       <c r="F97" s="18"/>
-      <c r="J97" s="17"/>
-      <c r="K97" s="17"/>
-      <c r="L97" s="17"/>
-      <c r="M97" s="17"/>
-    </row>
-    <row r="98" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G97" s="18"/>
+      <c r="H97" s="18"/>
+      <c r="I97" s="18"/>
+      <c r="K97" s="18"/>
+      <c r="M97" s="18"/>
+    </row>
+    <row r="98" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C98" s="18"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
       <c r="F98" s="18"/>
-      <c r="J98" s="17"/>
-      <c r="K98" s="17"/>
-      <c r="L98" s="17"/>
-      <c r="M98" s="17"/>
-    </row>
-    <row r="99" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="20"/>
+      <c r="G98" s="18"/>
+      <c r="H98" s="18"/>
+      <c r="I98" s="18"/>
+      <c r="K98" s="18"/>
+      <c r="M98" s="18"/>
+    </row>
+    <row r="99" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C99" s="18"/>
       <c r="D99" s="18"/>
       <c r="E99" s="18"/>
@@ -4695,98 +4444,20 @@
       <c r="K99" s="18"/>
       <c r="M99" s="18"/>
     </row>
-    <row r="100" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C100" s="18"/>
-      <c r="D100" s="18"/>
-      <c r="E100" s="18"/>
-      <c r="F100" s="18"/>
-      <c r="G100" s="18"/>
-      <c r="H100" s="18"/>
-      <c r="I100" s="18"/>
-      <c r="K100" s="18"/>
-      <c r="M100" s="18"/>
-    </row>
-    <row r="101" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C101" s="18"/>
-      <c r="D101" s="18"/>
-      <c r="E101" s="18"/>
-      <c r="F101" s="18"/>
-      <c r="G101" s="18"/>
-      <c r="H101" s="18"/>
-      <c r="I101" s="18"/>
-      <c r="K101" s="18"/>
-      <c r="M101" s="18"/>
-    </row>
-    <row r="102" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C102" s="18"/>
-      <c r="D102" s="18"/>
-      <c r="E102" s="18"/>
-      <c r="F102" s="18"/>
-      <c r="G102" s="18"/>
-      <c r="H102" s="18"/>
-      <c r="I102" s="18"/>
-      <c r="K102" s="18"/>
-      <c r="M102" s="18"/>
-    </row>
-    <row r="103" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C103" s="18"/>
-      <c r="D103" s="18"/>
-      <c r="E103" s="18"/>
-      <c r="F103" s="18"/>
-      <c r="G103" s="18"/>
-      <c r="H103" s="18"/>
-      <c r="I103" s="18"/>
-      <c r="K103" s="18"/>
-      <c r="M103" s="18"/>
-    </row>
-    <row r="104" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C104" s="18"/>
-      <c r="D104" s="18"/>
-      <c r="E104" s="18"/>
-      <c r="F104" s="18"/>
-      <c r="G104" s="18"/>
-      <c r="H104" s="18"/>
-      <c r="I104" s="18"/>
-      <c r="K104" s="18"/>
-      <c r="M104" s="18"/>
-    </row>
-    <row r="105" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C105" s="18"/>
-      <c r="D105" s="18"/>
-      <c r="E105" s="18"/>
-      <c r="F105" s="18"/>
-      <c r="G105" s="18"/>
-      <c r="H105" s="18"/>
-      <c r="I105" s="18"/>
-      <c r="K105" s="18"/>
-      <c r="M105" s="18"/>
-    </row>
-    <row r="106" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C106" s="18"/>
-      <c r="D106" s="18"/>
-      <c r="E106" s="18"/>
-      <c r="F106" s="18"/>
-      <c r="G106" s="18"/>
-      <c r="H106" s="18"/>
-      <c r="I106" s="18"/>
-      <c r="K106" s="18"/>
-      <c r="M106" s="18"/>
-    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A32:XFD32"/>
-    <mergeCell ref="A36:XFD36"/>
-    <mergeCell ref="A6:XFD6"/>
-    <mergeCell ref="A16:XFD16"/>
-    <mergeCell ref="A19:XFD19"/>
-    <mergeCell ref="A25:XFD25"/>
+    <mergeCell ref="A5:XFD5"/>
+    <mergeCell ref="A13:XFD13"/>
+    <mergeCell ref="A15:XFD15"/>
+    <mergeCell ref="A20:XFD20"/>
+    <mergeCell ref="A26:XFD26"/>
+    <mergeCell ref="A29:XFD29"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F33" r:id="rId1" location="/79590444732ud/detail/userstory/134825813356" display="https://rally1.rallydev.com/ - /79590444732ud/detail/userstory/134825813356"/>
-    <hyperlink ref="F35" r:id="rId2" location="/79590444732ud/detail/userstory/134825813356" display="https://rally1.rallydev.com/ - /79590444732ud/detail/userstory/134825813356"/>
-    <hyperlink ref="F34" r:id="rId3" location="/79590444732ud/detail/userstory/134825813356" display="https://rally1.rallydev.com/ - /79590444732ud/detail/userstory/134825813356"/>
+    <hyperlink ref="F27" r:id="rId1" location="/79590444732ud/detail/userstory/134825813356" display="https://rally1.rallydev.com/ - /79590444732ud/detail/userstory/134825813356"/>
+    <hyperlink ref="F28" r:id="rId2" location="/79590444732ud/detail/userstory/134825813356" display="https://rally1.rallydev.com/ - /79590444732ud/detail/userstory/134825813356"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
819544 Updated for IOC Exit
</commit_message>
<xml_diff>
--- a/Requirement/Build 4/TAS eBilling RTM IB_ 2.0_592.xlsx
+++ b/Requirement/Build 4/TAS eBilling RTM IB_ 2.0_592.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhaispbalchj\Documents\eBilling Docs\Build 3&amp;4\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="45" yWindow="-30" windowWidth="23040" windowHeight="9630" activeTab="2"/>
+    <workbookView xWindow="-12" yWindow="7692" windowWidth="19236" windowHeight="3900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="84">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -111,9 +116,6 @@
     <t>Test Case ID (for Testable US0</t>
   </si>
   <si>
-    <t>TC1221 - CIT eBilling TS9 Validate the new ‘Dental’ claim indicator displays on the TPJI screen when there is an Active Outpatient Dental Claim (O/D). US14</t>
-  </si>
-  <si>
     <t>US14 - TPJI Indicator (USEB-14)</t>
   </si>
   <si>
@@ -159,9 +161,6 @@
     <t>TC1259 - CIT eBilling TS7 Dental Claim Creation - AutoBiller US1109</t>
   </si>
   <si>
-    <t>TC1260 -  CIT eBilling TS8 Complete Dental Claim US1108 and US131</t>
-  </si>
-  <si>
     <t>TC1342 -  CIT eBilling TS6 Copy New Dental Fields 1108 and US131</t>
   </si>
   <si>
@@ -217,15 +216,6 @@
   </si>
   <si>
     <t>IB*2.0*592</t>
-  </si>
-  <si>
-    <t>DE319, DE320</t>
-  </si>
-  <si>
-    <t>DE294</t>
-  </si>
-  <si>
-    <t>DE295, DE296, DE357</t>
   </si>
   <si>
     <r>
@@ -264,35 +254,52 @@
     </r>
   </si>
   <si>
-    <t>DE269, DE292, DE293, DE336, DE338, DE350, DE351, DE359, DE365, DE374, DE379, DE381</t>
-  </si>
-  <si>
     <t>November 2017</t>
   </si>
   <si>
-    <t>DE383</t>
-  </si>
-  <si>
-    <t>DE282, DE291, DE384</t>
-  </si>
-  <si>
     <t>Initial Draft Version for review</t>
   </si>
   <si>
-    <t>DE304, DE305, DE314, DE358, DE363, DE373, DE380, DE411</t>
-  </si>
-  <si>
-    <t>DE412</t>
-  </si>
-  <si>
     <t>Deleted Section 8 for US2503 and Sections 5.5 through 5.9 for US2487, per eBiz changing the functionality of Blds. 3&amp;4 to only send the NPI for Dental transactions.</t>
   </si>
   <si>
-    <t>IB*2.0*592_T10</t>
+    <t>Updated with results of final build testing.</t>
+  </si>
+  <si>
+    <t>December 2017</t>
+  </si>
+  <si>
+    <t>US 1108 - Enter/Edit Dental Claims                  US 131 - Create 837D Transaction</t>
+  </si>
+  <si>
+    <t>US 1108 - Enter/Edit Dental Claims                             US 131 - Create 837D Transaction</t>
+  </si>
+  <si>
+    <t>US 1108 - Enter/Edit Dental Claims                                  US 131 - Create 837D Transaction</t>
+  </si>
+  <si>
+    <t>US 1108 - Enter/Edit Dental Claims                         US 131 - Create 837D Transaction</t>
+  </si>
+  <si>
+    <t>US 1108 - Enter/Edit Dental Claims                                     US 131 - Create 837D Transaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US 1108 - Enter/Edit Dental Claims
+US 131 - Create 837D Transaction
+</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US 1108/US131 - Enter/Edit Dental Claims    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">US2487 - Insurance Company Entry/Edit - Dental      </t>
   </si>
   <si>
     <r>
-      <t>Version 3.0</t>
+      <t>Version 4.0</t>
     </r>
     <r>
       <rPr>
@@ -306,98 +313,33 @@
     </r>
   </si>
   <si>
-    <t>Updated with results of final build testing.</t>
-  </si>
-  <si>
-    <t>December 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US3528 - Provider ID Maintenance_Dental_Removal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a member of the eBilling Team, I have determined during User Acceptance Testing (UAT) that I no longer want to be able to define either human or facility Secondary Provider IDs to be used on Dental claim.   </t>
-  </si>
-  <si>
-    <t>TS14 – Regression Insurance Co ID Default</t>
-  </si>
-  <si>
-    <t>TS15 – Regression Ins Co ID Parameters</t>
-  </si>
-  <si>
-    <t>TS16 – Regression Billing Provider Secondary IDs</t>
-  </si>
-  <si>
-    <t>TS17 – Regression Additional Billing Provider Secondary IDs</t>
-  </si>
-  <si>
-    <t>TS34 – Regression Ins Co VA Lab/Facilitiy ID</t>
-  </si>
-  <si>
-    <t>TS27 – Regression VA Provider’s Own IDs</t>
-  </si>
-  <si>
-    <t>DE418</t>
-  </si>
-  <si>
-    <t>TS28 – Regression VA Provider’s Insurance IDs</t>
-  </si>
-  <si>
-    <t>TS29 – Regression Care Units</t>
-  </si>
-  <si>
-    <t>TS30 – Regression Non-VA Provider’s Own IDs</t>
-  </si>
-  <si>
-    <t>TS31 – Regression Non-VA Provider’s Ins IDs</t>
-  </si>
-  <si>
-    <t>TS32 – Regression Non-VA Facility’s Own IDs</t>
-  </si>
-  <si>
-    <t>TS33 – Regression Non-VA Facility’s Ins IDs</t>
-  </si>
-  <si>
-    <t>DE316, DE318</t>
-  </si>
-  <si>
-    <t>US 1108 - Enter/Edit Dental Claims                  US 131 - Create 837D Transaction</t>
-  </si>
-  <si>
-    <t>US 1108 - Enter/Edit Dental Claims                             US 131 - Create 837D Transaction</t>
-  </si>
-  <si>
-    <t>US 1108 - Enter/Edit Dental Claims                                  US 131 - Create 837D Transaction</t>
-  </si>
-  <si>
-    <t>US 1108 - Enter/Edit Dental Claims                         US 131 - Create 837D Transaction</t>
-  </si>
-  <si>
-    <t>US 1108 - Enter/Edit Dental Claims                                     US 131 - Create 837D Transaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US 1108 - Enter/Edit Dental Claims
-US 131 - Create 837D Transaction
-</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US 1108/US131 - Enter/Edit Dental Claims    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">US2487 - Insurance Company Entry/Edit - Dental      </t>
+    <t>September 2018</t>
+  </si>
+  <si>
+    <t>Updated with results of final build testing for T20.</t>
+  </si>
+  <si>
+    <t>IB*2.0*592_T20</t>
+  </si>
+  <si>
+    <t>TC2534 - CIT eBilling TS27 – Dental Claim Creation – AutoBiller- Auto Populated Fields – Production Only</t>
+  </si>
+  <si>
+    <t>TC1260 -  CIT eBilling TS8 Complete Dental Claim - Prod Only US1108 and US131</t>
+  </si>
+  <si>
+    <t>TC1626 - CIT eBilling TS29 - Print Bill – View Dental Using GEN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -562,6 +504,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
@@ -629,7 +577,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -703,19 +651,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -743,7 +678,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -844,6 +779,9 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -858,19 +796,19 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -878,9 +816,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -892,45 +827,46 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="28" fillId="3" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="29" fillId="3" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="28" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -946,7 +882,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -955,10 +891,10 @@
     <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1206,7 +1142,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1290,7 +1226,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1323,9 +1259,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1358,6 +1311,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1536,134 +1506,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A23" sqref="A23:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="21.140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.109375" style="1"/>
+    <col min="3" max="3" width="21.109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:8" ht="22.9" x14ac:dyDescent="0.4">
-      <c r="A5" s="71" t="s">
+    <row r="5" spans="1:8" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A5" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-    </row>
-    <row r="6" spans="1:8" ht="22.9" x14ac:dyDescent="0.4">
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+    </row>
+    <row r="6" spans="1:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="72" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-    </row>
-    <row r="8" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
+      <c r="A7" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+    </row>
+    <row r="8" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="17.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C18" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="74" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
-    </row>
-    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="75" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+    </row>
+    <row r="24" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="75" t="s">
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A26" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="75"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="75"/>
-      <c r="H26" s="75"/>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="76"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="76"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
     </row>
-    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
     </row>
-    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
     </row>
-    <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
     </row>
   </sheetData>
@@ -1683,30 +1653,30 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.33203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
     </row>
-    <row r="2" spans="1:4" ht="17.45" x14ac:dyDescent="0.3">
-      <c r="A2" s="76" t="s">
+    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-    </row>
-    <row r="3" spans="1:4" ht="13.9" x14ac:dyDescent="0.25">
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+    </row>
+    <row r="3" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
         <v>2</v>
       </c>
@@ -1720,115 +1690,123 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="61" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B4" s="59">
         <v>1</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="61" customFormat="1" ht="55.15" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="61" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B5" s="59">
         <v>2</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="61" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B6" s="59">
         <v>3</v>
       </c>
       <c r="C6" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="61" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="60" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
-      <c r="B7" s="59"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="60"/>
-    </row>
-    <row r="8" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+      <c r="B7" s="59">
+        <v>4</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="61" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="58"/>
       <c r="B8" s="59"/>
       <c r="C8" s="62"/>
       <c r="D8" s="60"/>
     </row>
-    <row r="9" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="61" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="58"/>
       <c r="B9" s="59"/>
       <c r="C9" s="62"/>
       <c r="D9" s="60"/>
     </row>
-    <row r="10" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="61" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="58"/>
       <c r="B10" s="59"/>
       <c r="C10" s="62"/>
       <c r="D10" s="60"/>
     </row>
-    <row r="11" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="61" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="65"/>
       <c r="B11" s="63"/>
       <c r="C11" s="63"/>
       <c r="D11" s="64"/>
     </row>
-    <row r="12" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="61" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="65"/>
       <c r="B12" s="63"/>
       <c r="C12" s="63"/>
       <c r="D12" s="64"/>
     </row>
-    <row r="13" spans="1:4" s="61" customFormat="1" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="61" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="66"/>
       <c r="B13" s="67"/>
       <c r="C13" s="67"/>
       <c r="D13" s="68"/>
     </row>
-    <row r="14" spans="1:4" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="54"/>
     </row>
-    <row r="15" spans="1:4" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="54"/>
     </row>
-    <row r="16" spans="1:4" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="54"/>
     </row>
-    <row r="17" spans="1:1" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="54"/>
     </row>
-    <row r="18" spans="1:1" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
     </row>
-    <row r="19" spans="1:1" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
     </row>
-    <row r="20" spans="1:1" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
     </row>
-    <row r="21" spans="1:1" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
     </row>
-    <row r="22" spans="1:1" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
     </row>
   </sheetData>
@@ -1847,29 +1825,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DQ99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="19" style="10" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="46.28515625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="28.28515625" style="10" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" style="10" customWidth="1"/>
-    <col min="14" max="14" width="26" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="60.33203125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="10" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" customWidth="1"/>
+    <col min="11" max="11" width="28.33203125" style="10" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" style="10" customWidth="1"/>
+    <col min="14" max="14" width="33.6640625" style="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:121" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:121" s="11" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>6</v>
       </c>
@@ -1898,7 +1876,7 @@
         <v>26</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K1" s="25" t="s">
         <v>27</v>
@@ -2020,9 +1998,9 @@
       <c r="DP1" s="21"/>
       <c r="DQ1" s="21"/>
     </row>
-    <row r="2" spans="1:121" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:121" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -2038,916 +2016,887 @@
       <c r="M2" s="22"/>
       <c r="N2" s="22"/>
     </row>
-    <row r="3" spans="1:121" s="42" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:121" s="43" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="70" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="41" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="H3" s="41" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J3" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="53" t="s">
-        <v>35</v>
+      <c r="K3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="M3" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>16</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="N3" s="13"/>
       <c r="O3" s="13"/>
     </row>
-    <row r="4" spans="1:121" s="42" customFormat="1" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="13" t="s">
+    <row r="4" spans="1:121" s="78" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="79"/>
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="79"/>
+      <c r="S4" s="79"/>
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="79"/>
+      <c r="Z4" s="79"/>
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="79"/>
+      <c r="AG4" s="79"/>
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="79"/>
+      <c r="AN4" s="79"/>
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="79"/>
+      <c r="AU4" s="79"/>
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="79"/>
+      <c r="BB4" s="79"/>
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="79"/>
+      <c r="BI4" s="79"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="79"/>
+      <c r="BM4" s="79"/>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="79"/>
+      <c r="BP4" s="79"/>
+      <c r="BQ4" s="79"/>
+      <c r="BR4" s="79"/>
+      <c r="BS4" s="79"/>
+      <c r="BT4" s="79"/>
+      <c r="BU4" s="79"/>
+      <c r="BV4" s="79"/>
+      <c r="BW4" s="79"/>
+      <c r="BX4" s="79"/>
+      <c r="BY4" s="79"/>
+      <c r="BZ4" s="79"/>
+      <c r="CA4" s="79"/>
+      <c r="CB4" s="79"/>
+      <c r="CC4" s="79"/>
+      <c r="CD4" s="79"/>
+      <c r="CE4" s="79"/>
+      <c r="CF4" s="79"/>
+      <c r="CG4" s="79"/>
+      <c r="CH4" s="79"/>
+      <c r="CI4" s="79"/>
+      <c r="CJ4" s="79"/>
+      <c r="CK4" s="79"/>
+      <c r="CL4" s="79"/>
+      <c r="CM4" s="79"/>
+      <c r="CN4" s="79"/>
+      <c r="CO4" s="79"/>
+      <c r="CP4" s="79"/>
+      <c r="CQ4" s="79"/>
+      <c r="CR4" s="79"/>
+      <c r="CS4" s="79"/>
+      <c r="CT4" s="79"/>
+      <c r="CU4" s="79"/>
+      <c r="CV4" s="79"/>
+      <c r="CW4" s="79"/>
+      <c r="CX4" s="79"/>
+      <c r="CY4" s="79"/>
+      <c r="CZ4" s="79"/>
+      <c r="DA4" s="79"/>
+      <c r="DB4" s="79"/>
+      <c r="DC4" s="79"/>
+      <c r="DD4" s="79"/>
+      <c r="DE4" s="79"/>
+      <c r="DF4" s="79"/>
+      <c r="DG4" s="79"/>
+      <c r="DH4" s="79"/>
+      <c r="DI4" s="79"/>
+      <c r="DJ4" s="79"/>
+      <c r="DK4" s="79"/>
+      <c r="DL4" s="79"/>
+      <c r="DM4" s="79"/>
+      <c r="DN4" s="79"/>
+      <c r="DO4" s="79"/>
+      <c r="DP4" s="79"/>
+      <c r="DQ4" s="79"/>
+    </row>
+    <row r="5" spans="1:121" s="44" customFormat="1" ht="194.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="40" t="s">
+      <c r="D5" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J4" s="40" t="s">
+      <c r="H5" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="O4" s="13"/>
-    </row>
-    <row r="5" spans="1:121" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="78"/>
-      <c r="S5" s="78"/>
-      <c r="T5" s="78"/>
-      <c r="U5" s="78"/>
-      <c r="V5" s="78"/>
-      <c r="W5" s="78"/>
-      <c r="X5" s="78"/>
-      <c r="Y5" s="78"/>
-      <c r="Z5" s="78"/>
-      <c r="AA5" s="78"/>
-      <c r="AB5" s="78"/>
-      <c r="AC5" s="78"/>
-      <c r="AD5" s="78"/>
-      <c r="AE5" s="78"/>
-      <c r="AF5" s="78"/>
-      <c r="AG5" s="78"/>
-      <c r="AH5" s="78"/>
-      <c r="AI5" s="78"/>
-      <c r="AJ5" s="78"/>
-      <c r="AK5" s="78"/>
-      <c r="AL5" s="78"/>
-      <c r="AM5" s="78"/>
-      <c r="AN5" s="78"/>
-      <c r="AO5" s="78"/>
-      <c r="AP5" s="78"/>
-      <c r="AQ5" s="78"/>
-      <c r="AR5" s="78"/>
-      <c r="AS5" s="78"/>
-      <c r="AT5" s="78"/>
-      <c r="AU5" s="78"/>
-      <c r="AV5" s="78"/>
-      <c r="AW5" s="78"/>
-      <c r="AX5" s="78"/>
-      <c r="AY5" s="78"/>
-      <c r="AZ5" s="78"/>
-      <c r="BA5" s="78"/>
-      <c r="BB5" s="78"/>
-      <c r="BC5" s="78"/>
-      <c r="BD5" s="78"/>
-      <c r="BE5" s="78"/>
-      <c r="BF5" s="78"/>
-      <c r="BG5" s="78"/>
-      <c r="BH5" s="78"/>
-      <c r="BI5" s="78"/>
-      <c r="BJ5" s="78"/>
-      <c r="BK5" s="78"/>
-      <c r="BL5" s="78"/>
-      <c r="BM5" s="78"/>
-      <c r="BN5" s="78"/>
-      <c r="BO5" s="78"/>
-      <c r="BP5" s="78"/>
-      <c r="BQ5" s="78"/>
-      <c r="BR5" s="78"/>
-      <c r="BS5" s="78"/>
-      <c r="BT5" s="78"/>
-      <c r="BU5" s="78"/>
-      <c r="BV5" s="78"/>
-      <c r="BW5" s="78"/>
-      <c r="BX5" s="78"/>
-      <c r="BY5" s="78"/>
-      <c r="BZ5" s="78"/>
-      <c r="CA5" s="78"/>
-      <c r="CB5" s="78"/>
-      <c r="CC5" s="78"/>
-      <c r="CD5" s="78"/>
-      <c r="CE5" s="78"/>
-      <c r="CF5" s="78"/>
-      <c r="CG5" s="78"/>
-      <c r="CH5" s="78"/>
-      <c r="CI5" s="78"/>
-      <c r="CJ5" s="78"/>
-      <c r="CK5" s="78"/>
-      <c r="CL5" s="78"/>
-      <c r="CM5" s="78"/>
-      <c r="CN5" s="78"/>
-      <c r="CO5" s="78"/>
-      <c r="CP5" s="78"/>
-      <c r="CQ5" s="78"/>
-      <c r="CR5" s="78"/>
-      <c r="CS5" s="78"/>
-      <c r="CT5" s="78"/>
-      <c r="CU5" s="78"/>
-      <c r="CV5" s="78"/>
-      <c r="CW5" s="78"/>
-      <c r="CX5" s="78"/>
-      <c r="CY5" s="78"/>
-      <c r="CZ5" s="78"/>
-      <c r="DA5" s="78"/>
-      <c r="DB5" s="78"/>
-      <c r="DC5" s="78"/>
-      <c r="DD5" s="78"/>
-      <c r="DE5" s="78"/>
-      <c r="DF5" s="78"/>
-      <c r="DG5" s="78"/>
-      <c r="DH5" s="78"/>
-      <c r="DI5" s="78"/>
-      <c r="DJ5" s="78"/>
-      <c r="DK5" s="78"/>
-      <c r="DL5" s="78"/>
-      <c r="DM5" s="78"/>
-      <c r="DN5" s="78"/>
-      <c r="DO5" s="78"/>
-      <c r="DP5" s="78"/>
-      <c r="DQ5" s="78"/>
-    </row>
-    <row r="6" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
+      <c r="L5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="N5" s="13"/>
+    </row>
+    <row r="6" spans="1:121" s="44" customFormat="1" ht="193.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="41" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="40" t="s">
+      <c r="G6" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="41" t="s">
         <v>16</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J6" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="42" t="s">
         <v>17</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>38</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M6" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N6" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="N6" s="13"/>
+    </row>
+    <row r="7" spans="1:121" s="44" customFormat="1" ht="190.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="41" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="41" t="s">
         <v>16</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J7" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" s="42" t="s">
         <v>17</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>39</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M7" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="N7" s="13"/>
+    </row>
+    <row r="8" spans="1:121" s="44" customFormat="1" ht="191.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="41" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="40" t="s">
+      <c r="G8" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="40" t="s">
+      <c r="H8" s="41" t="s">
         <v>16</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J8" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="42" t="s">
         <v>17</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>40</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M8" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N8" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="N8" s="13"/>
+    </row>
+    <row r="9" spans="1:121" s="44" customFormat="1" ht="197.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="41" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="40" t="s">
+      <c r="G9" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="41" t="s">
         <v>16</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J9" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="42" t="s">
         <v>17</v>
       </c>
       <c r="K9" s="12" t="s">
         <v>41</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M9" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N9" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="N9" s="13"/>
+    </row>
+    <row r="10" spans="1:121" s="44" customFormat="1" ht="192.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>100</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="40" t="s">
+      <c r="G10" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="H10" s="41" t="s">
         <v>16</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J10" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="42" t="s">
         <v>17</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M10" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="N10" s="13"/>
+    </row>
+    <row r="11" spans="1:121" s="44" customFormat="1" ht="200.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="41" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="40" t="s">
+      <c r="G11" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="40" t="s">
+      <c r="H11" s="41" t="s">
         <v>16</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J11" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="42" t="s">
         <v>17</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M11" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N11" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:121" s="43" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="N11" s="13"/>
+    </row>
+    <row r="12" spans="1:121" s="78" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="40" t="s">
+      <c r="B12" s="79"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="79"/>
+      <c r="N12" s="79"/>
+      <c r="O12" s="79"/>
+      <c r="P12" s="79"/>
+      <c r="Q12" s="79"/>
+      <c r="R12" s="79"/>
+      <c r="S12" s="79"/>
+      <c r="T12" s="79"/>
+      <c r="U12" s="79"/>
+      <c r="V12" s="79"/>
+      <c r="W12" s="79"/>
+      <c r="X12" s="79"/>
+      <c r="Y12" s="79"/>
+      <c r="Z12" s="79"/>
+      <c r="AA12" s="79"/>
+      <c r="AB12" s="79"/>
+      <c r="AC12" s="79"/>
+      <c r="AD12" s="79"/>
+      <c r="AE12" s="79"/>
+      <c r="AF12" s="79"/>
+      <c r="AG12" s="79"/>
+      <c r="AH12" s="79"/>
+      <c r="AI12" s="79"/>
+      <c r="AJ12" s="79"/>
+      <c r="AK12" s="79"/>
+      <c r="AL12" s="79"/>
+      <c r="AM12" s="79"/>
+      <c r="AN12" s="79"/>
+      <c r="AO12" s="79"/>
+      <c r="AP12" s="79"/>
+      <c r="AQ12" s="79"/>
+      <c r="AR12" s="79"/>
+      <c r="AS12" s="79"/>
+      <c r="AT12" s="79"/>
+      <c r="AU12" s="79"/>
+      <c r="AV12" s="79"/>
+      <c r="AW12" s="79"/>
+      <c r="AX12" s="79"/>
+      <c r="AY12" s="79"/>
+      <c r="AZ12" s="79"/>
+      <c r="BA12" s="79"/>
+      <c r="BB12" s="79"/>
+      <c r="BC12" s="79"/>
+      <c r="BD12" s="79"/>
+      <c r="BE12" s="79"/>
+      <c r="BF12" s="79"/>
+      <c r="BG12" s="79"/>
+      <c r="BH12" s="79"/>
+      <c r="BI12" s="79"/>
+      <c r="BJ12" s="79"/>
+      <c r="BK12" s="79"/>
+      <c r="BL12" s="79"/>
+      <c r="BM12" s="79"/>
+      <c r="BN12" s="79"/>
+      <c r="BO12" s="79"/>
+      <c r="BP12" s="79"/>
+      <c r="BQ12" s="79"/>
+      <c r="BR12" s="79"/>
+      <c r="BS12" s="79"/>
+      <c r="BT12" s="79"/>
+      <c r="BU12" s="79"/>
+      <c r="BV12" s="79"/>
+      <c r="BW12" s="79"/>
+      <c r="BX12" s="79"/>
+      <c r="BY12" s="79"/>
+      <c r="BZ12" s="79"/>
+      <c r="CA12" s="79"/>
+      <c r="CB12" s="79"/>
+      <c r="CC12" s="79"/>
+      <c r="CD12" s="79"/>
+      <c r="CE12" s="79"/>
+      <c r="CF12" s="79"/>
+      <c r="CG12" s="79"/>
+      <c r="CH12" s="79"/>
+      <c r="CI12" s="79"/>
+      <c r="CJ12" s="79"/>
+      <c r="CK12" s="79"/>
+      <c r="CL12" s="79"/>
+      <c r="CM12" s="79"/>
+      <c r="CN12" s="79"/>
+      <c r="CO12" s="79"/>
+      <c r="CP12" s="79"/>
+      <c r="CQ12" s="79"/>
+      <c r="CR12" s="79"/>
+      <c r="CS12" s="79"/>
+      <c r="CT12" s="79"/>
+      <c r="CU12" s="79"/>
+      <c r="CV12" s="79"/>
+      <c r="CW12" s="79"/>
+      <c r="CX12" s="79"/>
+      <c r="CY12" s="79"/>
+      <c r="CZ12" s="79"/>
+      <c r="DA12" s="79"/>
+      <c r="DB12" s="79"/>
+      <c r="DC12" s="79"/>
+      <c r="DD12" s="79"/>
+      <c r="DE12" s="79"/>
+      <c r="DF12" s="79"/>
+      <c r="DG12" s="79"/>
+      <c r="DH12" s="79"/>
+      <c r="DI12" s="79"/>
+      <c r="DJ12" s="79"/>
+      <c r="DK12" s="79"/>
+      <c r="DL12" s="79"/>
+      <c r="DM12" s="79"/>
+      <c r="DN12" s="79"/>
+      <c r="DO12" s="79"/>
+      <c r="DP12" s="79"/>
+      <c r="DQ12" s="79"/>
+    </row>
+    <row r="13" spans="1:121" s="70" customFormat="1" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="41" t="s">
+      <c r="H13" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M12" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N12" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:121" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="77" t="s">
+      <c r="K13" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="78"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="78"/>
-      <c r="M13" s="78"/>
-      <c r="N13" s="78"/>
-      <c r="O13" s="78"/>
-      <c r="P13" s="78"/>
-      <c r="Q13" s="78"/>
-      <c r="R13" s="78"/>
-      <c r="S13" s="78"/>
-      <c r="T13" s="78"/>
-      <c r="U13" s="78"/>
-      <c r="V13" s="78"/>
-      <c r="W13" s="78"/>
-      <c r="X13" s="78"/>
-      <c r="Y13" s="78"/>
-      <c r="Z13" s="78"/>
-      <c r="AA13" s="78"/>
-      <c r="AB13" s="78"/>
-      <c r="AC13" s="78"/>
-      <c r="AD13" s="78"/>
-      <c r="AE13" s="78"/>
-      <c r="AF13" s="78"/>
-      <c r="AG13" s="78"/>
-      <c r="AH13" s="78"/>
-      <c r="AI13" s="78"/>
-      <c r="AJ13" s="78"/>
-      <c r="AK13" s="78"/>
-      <c r="AL13" s="78"/>
-      <c r="AM13" s="78"/>
-      <c r="AN13" s="78"/>
-      <c r="AO13" s="78"/>
-      <c r="AP13" s="78"/>
-      <c r="AQ13" s="78"/>
-      <c r="AR13" s="78"/>
-      <c r="AS13" s="78"/>
-      <c r="AT13" s="78"/>
-      <c r="AU13" s="78"/>
-      <c r="AV13" s="78"/>
-      <c r="AW13" s="78"/>
-      <c r="AX13" s="78"/>
-      <c r="AY13" s="78"/>
-      <c r="AZ13" s="78"/>
-      <c r="BA13" s="78"/>
-      <c r="BB13" s="78"/>
-      <c r="BC13" s="78"/>
-      <c r="BD13" s="78"/>
-      <c r="BE13" s="78"/>
-      <c r="BF13" s="78"/>
-      <c r="BG13" s="78"/>
-      <c r="BH13" s="78"/>
-      <c r="BI13" s="78"/>
-      <c r="BJ13" s="78"/>
-      <c r="BK13" s="78"/>
-      <c r="BL13" s="78"/>
-      <c r="BM13" s="78"/>
-      <c r="BN13" s="78"/>
-      <c r="BO13" s="78"/>
-      <c r="BP13" s="78"/>
-      <c r="BQ13" s="78"/>
-      <c r="BR13" s="78"/>
-      <c r="BS13" s="78"/>
-      <c r="BT13" s="78"/>
-      <c r="BU13" s="78"/>
-      <c r="BV13" s="78"/>
-      <c r="BW13" s="78"/>
-      <c r="BX13" s="78"/>
-      <c r="BY13" s="78"/>
-      <c r="BZ13" s="78"/>
-      <c r="CA13" s="78"/>
-      <c r="CB13" s="78"/>
-      <c r="CC13" s="78"/>
-      <c r="CD13" s="78"/>
-      <c r="CE13" s="78"/>
-      <c r="CF13" s="78"/>
-      <c r="CG13" s="78"/>
-      <c r="CH13" s="78"/>
-      <c r="CI13" s="78"/>
-      <c r="CJ13" s="78"/>
-      <c r="CK13" s="78"/>
-      <c r="CL13" s="78"/>
-      <c r="CM13" s="78"/>
-      <c r="CN13" s="78"/>
-      <c r="CO13" s="78"/>
-      <c r="CP13" s="78"/>
-      <c r="CQ13" s="78"/>
-      <c r="CR13" s="78"/>
-      <c r="CS13" s="78"/>
-      <c r="CT13" s="78"/>
-      <c r="CU13" s="78"/>
-      <c r="CV13" s="78"/>
-      <c r="CW13" s="78"/>
-      <c r="CX13" s="78"/>
-      <c r="CY13" s="78"/>
-      <c r="CZ13" s="78"/>
-      <c r="DA13" s="78"/>
-      <c r="DB13" s="78"/>
-      <c r="DC13" s="78"/>
-      <c r="DD13" s="78"/>
-      <c r="DE13" s="78"/>
-      <c r="DF13" s="78"/>
-      <c r="DG13" s="78"/>
-      <c r="DH13" s="78"/>
-      <c r="DI13" s="78"/>
-      <c r="DJ13" s="78"/>
-      <c r="DK13" s="78"/>
-      <c r="DL13" s="78"/>
-      <c r="DM13" s="78"/>
-      <c r="DN13" s="78"/>
-      <c r="DO13" s="78"/>
-      <c r="DP13" s="78"/>
-      <c r="DQ13" s="78"/>
-    </row>
-    <row r="14" spans="1:121" s="43" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="M13" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="N13" s="13"/>
+    </row>
+    <row r="14" spans="1:121" s="70" customFormat="1" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="41" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="40" t="s">
+      <c r="G14" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="40" t="s">
+      <c r="H14" s="41" t="s">
         <v>16</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J14" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="41" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M14" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="N14" s="13"/>
+    </row>
+    <row r="15" spans="1:121" s="80" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="N14" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:121" s="79" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="79" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="80"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="80"/>
-      <c r="K15" s="80"/>
-      <c r="L15" s="80"/>
-      <c r="M15" s="80"/>
-      <c r="N15" s="80"/>
-    </row>
-    <row r="16" spans="1:121" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="B15" s="81"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="81"/>
+      <c r="L15" s="81"/>
+      <c r="M15" s="81"/>
+      <c r="N15" s="81"/>
+    </row>
+    <row r="16" spans="1:121" s="44" customFormat="1" ht="159.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="41" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="40" t="s">
+      <c r="G16" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="41" t="s">
         <v>16</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J16" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" s="41" t="s">
         <v>17</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M16" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N16" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="N16" s="13"/>
+    </row>
+    <row r="17" spans="1:14" s="44" customFormat="1" ht="155.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="41" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="40" t="s">
+      <c r="G17" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="40" t="s">
+      <c r="H17" s="41" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J17" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="41" t="s">
         <v>17</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M17" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N17" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="N17" s="13"/>
+    </row>
+    <row r="18" spans="1:14" s="44" customFormat="1" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="41" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="40" t="s">
+      <c r="G18" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="40" t="s">
+      <c r="H18" s="41" t="s">
         <v>16</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J18" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="41" t="s">
         <v>17</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M18" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N18" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" s="43" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="N18" s="13"/>
+    </row>
+    <row r="19" spans="1:14" s="44" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="41" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="40" t="s">
+      <c r="G19" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="40" t="s">
+      <c r="H19" s="41" t="s">
         <v>16</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J19" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" s="41" t="s">
         <v>17</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M19" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N19" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="77" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="78"/>
-      <c r="C20" s="78"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="78"/>
-      <c r="L20" s="78"/>
-      <c r="M20" s="78"/>
-      <c r="N20" s="78"/>
-    </row>
-    <row r="21" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="N19" s="13"/>
+    </row>
+    <row r="20" spans="1:14" s="78" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="78" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="79"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="79"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="79"/>
+      <c r="N20" s="79"/>
+    </row>
+    <row r="21" spans="1:14" s="49" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>18</v>
@@ -2956,7 +2905,7 @@
         <v>16</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F21" s="14" t="s">
         <v>23</v>
@@ -2968,30 +2917,28 @@
         <v>16</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J21" s="12" t="s">
         <v>17</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L21" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M21" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N21" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="N21" s="13"/>
+    </row>
+    <row r="22" spans="1:14" s="49" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>18</v>
@@ -3000,7 +2947,7 @@
         <v>16</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>23</v>
@@ -3012,30 +2959,28 @@
         <v>16</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J22" s="12" t="s">
         <v>17</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L22" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M22" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N22" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="N22" s="13"/>
+    </row>
+    <row r="23" spans="1:14" s="49" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>18</v>
@@ -3044,7 +2989,7 @@
         <v>16</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>23</v>
@@ -3056,30 +3001,28 @@
         <v>16</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J23" s="12" t="s">
         <v>17</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L23" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M23" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N23" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="N23" s="13"/>
+    </row>
+    <row r="24" spans="1:14" s="49" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>18</v>
@@ -3088,7 +3031,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>23</v>
@@ -3100,30 +3043,28 @@
         <v>16</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J24" s="12" t="s">
         <v>17</v>
       </c>
       <c r="K24" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L24" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M24" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N24" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" s="48" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="N24" s="13"/>
+    </row>
+    <row r="25" spans="1:14" s="49" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>18</v>
@@ -3132,7 +3073,7 @@
         <v>16</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>23</v>
@@ -3144,677 +3085,359 @@
         <v>16</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J25" s="12" t="s">
         <v>17</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M25" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N25" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="77" t="s">
+        <v>80</v>
+      </c>
+      <c r="N25" s="13"/>
+    </row>
+    <row r="26" spans="1:14" s="49" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="78"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="78"/>
-      <c r="I26" s="78"/>
-      <c r="J26" s="78"/>
-      <c r="K26" s="78"/>
-      <c r="L26" s="78"/>
-      <c r="M26" s="78"/>
-      <c r="N26" s="78"/>
-    </row>
-    <row r="27" spans="1:14" s="29" customFormat="1" ht="51" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F27" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="40" t="s">
+      <c r="F26" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J27" s="40" t="s">
+      <c r="H26" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J26" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L27" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M27" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N27" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" s="29" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+      <c r="K26" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M26" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="N26" s="13"/>
+    </row>
+    <row r="27" spans="1:14" s="78" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="78" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="79"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="79"/>
+      <c r="I27" s="79"/>
+      <c r="J27" s="79"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="79"/>
+      <c r="M27" s="79"/>
+      <c r="N27" s="79"/>
+    </row>
+    <row r="28" spans="1:14" s="29" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="41" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F28" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J28" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G28" s="40" t="s">
+      <c r="L28" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M28" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="N28" s="13"/>
+    </row>
+    <row r="29" spans="1:14" s="29" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J28" s="40" t="s">
+      <c r="H29" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J29" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="L28" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M28" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N28" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" s="77" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="77" t="s">
+      <c r="K29" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M29" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="78"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="78"/>
-      <c r="I29" s="78"/>
-      <c r="J29" s="78"/>
-      <c r="K29" s="78"/>
-      <c r="L29" s="78"/>
-      <c r="M29" s="78"/>
-      <c r="N29" s="78"/>
-    </row>
-    <row r="30" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F30" s="69" t="s">
-        <v>81</v>
-      </c>
-      <c r="G30" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J30" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K30" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="L30" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M30" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N30" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G31" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J31" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="L31" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M31" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N31" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G32" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J32" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K32" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="L32" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M32" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N32" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G33" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J33" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K33" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="L33" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M33" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N33" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G34" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H34" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J34" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K34" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="L34" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M34" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N34" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G35" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H35" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J35" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="L35" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M35" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N35" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G36" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H36" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J36" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="L36" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M36" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N36" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G37" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H37" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I37" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J37" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K37" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="L37" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M37" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N37" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G38" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H38" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J38" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="L38" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M38" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N38" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G39" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H39" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J39" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="L39" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M39" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N39" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G40" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H40" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J40" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K40" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="L40" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M40" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N40" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" s="55" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F41" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G41" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H41" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J41" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="K41" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="L41" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M41" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N41" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N29" s="13"/>
+    </row>
+    <row r="30" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="13"/>
+    </row>
+    <row r="31" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="13"/>
+    </row>
+    <row r="32" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="13"/>
+    </row>
+    <row r="33" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="56"/>
+      <c r="N33" s="13"/>
+    </row>
+    <row r="34" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="56"/>
+      <c r="N34" s="13"/>
+    </row>
+    <row r="35" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="13"/>
+    </row>
+    <row r="36" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="56"/>
+      <c r="N36" s="13"/>
+    </row>
+    <row r="37" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="41"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="56"/>
+      <c r="N37" s="13"/>
+    </row>
+    <row r="38" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="41"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="56"/>
+      <c r="N38" s="13"/>
+    </row>
+    <row r="39" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="56"/>
+      <c r="N39" s="13"/>
+    </row>
+    <row r="40" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="41"/>
+      <c r="H40" s="41"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="41"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="56"/>
+      <c r="N40" s="13"/>
+    </row>
+    <row r="41" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="41"/>
+      <c r="H41" s="41"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="41"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="56"/>
+      <c r="N41" s="13"/>
+    </row>
+    <row r="42" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -3828,9 +3451,9 @@
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
       <c r="M42" s="12"/>
-      <c r="N42" s="12"/>
-    </row>
-    <row r="43" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N42" s="13"/>
+    </row>
+    <row r="43" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
@@ -3844,9 +3467,9 @@
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
       <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-    </row>
-    <row r="44" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N43" s="13"/>
+    </row>
+    <row r="44" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
@@ -3860,9 +3483,9 @@
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
       <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
-    </row>
-    <row r="45" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N44" s="13"/>
+    </row>
+    <row r="45" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
@@ -3876,9 +3499,9 @@
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
       <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-    </row>
-    <row r="46" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N45" s="13"/>
+    </row>
+    <row r="46" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
@@ -3892,9 +3515,9 @@
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
       <c r="M46" s="12"/>
-      <c r="N46" s="12"/>
-    </row>
-    <row r="47" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N46" s="13"/>
+    </row>
+    <row r="47" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
@@ -3908,9 +3531,9 @@
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
       <c r="M47" s="12"/>
-      <c r="N47" s="12"/>
-    </row>
-    <row r="48" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N47" s="13"/>
+    </row>
+    <row r="48" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
@@ -3924,9 +3547,9 @@
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
       <c r="M48" s="12"/>
-      <c r="N48" s="12"/>
-    </row>
-    <row r="49" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N48" s="13"/>
+    </row>
+    <row r="49" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
@@ -3940,9 +3563,9 @@
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
       <c r="M49" s="12"/>
-      <c r="N49" s="12"/>
-    </row>
-    <row r="50" spans="1:14" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N49" s="13"/>
+    </row>
+    <row r="50" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
@@ -3956,9 +3579,9 @@
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
       <c r="M50" s="12"/>
-      <c r="N50" s="12"/>
-    </row>
-    <row r="51" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N50" s="13"/>
+    </row>
+    <row r="51" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
@@ -3974,7 +3597,7 @@
       <c r="M51" s="13"/>
       <c r="N51" s="13"/>
     </row>
-    <row r="52" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="13"/>
@@ -3990,7 +3613,7 @@
       <c r="M52" s="13"/>
       <c r="N52" s="13"/>
     </row>
-    <row r="53" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
@@ -4006,7 +3629,7 @@
       <c r="M53" s="13"/>
       <c r="N53" s="13"/>
     </row>
-    <row r="54" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
@@ -4016,13 +3639,13 @@
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
-      <c r="J54" s="46"/>
-      <c r="K54" s="46"/>
-      <c r="L54" s="46"/>
-      <c r="M54" s="46"/>
+      <c r="J54" s="47"/>
+      <c r="K54" s="47"/>
+      <c r="L54" s="47"/>
+      <c r="M54" s="47"/>
       <c r="N54" s="13"/>
     </row>
-    <row r="55" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="13"/>
@@ -4032,13 +3655,13 @@
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
       <c r="I55" s="13"/>
-      <c r="J55" s="47"/>
+      <c r="J55" s="48"/>
       <c r="K55" s="13"/>
-      <c r="L55" s="47"/>
-      <c r="M55" s="47"/>
+      <c r="L55" s="48"/>
+      <c r="M55" s="48"/>
       <c r="N55" s="13"/>
     </row>
-    <row r="56" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
@@ -4050,11 +3673,11 @@
       <c r="I56" s="13"/>
       <c r="J56" s="13"/>
       <c r="K56" s="13"/>
-      <c r="L56" s="47"/>
-      <c r="M56" s="47"/>
+      <c r="L56" s="48"/>
+      <c r="M56" s="48"/>
       <c r="N56" s="13"/>
     </row>
-    <row r="57" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="13"/>
@@ -4066,11 +3689,11 @@
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
       <c r="K57" s="13"/>
-      <c r="L57" s="47"/>
-      <c r="M57" s="47"/>
+      <c r="L57" s="48"/>
+      <c r="M57" s="48"/>
       <c r="N57" s="13"/>
     </row>
-    <row r="58" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
@@ -4086,7 +3709,7 @@
       <c r="M58" s="13"/>
       <c r="N58" s="13"/>
     </row>
-    <row r="59" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
@@ -4102,7 +3725,7 @@
       <c r="M59" s="13"/>
       <c r="N59" s="13"/>
     </row>
-    <row r="60" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
@@ -4118,7 +3741,7 @@
       <c r="M60" s="13"/>
       <c r="N60" s="13"/>
     </row>
-    <row r="61" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
@@ -4134,7 +3757,7 @@
       <c r="M61" s="13"/>
       <c r="N61" s="13"/>
     </row>
-    <row r="62" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -4150,7 +3773,7 @@
       <c r="M62" s="13"/>
       <c r="N62" s="13"/>
     </row>
-    <row r="63" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
@@ -4166,36 +3789,36 @@
       <c r="M63" s="13"/>
       <c r="N63" s="13"/>
     </row>
-    <row r="64" spans="1:14" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="65" spans="3:13" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="66" spans="3:13" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="J66" s="49"/>
-      <c r="K66" s="49"/>
-      <c r="L66" s="49"/>
-      <c r="M66" s="49"/>
-    </row>
-    <row r="67" spans="3:13" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="J67" s="50"/>
-      <c r="L67" s="50"/>
-      <c r="M67" s="50"/>
-    </row>
-    <row r="68" spans="3:13" s="44" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C68" s="48"/>
-      <c r="F68" s="48"/>
-      <c r="J68" s="51"/>
-      <c r="K68" s="48"/>
-      <c r="L68" s="50"/>
-      <c r="M68" s="50"/>
-    </row>
-    <row r="69" spans="3:13" s="44" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C69" s="48"/>
-      <c r="F69" s="48"/>
-      <c r="J69" s="51"/>
-      <c r="K69" s="48"/>
-      <c r="L69" s="50"/>
-      <c r="M69" s="50"/>
-    </row>
-    <row r="70" spans="3:13" s="24" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="3:13" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="3:13" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J66" s="50"/>
+      <c r="K66" s="50"/>
+      <c r="L66" s="50"/>
+      <c r="M66" s="50"/>
+    </row>
+    <row r="67" spans="3:13" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J67" s="51"/>
+      <c r="L67" s="51"/>
+      <c r="M67" s="51"/>
+    </row>
+    <row r="68" spans="3:13" s="45" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C68" s="49"/>
+      <c r="F68" s="49"/>
+      <c r="J68" s="52"/>
+      <c r="K68" s="49"/>
+      <c r="L68" s="51"/>
+      <c r="M68" s="51"/>
+    </row>
+    <row r="69" spans="3:13" s="45" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C69" s="49"/>
+      <c r="F69" s="49"/>
+      <c r="J69" s="52"/>
+      <c r="K69" s="49"/>
+      <c r="L69" s="51"/>
+      <c r="M69" s="51"/>
+    </row>
+    <row r="70" spans="3:13" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C70" s="30"/>
       <c r="F70" s="30"/>
       <c r="J70" s="32"/>
@@ -4203,7 +3826,7 @@
       <c r="L70" s="31"/>
       <c r="M70" s="31"/>
     </row>
-    <row r="71" spans="3:13" s="24" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:13" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C71" s="30"/>
       <c r="F71" s="30"/>
       <c r="J71" s="32"/>
@@ -4211,31 +3834,31 @@
       <c r="L71" s="31"/>
       <c r="M71" s="31"/>
     </row>
-    <row r="72" spans="3:13" s="33" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:13" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C72" s="34"/>
       <c r="F72" s="34"/>
       <c r="K72" s="34"/>
       <c r="M72" s="34"/>
     </row>
-    <row r="73" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C73" s="35"/>
       <c r="F73" s="35"/>
       <c r="K73" s="35"/>
       <c r="M73" s="35"/>
     </row>
-    <row r="74" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C74" s="35"/>
       <c r="F74" s="35"/>
       <c r="K74" s="35"/>
       <c r="M74" s="35"/>
     </row>
-    <row r="75" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C75" s="35"/>
       <c r="F75" s="35"/>
       <c r="K75" s="35"/>
       <c r="M75" s="35"/>
     </row>
-    <row r="76" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C76" s="35"/>
       <c r="F76" s="35"/>
       <c r="J76" s="37"/>
@@ -4243,7 +3866,7 @@
       <c r="L76" s="37"/>
       <c r="M76" s="37"/>
     </row>
-    <row r="77" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C77" s="35"/>
       <c r="F77" s="35"/>
       <c r="J77" s="38"/>
@@ -4251,7 +3874,7 @@
       <c r="L77" s="39"/>
       <c r="M77" s="39"/>
     </row>
-    <row r="78" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C78" s="35"/>
       <c r="F78" s="35"/>
       <c r="J78" s="38"/>
@@ -4259,7 +3882,7 @@
       <c r="L78" s="39"/>
       <c r="M78" s="39"/>
     </row>
-    <row r="79" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C79" s="35"/>
       <c r="F79" s="35"/>
       <c r="J79" s="38"/>
@@ -4267,7 +3890,7 @@
       <c r="L79" s="39"/>
       <c r="M79" s="39"/>
     </row>
-    <row r="80" spans="3:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C80" s="35"/>
       <c r="F80" s="35"/>
       <c r="J80" s="38"/>
@@ -4275,7 +3898,7 @@
       <c r="L80" s="38"/>
       <c r="M80" s="38"/>
     </row>
-    <row r="81" spans="1:13" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C81" s="35"/>
       <c r="F81" s="35"/>
       <c r="J81" s="38"/>
@@ -4283,31 +3906,31 @@
       <c r="L81" s="38"/>
       <c r="M81" s="38"/>
     </row>
-    <row r="82" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C82" s="18"/>
       <c r="F82" s="18"/>
       <c r="K82" s="18"/>
       <c r="M82" s="18"/>
     </row>
-    <row r="83" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C83" s="18"/>
       <c r="F83" s="18"/>
       <c r="K83" s="18"/>
       <c r="M83" s="18"/>
     </row>
-    <row r="84" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C84" s="18"/>
       <c r="F84" s="18"/>
       <c r="K84" s="18"/>
       <c r="M84" s="18"/>
     </row>
-    <row r="85" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C85" s="18"/>
       <c r="F85" s="18"/>
       <c r="K85" s="18"/>
       <c r="M85" s="18"/>
     </row>
-    <row r="86" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C86" s="18"/>
       <c r="F86" s="18"/>
       <c r="J86" s="15"/>
@@ -4315,7 +3938,7 @@
       <c r="L86" s="15"/>
       <c r="M86" s="15"/>
     </row>
-    <row r="87" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C87" s="18"/>
       <c r="F87" s="18"/>
       <c r="J87" s="17"/>
@@ -4323,7 +3946,7 @@
       <c r="L87" s="16"/>
       <c r="M87" s="16"/>
     </row>
-    <row r="88" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C88" s="18"/>
       <c r="F88" s="18"/>
       <c r="J88" s="17"/>
@@ -4331,7 +3954,7 @@
       <c r="L88" s="16"/>
       <c r="M88" s="16"/>
     </row>
-    <row r="89" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C89" s="18"/>
       <c r="F89" s="18"/>
       <c r="J89" s="17"/>
@@ -4339,7 +3962,7 @@
       <c r="L89" s="16"/>
       <c r="M89" s="16"/>
     </row>
-    <row r="90" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C90" s="18"/>
       <c r="F90" s="18"/>
       <c r="J90" s="17"/>
@@ -4347,7 +3970,7 @@
       <c r="L90" s="17"/>
       <c r="M90" s="17"/>
     </row>
-    <row r="91" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C91" s="18"/>
       <c r="F91" s="18"/>
       <c r="J91" s="17"/>
@@ -4355,7 +3978,7 @@
       <c r="L91" s="17"/>
       <c r="M91" s="17"/>
     </row>
-    <row r="92" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="20"/>
       <c r="C92" s="18"/>
       <c r="D92" s="18"/>
@@ -4367,7 +3990,7 @@
       <c r="K92" s="18"/>
       <c r="M92" s="18"/>
     </row>
-    <row r="93" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C93" s="18"/>
       <c r="D93" s="18"/>
       <c r="E93" s="18"/>
@@ -4378,7 +4001,7 @@
       <c r="K93" s="18"/>
       <c r="M93" s="18"/>
     </row>
-    <row r="94" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C94" s="18"/>
       <c r="D94" s="18"/>
       <c r="E94" s="18"/>
@@ -4389,7 +4012,7 @@
       <c r="K94" s="18"/>
       <c r="M94" s="18"/>
     </row>
-    <row r="95" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C95" s="18"/>
       <c r="D95" s="18"/>
       <c r="E95" s="18"/>
@@ -4400,7 +4023,7 @@
       <c r="K95" s="18"/>
       <c r="M95" s="18"/>
     </row>
-    <row r="96" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C96" s="18"/>
       <c r="D96" s="18"/>
       <c r="E96" s="18"/>
@@ -4411,7 +4034,7 @@
       <c r="K96" s="18"/>
       <c r="M96" s="18"/>
     </row>
-    <row r="97" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C97" s="18"/>
       <c r="D97" s="18"/>
       <c r="E97" s="18"/>
@@ -4422,7 +4045,7 @@
       <c r="K97" s="18"/>
       <c r="M97" s="18"/>
     </row>
-    <row r="98" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C98" s="18"/>
       <c r="D98" s="18"/>
       <c r="E98" s="18"/>
@@ -4433,7 +4056,7 @@
       <c r="K98" s="18"/>
       <c r="M98" s="18"/>
     </row>
-    <row r="99" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C99" s="18"/>
       <c r="D99" s="18"/>
       <c r="E99" s="18"/>
@@ -4445,17 +4068,17 @@
       <c r="M99" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A5:XFD5"/>
-    <mergeCell ref="A13:XFD13"/>
+  <autoFilter ref="A1:N1"/>
+  <mergeCells count="5">
+    <mergeCell ref="A4:XFD4"/>
+    <mergeCell ref="A12:XFD12"/>
     <mergeCell ref="A15:XFD15"/>
     <mergeCell ref="A20:XFD20"/>
-    <mergeCell ref="A26:XFD26"/>
-    <mergeCell ref="A29:XFD29"/>
+    <mergeCell ref="A27:XFD27"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F27" r:id="rId1" location="/79590444732ud/detail/userstory/134825813356" display="https://rally1.rallydev.com/ - /79590444732ud/detail/userstory/134825813356"/>
-    <hyperlink ref="F28" r:id="rId2" location="/79590444732ud/detail/userstory/134825813356" display="https://rally1.rallydev.com/ - /79590444732ud/detail/userstory/134825813356"/>
+    <hyperlink ref="F28" r:id="rId1" location="/79590444732ud/detail/userstory/134825813356" display="https://rally1.rallydev.com/ - /79590444732ud/detail/userstory/134825813356"/>
+    <hyperlink ref="F29" r:id="rId2" location="/79590444732ud/detail/userstory/134825813356" display="https://rally1.rallydev.com/ - /79590444732ud/detail/userstory/134825813356"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
819544 updated RTM 100218 to fix reviewer finding
</commit_message>
<xml_diff>
--- a/Requirement/Build 4/TAS eBilling RTM IB_ 2.0_592.xlsx
+++ b/Requirement/Build 4/TAS eBilling RTM IB_ 2.0_592.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="7692" windowWidth="19236" windowHeight="3900" activeTab="2"/>
+    <workbookView xWindow="-12" yWindow="7692" windowWidth="19236" windowHeight="3900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="85">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -298,8 +298,26 @@
     <t xml:space="preserve">US2487 - Insurance Company Entry/Edit - Dental      </t>
   </si>
   <si>
+    <t>September 2018</t>
+  </si>
+  <si>
+    <t>Updated with results of final build testing for T20.</t>
+  </si>
+  <si>
+    <t>IB*2.0*592_T20</t>
+  </si>
+  <si>
+    <t>TC2534 - CIT eBilling TS27 – Dental Claim Creation – AutoBiller- Auto Populated Fields – Production Only</t>
+  </si>
+  <si>
+    <t>TC1260 -  CIT eBilling TS8 Complete Dental Claim - Prod Only US1108 and US131</t>
+  </si>
+  <si>
+    <t>October 2018</t>
+  </si>
+  <si>
     <r>
-      <t>Version 4.0</t>
+      <t>Version 5.0</t>
     </r>
     <r>
       <rPr>
@@ -313,22 +331,7 @@
     </r>
   </si>
   <si>
-    <t>September 2018</t>
-  </si>
-  <si>
-    <t>Updated with results of final build testing for T20.</t>
-  </si>
-  <si>
-    <t>IB*2.0*592_T20</t>
-  </si>
-  <si>
-    <t>TC2534 - CIT eBilling TS27 – Dental Claim Creation – AutoBiller- Auto Populated Fields – Production Only</t>
-  </si>
-  <si>
-    <t>TC1260 -  CIT eBilling TS8 Complete Dental Claim - Prod Only US1108 and US131</t>
-  </si>
-  <si>
-    <t>TC1626 - CIT eBilling TS29 - Print Bill – View Dental Using GEN</t>
+    <t>Updated to correct name of Dental TC1626, as it had been changed, and so that it may coincide with the TEL</t>
   </si>
 </sst>
 </file>
@@ -1507,7 +1510,7 @@
   <dimension ref="A5:H34"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:H23"/>
+      <selection activeCell="A26" sqref="A26:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1588,7 +1591,7 @@
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="75" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" s="75"/>
       <c r="C23" s="75"/>
@@ -1608,7 +1611,7 @@
     </row>
     <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="76" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B26" s="76"/>
       <c r="C26" s="76"/>
@@ -1652,8 +1655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1734,23 +1737,31 @@
     </row>
     <row r="7" spans="1:4" s="61" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="59">
         <v>4</v>
       </c>
       <c r="C7" s="62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7" s="60" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="61" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="58"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="60"/>
+    <row r="8" spans="1:4" s="61" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="59">
+        <v>5</v>
+      </c>
+      <c r="C8" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="60" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="9" spans="1:4" s="61" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="58"/>
@@ -1825,8 +1836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DQ99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView topLeftCell="E13" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2054,7 +2065,7 @@
         <v>34</v>
       </c>
       <c r="M3" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -2222,7 +2233,7 @@
         <v>34</v>
       </c>
       <c r="M5" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N5" s="13"/>
     </row>
@@ -2264,7 +2275,7 @@
         <v>34</v>
       </c>
       <c r="M6" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N6" s="13"/>
     </row>
@@ -2306,7 +2317,7 @@
         <v>34</v>
       </c>
       <c r="M7" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N7" s="13"/>
     </row>
@@ -2348,7 +2359,7 @@
         <v>34</v>
       </c>
       <c r="M8" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N8" s="13"/>
     </row>
@@ -2390,7 +2401,7 @@
         <v>34</v>
       </c>
       <c r="M9" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N9" s="13"/>
     </row>
@@ -2426,13 +2437,13 @@
         <v>17</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L10" s="13" t="s">
         <v>34</v>
       </c>
       <c r="M10" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N10" s="13"/>
     </row>
@@ -2474,7 +2485,7 @@
         <v>34</v>
       </c>
       <c r="M11" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N11" s="13"/>
     </row>
@@ -2641,7 +2652,7 @@
         <v>34</v>
       </c>
       <c r="M13" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N13" s="13"/>
     </row>
@@ -2677,13 +2688,13 @@
         <v>17</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L14" s="13" t="s">
         <v>34</v>
       </c>
       <c r="M14" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N14" s="13"/>
     </row>
@@ -2743,7 +2754,7 @@
         <v>34</v>
       </c>
       <c r="M16" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N16" s="13"/>
     </row>
@@ -2785,7 +2796,7 @@
         <v>34</v>
       </c>
       <c r="M17" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N17" s="13"/>
     </row>
@@ -2827,7 +2838,7 @@
         <v>34</v>
       </c>
       <c r="M18" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N18" s="13"/>
     </row>
@@ -2869,7 +2880,7 @@
         <v>34</v>
       </c>
       <c r="M19" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N19" s="13"/>
     </row>
@@ -2929,7 +2940,7 @@
         <v>34</v>
       </c>
       <c r="M21" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N21" s="13"/>
     </row>
@@ -2971,7 +2982,7 @@
         <v>34</v>
       </c>
       <c r="M22" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N22" s="13"/>
     </row>
@@ -3013,7 +3024,7 @@
         <v>34</v>
       </c>
       <c r="M23" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N23" s="13"/>
     </row>
@@ -3055,7 +3066,7 @@
         <v>34</v>
       </c>
       <c r="M24" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N24" s="13"/>
     </row>
@@ -3097,7 +3108,7 @@
         <v>34</v>
       </c>
       <c r="M25" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N25" s="13"/>
     </row>
@@ -3133,13 +3144,13 @@
         <v>17</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="L26" s="13" t="s">
         <v>34</v>
       </c>
       <c r="M26" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N26" s="13"/>
     </row>
@@ -3199,7 +3210,7 @@
         <v>34</v>
       </c>
       <c r="M28" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N28" s="13"/>
     </row>
@@ -3241,7 +3252,7 @@
         <v>34</v>
       </c>
       <c r="M29" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N29" s="13"/>
     </row>

</xml_diff>

<commit_message>
819544 Update to add US 3528 addressing reviewer comment.
</commit_message>
<xml_diff>
--- a/Requirement/Build 4/TAS eBilling RTM IB_ 2.0_592.xlsx
+++ b/Requirement/Build 4/TAS eBilling RTM IB_ 2.0_592.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="7692" windowWidth="19236" windowHeight="3900" activeTab="1"/>
+    <workbookView xWindow="-12" yWindow="7692" windowWidth="19236" windowHeight="3900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="100">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -316,8 +316,56 @@
     <t>October 2018</t>
   </si>
   <si>
+    <t>Updated to correct name of Dental TC1626, as it had been changed, and so that it may coincide with the TEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US3528 - Provider ID Maintenance_Dental_Removal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a member of the eBilling Team, I have determined during User Acceptance Testing (UAT) that I no longer want to be able to define either human or facility Secondary Provider IDs to be used on Dental claim.   </t>
+  </si>
+  <si>
+    <t>TS14 – Regression Insurance Co ID Default</t>
+  </si>
+  <si>
+    <t>TS15 – Regression Ins Co ID Parameters</t>
+  </si>
+  <si>
+    <t>TS16 – Regression Billing Provider Secondary IDs</t>
+  </si>
+  <si>
+    <t>TS17 – Regression Additional Billing Provider Secondary IDs</t>
+  </si>
+  <si>
+    <t>TS34 – Regression Ins Co VA Lab/Facilitiy ID</t>
+  </si>
+  <si>
+    <t>TS27 – Regression VA Provider’s Own IDs</t>
+  </si>
+  <si>
+    <t>TS28 – Regression VA Provider’s Insurance IDs</t>
+  </si>
+  <si>
+    <t>TS29 – Regression Care Units</t>
+  </si>
+  <si>
+    <t>TS30 – Regression Non-VA Provider’s Own IDs</t>
+  </si>
+  <si>
+    <t>TS31 – Regression Non-VA Provider’s Ins IDs</t>
+  </si>
+  <si>
+    <t>TS32 – Regression Non-VA Facility’s Own IDs</t>
+  </si>
+  <si>
+    <t>TS33 – Regression Non-VA Facility’s Ins IDs</t>
+  </si>
+  <si>
+    <t>Updated to add US3528 and all associated test cases. Somehow did not copy over from prior version.</t>
+  </si>
+  <si>
     <r>
-      <t>Version 5.0</t>
+      <t>Version 6.0</t>
     </r>
     <r>
       <rPr>
@@ -329,9 +377,6 @@
       </rPr>
       <t xml:space="preserve">               </t>
     </r>
-  </si>
-  <si>
-    <t>Updated to correct name of Dental TC1626, as it had been changed, and so that it may coincide with the TEL</t>
   </si>
 </sst>
 </file>
@@ -1510,7 +1555,7 @@
   <dimension ref="A5:H34"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:H26"/>
+      <selection activeCell="A23" sqref="A23:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1591,7 +1636,7 @@
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="75" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B23" s="75"/>
       <c r="C23" s="75"/>
@@ -1611,7 +1656,7 @@
     </row>
     <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="76" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B26" s="76"/>
       <c r="C26" s="76"/>
@@ -1655,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1757,17 +1802,25 @@
         <v>5</v>
       </c>
       <c r="C8" s="62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="60" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="61" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="60"/>
+    <row r="9" spans="1:4" s="61" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="59">
+        <v>6</v>
+      </c>
+      <c r="C9" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="10" spans="1:4" s="61" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="58"/>
@@ -1836,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DQ99"/>
   <sheetViews>
-    <sheetView topLeftCell="E13" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3256,212 +3309,526 @@
       </c>
       <c r="N29" s="13"/>
     </row>
-    <row r="30" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="56"/>
-      <c r="N30" s="13"/>
-    </row>
-    <row r="31" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="56"/>
+    <row r="30" spans="1:14" s="78" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="79"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="79"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="79"/>
+      <c r="N30" s="79"/>
+    </row>
+    <row r="31" spans="1:14" s="55" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="69" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J31" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M31" s="56" t="s">
+        <v>79</v>
+      </c>
       <c r="N31" s="13"/>
     </row>
-    <row r="32" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="41"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="56"/>
+    <row r="32" spans="1:14" s="55" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J32" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="L32" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M32" s="56" t="s">
+        <v>79</v>
+      </c>
       <c r="N32" s="13"/>
     </row>
-    <row r="33" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="56"/>
+    <row r="33" spans="1:14" s="55" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J33" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="L33" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M33" s="56" t="s">
+        <v>79</v>
+      </c>
       <c r="N33" s="13"/>
     </row>
-    <row r="34" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="56"/>
+    <row r="34" spans="1:14" s="55" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G34" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J34" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K34" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="L34" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M34" s="56" t="s">
+        <v>79</v>
+      </c>
       <c r="N34" s="13"/>
     </row>
-    <row r="35" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="41"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="56"/>
+    <row r="35" spans="1:14" s="55" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G35" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J35" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="L35" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M35" s="56" t="s">
+        <v>79</v>
+      </c>
       <c r="N35" s="13"/>
     </row>
-    <row r="36" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="56"/>
+    <row r="36" spans="1:14" s="55" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G36" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J36" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="L36" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M36" s="56" t="s">
+        <v>79</v>
+      </c>
       <c r="N36" s="13"/>
     </row>
-    <row r="37" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="56"/>
+    <row r="37" spans="1:14" s="55" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G37" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J37" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="L37" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M37" s="56" t="s">
+        <v>79</v>
+      </c>
       <c r="N37" s="13"/>
     </row>
-    <row r="38" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="56"/>
+    <row r="38" spans="1:14" s="55" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G38" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J38" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="L38" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M38" s="56" t="s">
+        <v>79</v>
+      </c>
       <c r="N38" s="13"/>
     </row>
-    <row r="39" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="41"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="13"/>
-      <c r="M39" s="56"/>
+    <row r="39" spans="1:14" s="55" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G39" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J39" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="L39" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M39" s="56" t="s">
+        <v>79</v>
+      </c>
       <c r="N39" s="13"/>
     </row>
-    <row r="40" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="41"/>
-      <c r="H40" s="41"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="41"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="56"/>
+    <row r="40" spans="1:14" s="55" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J40" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K40" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="L40" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M40" s="56" t="s">
+        <v>79</v>
+      </c>
       <c r="N40" s="13"/>
     </row>
-    <row r="41" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="41"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="41"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="56"/>
+    <row r="41" spans="1:14" s="55" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G41" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J41" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K41" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="L41" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M41" s="56" t="s">
+        <v>79</v>
+      </c>
       <c r="N41" s="13"/>
     </row>
-    <row r="42" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="12"/>
-      <c r="M42" s="12"/>
+    <row r="42" spans="1:14" s="55" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G42" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J42" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="L42" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M42" s="56" t="s">
+        <v>79</v>
+      </c>
       <c r="N42" s="13"/>
     </row>
     <row r="43" spans="1:14" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -4080,7 +4447,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:N1"/>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A30:XFD30"/>
     <mergeCell ref="A4:XFD4"/>
     <mergeCell ref="A12:XFD12"/>
     <mergeCell ref="A15:XFD15"/>

</xml_diff>